<commit_message>
Modify table definition for UC
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13C3287-3613-4B9E-90B9-549039A8DF05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33150ED-5732-452C-B9C3-599FB5C1A9CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>~UC_Sets: T_E:</t>
   </si>
   <si>
-    <t>UC_T</t>
-  </si>
-  <si>
     <t>UC_N</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>UC_CAP*CAP_BEV1(t1)+UC_CAP*CAP_BEV2(t1)&gt;=UC_CAP*CAP_BEV1(t1+1)+UC_CAP*CAP_BEV2(t1+1)-0.24</t>
+  </si>
+  <si>
+    <t>~UC_T</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="B2:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,7 +579,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -589,67 +589,67 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" s="2">
         <v>1.1000000000000001</v>
@@ -664,7 +664,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -699,23 +699,23 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s">
         <v>22</v>
-      </c>
-      <c r="K10" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L12">
         <v>130</v>
@@ -723,13 +723,13 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="J15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" t="s">
         <v>27</v>
-      </c>
-      <c r="K15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L15" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -738,15 +738,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -957,6 +948,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -964,14 +964,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -990,6 +982,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Add growth rate constraint for advanced vehicles (BEV, HEV, PHEV, FCV)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33150ED-5732-452C-B9C3-599FB5C1A9CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948B6F11-491F-44E5-A36B-FEAA11855BC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -87,50 +87,123 @@
     <t>DMD</t>
   </si>
   <si>
-    <t>TRAELC</t>
-  </si>
-  <si>
-    <t>T-CAR-BEV*</t>
-  </si>
-  <si>
-    <t>Maximum growth rate of BEVs private cars</t>
-  </si>
-  <si>
-    <t>UC_BEVMaxGrowthPC</t>
-  </si>
-  <si>
-    <t>1.3*cap(t)</t>
-  </si>
-  <si>
-    <t>cap(t+1)+0</t>
-  </si>
-  <si>
-    <t>90*1.3</t>
-  </si>
-  <si>
     <t>LO</t>
   </si>
   <si>
-    <t>&gt;=</t>
-  </si>
-  <si>
-    <t>0*1.3</t>
-  </si>
-  <si>
-    <t>130-130</t>
-  </si>
-  <si>
-    <t>UC_CAP*CAP_BEV1(t1)+UC_CAP*CAP_BEV2(t1)&gt;=UC_CAP*CAP_BEV1(t1+1)+UC_CAP*CAP_BEV2(t1+1)-0.24</t>
-  </si>
-  <si>
     <t>~UC_T</t>
+  </si>
+  <si>
+    <t>Large PSVs</t>
+  </si>
+  <si>
+    <t>Small PSVs</t>
+  </si>
+  <si>
+    <t>Motor cycles</t>
+  </si>
+  <si>
+    <t>Private cars</t>
+  </si>
+  <si>
+    <t>Over 12.5 tonnes</t>
+  </si>
+  <si>
+    <t>10 - 12.5 tonnes</t>
+  </si>
+  <si>
+    <t>7.5 - 10 tonnes</t>
+  </si>
+  <si>
+    <t>5 - 7.5 tonnes</t>
+  </si>
+  <si>
+    <t>2 - 5 tonnes</t>
+  </si>
+  <si>
+    <t>0 - 2 tonnes</t>
+  </si>
+  <si>
+    <t>Freight</t>
+  </si>
+  <si>
+    <t>CSO, Table THA17</t>
+  </si>
+  <si>
+    <t>New registered vehicles and total number of vehicles in 2019</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Proportion</t>
+  </si>
+  <si>
+    <t>Growth rate</t>
+  </si>
+  <si>
+    <t>New sales</t>
+  </si>
+  <si>
+    <t>HGV</t>
+  </si>
+  <si>
+    <t>MGV</t>
+  </si>
+  <si>
+    <t>LGV</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>T-CAR-BEV*,T-CAR-PHEV*,T-CAR-FCVs*</t>
+  </si>
+  <si>
+    <t>T-LGT-BEV*,T-LGT-PHEV*,T-LGT-FCVs*</t>
+  </si>
+  <si>
+    <t>T-MGT-BEV*,T-MGT-HEV*,T-MGT-FCVs*</t>
+  </si>
+  <si>
+    <t>T-HGT-BEV*,T-HGT-HEV*,T-HGT-FCVs*</t>
+  </si>
+  <si>
+    <t>UC_MaxGrowthPC</t>
+  </si>
+  <si>
+    <t>UC_MaxGrowthLGT</t>
+  </si>
+  <si>
+    <t>UC_MaxGrowthMGT</t>
+  </si>
+  <si>
+    <t>UC_MaxGrowthHGT</t>
+  </si>
+  <si>
+    <t>Maximum growth rate of advanced private cars</t>
+  </si>
+  <si>
+    <t>Maximum growth rate of advanced Light Goods Truck</t>
+  </si>
+  <si>
+    <t>Maximum growth rate of advanced Medium Goods Truck</t>
+  </si>
+  <si>
+    <t>Maximum growth rate of advanced Heavy Goods Truck</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +228,27 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -184,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -192,20 +286,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{B99A9728-4181-4E10-9A7D-F6FA2D41C1C2}"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -517,26 +647,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
-  <dimension ref="B2:N15"/>
+  <dimension ref="A2:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="34" customWidth="1"/>
     <col min="10" max="10" width="11.44140625" customWidth="1"/>
     <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +684,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -570,7 +701,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -579,7 +710,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -587,7 +718,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -628,9 +759,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -638,106 +769,611 @@
       <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="J6" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
-      <c r="L6" s="2">
-        <v>-0.9</v>
+      <c r="L6" s="20">
+        <f>-0.001*(D23/5)</f>
+        <v>-24.2242</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="20">
+        <f>-0.001*((D17+D18)/10)</f>
+        <v>-1.6539000000000001</v>
+      </c>
+      <c r="M7" s="2">
+        <v>5</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="J10" t="s">
+      <c r="G8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="20">
+        <f>-0.001*((D19+D20)/10)</f>
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="M8" s="2">
+        <v>5</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="21">
+        <v>2018</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="21">
+        <v>1.3</v>
+      </c>
+      <c r="K9" s="21">
+        <v>1</v>
+      </c>
+      <c r="L9" s="22">
+        <f>-0.001*((D21+D22)/10)</f>
+        <v>-0.15180000000000002</v>
+      </c>
+      <c r="M9" s="21">
+        <v>5</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="12">
+        <v>228046</v>
+      </c>
+      <c r="D17" s="12">
+        <v>9959</v>
+      </c>
+      <c r="E17" s="15">
+        <f t="shared" ref="E17:E22" si="0">D17/C17</f>
+        <v>4.3671013742841359E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="12">
+        <v>100649</v>
+      </c>
+      <c r="D18" s="12">
+        <v>6580</v>
+      </c>
+      <c r="E18" s="15">
+        <f t="shared" si="0"/>
+        <v>6.5375711631511485E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="12">
+        <v>4546</v>
+      </c>
+      <c r="D19" s="12">
+        <v>201</v>
+      </c>
+      <c r="E19" s="15">
+        <f t="shared" si="0"/>
+        <v>4.4214694236691596E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="12">
+        <v>6661</v>
+      </c>
+      <c r="D20" s="12">
+        <v>329</v>
+      </c>
+      <c r="E20" s="15">
+        <f t="shared" si="0"/>
+        <v>4.9391983185707852E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="12">
+        <v>8424</v>
+      </c>
+      <c r="D21" s="12">
+        <v>485</v>
+      </c>
+      <c r="E21" s="15">
+        <f t="shared" si="0"/>
+        <v>5.7573599240265907E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="12">
+        <v>14373</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1033</v>
+      </c>
+      <c r="E22" s="15">
+        <f t="shared" si="0"/>
+        <v>7.187086899046824E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="12">
+        <v>2168099</v>
+      </c>
+      <c r="D23" s="12">
+        <v>121121</v>
+      </c>
+      <c r="E23" s="15">
+        <f>D23/C23</f>
+        <v>5.5865068892149296E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K10" t="s">
-        <v>25</v>
-      </c>
-      <c r="L10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="J12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="J15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K15" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" t="s">
-        <v>27</v>
+      <c r="C24" s="12">
+        <v>41471</v>
+      </c>
+      <c r="D24" s="12">
+        <v>2566</v>
+      </c>
+      <c r="E24" s="15">
+        <f t="shared" ref="E24:E26" si="1">D24/C24</f>
+        <v>6.1874562947601935E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="12">
+        <v>21457</v>
+      </c>
+      <c r="D25" s="12">
+        <v>1224</v>
+      </c>
+      <c r="E25" s="15">
+        <f t="shared" si="1"/>
+        <v>5.7044321200540614E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="13">
+        <v>11206</v>
+      </c>
+      <c r="D26" s="13">
+        <v>551</v>
+      </c>
+      <c r="E26" s="16">
+        <f t="shared" si="1"/>
+        <v>4.9170087453150095E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B34" s="17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c r="H36">
+        <v>6</v>
+      </c>
+      <c r="I36">
+        <v>7</v>
+      </c>
+      <c r="J36">
+        <v>8</v>
+      </c>
+      <c r="K36">
+        <v>9</v>
+      </c>
+      <c r="L36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="19">
+        <f>D22+D21</f>
+        <v>1518</v>
+      </c>
+      <c r="C37" s="18">
+        <f>B37/10</f>
+        <v>151.80000000000001</v>
+      </c>
+      <c r="D37" s="18">
+        <f>C37*(1+$B$34)</f>
+        <v>197.34000000000003</v>
+      </c>
+      <c r="E37" s="18">
+        <f>D37*(1+$B$34)</f>
+        <v>256.54200000000003</v>
+      </c>
+      <c r="F37" s="18">
+        <f>E37*(1+$B$34)</f>
+        <v>333.50460000000004</v>
+      </c>
+      <c r="G37" s="18">
+        <f>F37*(1+$B$34)</f>
+        <v>433.55598000000009</v>
+      </c>
+      <c r="H37" s="18">
+        <f>G37*(1+$B$34)</f>
+        <v>563.62277400000016</v>
+      </c>
+      <c r="I37" s="18">
+        <f>H37*(1+$B$34)</f>
+        <v>732.70960620000028</v>
+      </c>
+      <c r="J37" s="18">
+        <f>I37*(1+$B$34)</f>
+        <v>952.52248806000034</v>
+      </c>
+      <c r="K37" s="18">
+        <f>J37*(1+$B$34)</f>
+        <v>1238.2792344780005</v>
+      </c>
+      <c r="L37" s="18">
+        <f>K37*(1+$B$34)</f>
+        <v>1609.7630048214007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="19">
+        <f>D20+D19</f>
+        <v>530</v>
+      </c>
+      <c r="C38" s="18">
+        <f>B38/10</f>
+        <v>53</v>
+      </c>
+      <c r="D38" s="18">
+        <f>C38*(1+$B$34)</f>
+        <v>68.900000000000006</v>
+      </c>
+      <c r="E38" s="18">
+        <f>D38*(1+$B$34)</f>
+        <v>89.570000000000007</v>
+      </c>
+      <c r="F38" s="18">
+        <f>E38*(1+$B$34)</f>
+        <v>116.44100000000002</v>
+      </c>
+      <c r="G38" s="18">
+        <f>F38*(1+$B$34)</f>
+        <v>151.37330000000003</v>
+      </c>
+      <c r="H38" s="18">
+        <f>G38*(1+$B$34)</f>
+        <v>196.78529000000003</v>
+      </c>
+      <c r="I38" s="18">
+        <f>H38*(1+$B$34)</f>
+        <v>255.82087700000005</v>
+      </c>
+      <c r="J38" s="18">
+        <f>I38*(1+$B$34)</f>
+        <v>332.56714010000007</v>
+      </c>
+      <c r="K38" s="18">
+        <f>J38*(1+$B$34)</f>
+        <v>432.33728213000012</v>
+      </c>
+      <c r="L38" s="18">
+        <f>K38*(1+$B$34)</f>
+        <v>562.03846676900014</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="19">
+        <f>D18+D17</f>
+        <v>16539</v>
+      </c>
+      <c r="C39" s="18">
+        <f>B39/10</f>
+        <v>1653.9</v>
+      </c>
+      <c r="D39" s="18">
+        <f>C39*(1+$B$34)</f>
+        <v>2150.0700000000002</v>
+      </c>
+      <c r="E39" s="18">
+        <f>D39*(1+$B$34)</f>
+        <v>2795.0910000000003</v>
+      </c>
+      <c r="F39" s="18">
+        <f>E39*(1+$B$34)</f>
+        <v>3633.6183000000005</v>
+      </c>
+      <c r="G39" s="18">
+        <f>F39*(1+$B$34)</f>
+        <v>4723.7037900000005</v>
+      </c>
+      <c r="H39" s="18">
+        <f>G39*(1+$B$34)</f>
+        <v>6140.8149270000013</v>
+      </c>
+      <c r="I39" s="18">
+        <f>H39*(1+$B$34)</f>
+        <v>7983.0594051000016</v>
+      </c>
+      <c r="J39" s="18">
+        <f>I39*(1+$B$34)</f>
+        <v>10377.977226630002</v>
+      </c>
+      <c r="K39" s="18">
+        <f>J39*(1+$B$34)</f>
+        <v>13491.370394619003</v>
+      </c>
+      <c r="L39" s="18">
+        <f>K39*(1+$B$34)</f>
+        <v>17538.781513004706</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="19">
+        <f>D23</f>
+        <v>121121</v>
+      </c>
+      <c r="C40" s="18">
+        <f>B40/5</f>
+        <v>24224.2</v>
+      </c>
+      <c r="D40" s="18">
+        <f>C40*(1+$B$34)</f>
+        <v>31491.460000000003</v>
+      </c>
+      <c r="E40" s="18">
+        <f>D40*(1+$B$34)</f>
+        <v>40938.898000000008</v>
+      </c>
+      <c r="F40" s="18">
+        <f>E40*(1+$B$34)</f>
+        <v>53220.567400000014</v>
+      </c>
+      <c r="G40" s="18">
+        <f>F40*(1+$B$34)</f>
+        <v>69186.737620000014</v>
+      </c>
+      <c r="H40" s="18">
+        <f>G40*(1+$B$34)</f>
+        <v>89942.758906000017</v>
+      </c>
+      <c r="I40" s="18">
+        <f>H40*(1+$B$34)</f>
+        <v>116925.58657780003</v>
+      </c>
+      <c r="J40" s="18">
+        <f>I40*(1+$B$34)</f>
+        <v>152003.26255114004</v>
+      </c>
+      <c r="K40" s="18">
+        <f>J40*(1+$B$34)</f>
+        <v>197604.24131648205</v>
+      </c>
+      <c r="L40" s="18">
+        <f>K40*(1+$B$34)</f>
+        <v>256885.51371142667</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A17:A22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -948,22 +1584,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -980,21 +1618,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modify UC for maximum light-duty trucks
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948B6F11-491F-44E5-A36B-FEAA11855BC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB8FE75-D9BC-4496-811E-EAA3B9EAF6A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -162,9 +162,6 @@
     <t>T-CAR-BEV*,T-CAR-PHEV*,T-CAR-FCVs*</t>
   </si>
   <si>
-    <t>T-LGT-BEV*,T-LGT-PHEV*,T-LGT-FCVs*</t>
-  </si>
-  <si>
     <t>T-MGT-BEV*,T-MGT-HEV*,T-MGT-FCVs*</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>Maximum growth rate of advanced Heavy Goods Truck</t>
+  </si>
+  <si>
+    <t>T-LGT-BEV*</t>
   </si>
 </sst>
 </file>
@@ -201,7 +201,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -310,15 +310,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -326,10 +323,13 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -650,7 +650,7 @@
   <dimension ref="A2:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,7 +761,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -786,7 +786,7 @@
       <c r="K6" s="2">
         <v>1</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="19">
         <f>-0.001*(D23/5)</f>
         <v>-24.2242</v>
       </c>
@@ -794,12 +794,12 @@
         <v>5</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
@@ -810,7 +810,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="H7" s="2">
         <v>2018</v>
@@ -824,7 +824,7 @@
       <c r="K7" s="2">
         <v>1</v>
       </c>
-      <c r="L7" s="20">
+      <c r="L7" s="19">
         <f>-0.001*((D17+D18)/10)</f>
         <v>-1.6539000000000001</v>
       </c>
@@ -832,12 +832,12 @@
         <v>5</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>15</v>
@@ -848,7 +848,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8" s="2">
         <v>2018</v>
@@ -862,7 +862,7 @@
       <c r="K8" s="2">
         <v>1</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="19">
         <f>-0.001*((D19+D20)/10)</f>
         <v>-5.2999999999999999E-2</v>
       </c>
@@ -870,45 +870,45 @@
         <v>5</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="21">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="20">
         <v>2018</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="20">
         <v>1.3</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="20">
         <v>1</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="21">
         <f>-0.001*((D21+D22)/10)</f>
         <v>-0.15180000000000002</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="20">
         <v>5</v>
       </c>
-      <c r="N9" s="21" t="s">
-        <v>52</v>
+      <c r="N9" s="20" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -927,117 +927,117 @@
       <c r="N10" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="14" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>228046</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <v>9959</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="14">
         <f t="shared" ref="E17:E22" si="0">D17/C17</f>
         <v>4.3671013742841359E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <v>100649</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <v>6580</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="14">
         <f t="shared" si="0"/>
         <v>6.5375711631511485E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>4546</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="11">
         <v>201</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="14">
         <f t="shared" si="0"/>
         <v>4.4214694236691596E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="11">
         <v>6661</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="11">
         <v>329</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="14">
         <f t="shared" si="0"/>
         <v>4.9391983185707852E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="11">
         <v>8424</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="11">
         <v>485</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="14">
         <f t="shared" si="0"/>
         <v>5.7573599240265907E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <v>14373</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="11">
         <v>1033</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="14">
         <f t="shared" si="0"/>
         <v>7.187086899046824E-2</v>
       </c>
@@ -1046,13 +1046,13 @@
       <c r="B23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <v>2168099</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="11">
         <v>121121</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="14">
         <f>D23/C23</f>
         <v>5.5865068892149296E-2</v>
       </c>
@@ -1061,13 +1061,13 @@
       <c r="B24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="11">
         <v>41471</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="11">
         <v>2566</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="14">
         <f t="shared" ref="E24:E26" si="1">D24/C24</f>
         <v>6.1874562947601935E-2</v>
       </c>
@@ -1076,29 +1076,29 @@
       <c r="B25" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="11">
         <v>21457</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="11">
         <v>1224</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="14">
         <f t="shared" si="1"/>
         <v>5.7044321200540614E-2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="12">
         <v>11206</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="12">
         <v>551</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="15">
         <f t="shared" si="1"/>
         <v>4.9170087453150095E-2</v>
       </c>
@@ -1114,7 +1114,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B34" s="17">
+      <c r="B34" s="16">
         <v>0.3</v>
       </c>
     </row>
@@ -1157,48 +1157,48 @@
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="19">
+      <c r="B37" s="18">
         <f>D22+D21</f>
         <v>1518</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="17">
         <f>B37/10</f>
         <v>151.80000000000001</v>
       </c>
-      <c r="D37" s="18">
-        <f>C37*(1+$B$34)</f>
+      <c r="D37" s="17">
+        <f t="shared" ref="D37:L37" si="2">C37*(1+$B$34)</f>
         <v>197.34000000000003</v>
       </c>
-      <c r="E37" s="18">
-        <f>D37*(1+$B$34)</f>
+      <c r="E37" s="17">
+        <f t="shared" si="2"/>
         <v>256.54200000000003</v>
       </c>
-      <c r="F37" s="18">
-        <f>E37*(1+$B$34)</f>
+      <c r="F37" s="17">
+        <f t="shared" si="2"/>
         <v>333.50460000000004</v>
       </c>
-      <c r="G37" s="18">
-        <f>F37*(1+$B$34)</f>
+      <c r="G37" s="17">
+        <f t="shared" si="2"/>
         <v>433.55598000000009</v>
       </c>
-      <c r="H37" s="18">
-        <f>G37*(1+$B$34)</f>
+      <c r="H37" s="17">
+        <f t="shared" si="2"/>
         <v>563.62277400000016</v>
       </c>
-      <c r="I37" s="18">
-        <f>H37*(1+$B$34)</f>
+      <c r="I37" s="17">
+        <f t="shared" si="2"/>
         <v>732.70960620000028</v>
       </c>
-      <c r="J37" s="18">
-        <f>I37*(1+$B$34)</f>
+      <c r="J37" s="17">
+        <f t="shared" si="2"/>
         <v>952.52248806000034</v>
       </c>
-      <c r="K37" s="18">
-        <f>J37*(1+$B$34)</f>
+      <c r="K37" s="17">
+        <f t="shared" si="2"/>
         <v>1238.2792344780005</v>
       </c>
-      <c r="L37" s="18">
-        <f>K37*(1+$B$34)</f>
+      <c r="L37" s="17">
+        <f t="shared" si="2"/>
         <v>1609.7630048214007</v>
       </c>
     </row>
@@ -1206,48 +1206,48 @@
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="19">
+      <c r="B38" s="18">
         <f>D20+D19</f>
         <v>530</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="17">
         <f>B38/10</f>
         <v>53</v>
       </c>
-      <c r="D38" s="18">
-        <f>C38*(1+$B$34)</f>
+      <c r="D38" s="17">
+        <f t="shared" ref="D38:L38" si="3">C38*(1+$B$34)</f>
         <v>68.900000000000006</v>
       </c>
-      <c r="E38" s="18">
-        <f>D38*(1+$B$34)</f>
+      <c r="E38" s="17">
+        <f t="shared" si="3"/>
         <v>89.570000000000007</v>
       </c>
-      <c r="F38" s="18">
-        <f>E38*(1+$B$34)</f>
+      <c r="F38" s="17">
+        <f t="shared" si="3"/>
         <v>116.44100000000002</v>
       </c>
-      <c r="G38" s="18">
-        <f>F38*(1+$B$34)</f>
+      <c r="G38" s="17">
+        <f t="shared" si="3"/>
         <v>151.37330000000003</v>
       </c>
-      <c r="H38" s="18">
-        <f>G38*(1+$B$34)</f>
+      <c r="H38" s="17">
+        <f t="shared" si="3"/>
         <v>196.78529000000003</v>
       </c>
-      <c r="I38" s="18">
-        <f>H38*(1+$B$34)</f>
+      <c r="I38" s="17">
+        <f t="shared" si="3"/>
         <v>255.82087700000005</v>
       </c>
-      <c r="J38" s="18">
-        <f>I38*(1+$B$34)</f>
+      <c r="J38" s="17">
+        <f t="shared" si="3"/>
         <v>332.56714010000007</v>
       </c>
-      <c r="K38" s="18">
-        <f>J38*(1+$B$34)</f>
+      <c r="K38" s="17">
+        <f t="shared" si="3"/>
         <v>432.33728213000012</v>
       </c>
-      <c r="L38" s="18">
-        <f>K38*(1+$B$34)</f>
+      <c r="L38" s="17">
+        <f t="shared" si="3"/>
         <v>562.03846676900014</v>
       </c>
     </row>
@@ -1255,48 +1255,48 @@
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="19">
+      <c r="B39" s="18">
         <f>D18+D17</f>
         <v>16539</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="17">
         <f>B39/10</f>
         <v>1653.9</v>
       </c>
-      <c r="D39" s="18">
-        <f>C39*(1+$B$34)</f>
+      <c r="D39" s="17">
+        <f t="shared" ref="D39:L39" si="4">C39*(1+$B$34)</f>
         <v>2150.0700000000002</v>
       </c>
-      <c r="E39" s="18">
-        <f>D39*(1+$B$34)</f>
+      <c r="E39" s="17">
+        <f t="shared" si="4"/>
         <v>2795.0910000000003</v>
       </c>
-      <c r="F39" s="18">
-        <f>E39*(1+$B$34)</f>
+      <c r="F39" s="17">
+        <f t="shared" si="4"/>
         <v>3633.6183000000005</v>
       </c>
-      <c r="G39" s="18">
-        <f>F39*(1+$B$34)</f>
+      <c r="G39" s="17">
+        <f t="shared" si="4"/>
         <v>4723.7037900000005</v>
       </c>
-      <c r="H39" s="18">
-        <f>G39*(1+$B$34)</f>
+      <c r="H39" s="17">
+        <f t="shared" si="4"/>
         <v>6140.8149270000013</v>
       </c>
-      <c r="I39" s="18">
-        <f>H39*(1+$B$34)</f>
+      <c r="I39" s="17">
+        <f t="shared" si="4"/>
         <v>7983.0594051000016</v>
       </c>
-      <c r="J39" s="18">
-        <f>I39*(1+$B$34)</f>
+      <c r="J39" s="17">
+        <f t="shared" si="4"/>
         <v>10377.977226630002</v>
       </c>
-      <c r="K39" s="18">
-        <f>J39*(1+$B$34)</f>
+      <c r="K39" s="17">
+        <f t="shared" si="4"/>
         <v>13491.370394619003</v>
       </c>
-      <c r="L39" s="18">
-        <f>K39*(1+$B$34)</f>
+      <c r="L39" s="17">
+        <f t="shared" si="4"/>
         <v>17538.781513004706</v>
       </c>
     </row>
@@ -1304,48 +1304,48 @@
       <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="19">
+      <c r="B40" s="18">
         <f>D23</f>
         <v>121121</v>
       </c>
-      <c r="C40" s="18">
+      <c r="C40" s="17">
         <f>B40/5</f>
         <v>24224.2</v>
       </c>
-      <c r="D40" s="18">
-        <f>C40*(1+$B$34)</f>
+      <c r="D40" s="17">
+        <f t="shared" ref="D40:L40" si="5">C40*(1+$B$34)</f>
         <v>31491.460000000003</v>
       </c>
-      <c r="E40" s="18">
-        <f>D40*(1+$B$34)</f>
+      <c r="E40" s="17">
+        <f t="shared" si="5"/>
         <v>40938.898000000008</v>
       </c>
-      <c r="F40" s="18">
-        <f>E40*(1+$B$34)</f>
+      <c r="F40" s="17">
+        <f t="shared" si="5"/>
         <v>53220.567400000014</v>
       </c>
-      <c r="G40" s="18">
-        <f>F40*(1+$B$34)</f>
+      <c r="G40" s="17">
+        <f t="shared" si="5"/>
         <v>69186.737620000014</v>
       </c>
-      <c r="H40" s="18">
-        <f>G40*(1+$B$34)</f>
+      <c r="H40" s="17">
+        <f t="shared" si="5"/>
         <v>89942.758906000017</v>
       </c>
-      <c r="I40" s="18">
-        <f>H40*(1+$B$34)</f>
+      <c r="I40" s="17">
+        <f t="shared" si="5"/>
         <v>116925.58657780003</v>
       </c>
-      <c r="J40" s="18">
-        <f>I40*(1+$B$34)</f>
+      <c r="J40" s="17">
+        <f t="shared" si="5"/>
         <v>152003.26255114004</v>
       </c>
-      <c r="K40" s="18">
-        <f>J40*(1+$B$34)</f>
+      <c r="K40" s="17">
+        <f t="shared" si="5"/>
         <v>197604.24131648205</v>
       </c>
-      <c r="L40" s="18">
-        <f>K40*(1+$B$34)</f>
+      <c r="L40" s="17">
+        <f t="shared" si="5"/>
         <v>256885.51371142667</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test UC for maximum growth rate
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB8FE75-D9BC-4496-811E-EAA3B9EAF6A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6C1E5E-F804-43F0-B836-088924C6301C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -159,15 +159,6 @@
     <t>PC</t>
   </si>
   <si>
-    <t>T-CAR-BEV*,T-CAR-PHEV*,T-CAR-FCVs*</t>
-  </si>
-  <si>
-    <t>T-MGT-BEV*,T-MGT-HEV*,T-MGT-FCVs*</t>
-  </si>
-  <si>
-    <t>T-HGT-BEV*,T-HGT-HEV*,T-HGT-FCVs*</t>
-  </si>
-  <si>
     <t>UC_MaxGrowthPC</t>
   </si>
   <si>
@@ -193,6 +184,15 @@
   </si>
   <si>
     <t>T-LGT-BEV*</t>
+  </si>
+  <si>
+    <t>T-MGT-BEV*</t>
+  </si>
+  <si>
+    <t>T-HGT-BEV*</t>
+  </si>
+  <si>
+    <t>T-CAR-BEV*</t>
   </si>
 </sst>
 </file>
@@ -650,7 +650,7 @@
   <dimension ref="A2:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,7 +761,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -772,7 +772,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
@@ -794,12 +794,12 @@
         <v>5</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
@@ -810,7 +810,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H7" s="2">
         <v>2018</v>
@@ -832,12 +832,12 @@
         <v>5</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>15</v>
@@ -848,7 +848,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="H8" s="2">
         <v>2018</v>
@@ -870,12 +870,12 @@
         <v>5</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>15</v>
@@ -886,7 +886,7 @@
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H9" s="20">
         <v>2018</v>
@@ -908,7 +908,7 @@
         <v>5</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1359,21 +1359,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -1584,24 +1569,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1618,4 +1601,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change seed value for LGT
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6C1E5E-F804-43F0-B836-088924C6301C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AEE86C-9BF5-4874-AF96-9F3B0ED5C127}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -650,7 +650,7 @@
   <dimension ref="A2:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,8 +825,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="19">
-        <f>-0.001*((D17+D18)/10)</f>
-        <v>-1.6539000000000001</v>
+        <v>-3</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
@@ -1359,6 +1358,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -1569,22 +1583,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1601,21 +1617,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add UC growth rate in 2050
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AEE86C-9BF5-4874-AF96-9F3B0ED5C127}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B695532-5D25-47C0-B833-E3869FD7DB96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -72,9 +72,6 @@
     <t>UC_CAP~RHS</t>
   </si>
   <si>
-    <t>UC_RHSRTS</t>
-  </si>
-  <si>
     <t>UC_RHSRTS~0</t>
   </si>
   <si>
@@ -193,6 +190,12 @@
   </si>
   <si>
     <t>T-CAR-BEV*</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS~2018</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS~2050</t>
   </si>
 </sst>
 </file>
@@ -203,7 +206,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +253,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -647,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
-  <dimension ref="A2:N40"/>
+  <dimension ref="A2:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,12 +671,13 @@
     <col min="7" max="7" width="34" customWidth="1"/>
     <col min="10" max="10" width="11.44140625" customWidth="1"/>
     <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="48.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,8 +693,9 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -700,8 +711,9 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -710,15 +722,16 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -750,35 +763,38 @@
         <v>11</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="2">
         <v>1.3</v>
@@ -790,33 +806,37 @@
         <f>-0.001*(D23/5)</f>
         <v>-24.2242</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="19">
+        <f>L6*200</f>
+        <v>-4844.84</v>
+      </c>
+      <c r="N6" s="2">
         <v>5</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H7" s="2">
         <v>2018</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J7" s="2">
         <v>1.3</v>
@@ -827,33 +847,37 @@
       <c r="L7" s="19">
         <v>-3</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="19">
+        <f t="shared" ref="M7:M9" si="0">L7*200</f>
+        <v>-600</v>
+      </c>
+      <c r="N7" s="2">
         <v>5</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8" s="2">
         <v>2018</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J8" s="2">
         <v>1.3</v>
@@ -865,33 +889,37 @@
         <f>-0.001*((D19+D20)/10)</f>
         <v>-5.2999999999999999E-2</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="19">
+        <f>L8*300</f>
+        <v>-15.9</v>
+      </c>
+      <c r="N8" s="2">
         <v>5</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O8" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>15</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>16</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" s="20">
         <v>2018</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J9" s="20">
         <v>1.3</v>
@@ -903,14 +931,18 @@
         <f>-0.001*((D21+D22)/10)</f>
         <v>-0.15180000000000002</v>
       </c>
-      <c r="M9" s="20">
+      <c r="M9" s="21">
+        <f>L9*300</f>
+        <v>-45.540000000000006</v>
+      </c>
+      <c r="N9" s="20">
         <v>5</v>
       </c>
-      <c r="N9" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -924,31 +956,32 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>33</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="11">
         <v>228046</v>
@@ -957,14 +990,14 @@
         <v>9959</v>
       </c>
       <c r="E17" s="14">
-        <f t="shared" ref="E17:E22" si="0">D17/C17</f>
+        <f t="shared" ref="E17:E22" si="1">D17/C17</f>
         <v>4.3671013742841359E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="11">
         <v>100649</v>
@@ -973,14 +1006,14 @@
         <v>6580</v>
       </c>
       <c r="E18" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.5375711631511485E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
       <c r="B19" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="11">
         <v>4546</v>
@@ -989,14 +1022,14 @@
         <v>201</v>
       </c>
       <c r="E19" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4214694236691596E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="11">
         <v>6661</v>
@@ -1005,14 +1038,14 @@
         <v>329</v>
       </c>
       <c r="E20" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.9391983185707852E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="11">
         <v>8424</v>
@@ -1021,14 +1054,14 @@
         <v>485</v>
       </c>
       <c r="E21" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.7573599240265907E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="11">
         <v>14373</v>
@@ -1037,13 +1070,13 @@
         <v>1033</v>
       </c>
       <c r="E22" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.187086899046824E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="11">
         <v>2168099</v>
@@ -1058,7 +1091,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="11">
         <v>41471</v>
@@ -1067,13 +1100,13 @@
         <v>2566</v>
       </c>
       <c r="E24" s="14">
-        <f t="shared" ref="E24:E26" si="1">D24/C24</f>
+        <f t="shared" ref="E24:E26" si="2">D24/C24</f>
         <v>6.1874562947601935E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="11">
         <v>21457</v>
@@ -1082,14 +1115,14 @@
         <v>1224</v>
       </c>
       <c r="E25" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.7044321200540614E-2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="12">
         <v>11206</v>
@@ -1098,28 +1131,28 @@
         <v>551</v>
       </c>
       <c r="E26" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.9170087453150095E-2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B34" s="16">
         <v>0.3</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1152,9 +1185,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="18">
         <f>D22+D21</f>
@@ -1165,45 +1198,46 @@
         <v>151.80000000000001</v>
       </c>
       <c r="D37" s="17">
-        <f t="shared" ref="D37:L37" si="2">C37*(1+$B$34)</f>
+        <f t="shared" ref="D37:L37" si="3">C37*(1+$B$34)</f>
         <v>197.34000000000003</v>
       </c>
       <c r="E37" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>256.54200000000003</v>
       </c>
       <c r="F37" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>333.50460000000004</v>
       </c>
       <c r="G37" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>433.55598000000009</v>
       </c>
       <c r="H37" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>563.62277400000016</v>
       </c>
       <c r="I37" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>732.70960620000028</v>
       </c>
       <c r="J37" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>952.52248806000034</v>
       </c>
       <c r="K37" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1238.2792344780005</v>
       </c>
       <c r="L37" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1609.7630048214007</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37" s="17"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="18">
         <f>D20+D19</f>
@@ -1214,45 +1248,46 @@
         <v>53</v>
       </c>
       <c r="D38" s="17">
-        <f t="shared" ref="D38:L38" si="3">C38*(1+$B$34)</f>
+        <f t="shared" ref="D38:L38" si="4">C38*(1+$B$34)</f>
         <v>68.900000000000006</v>
       </c>
       <c r="E38" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89.570000000000007</v>
       </c>
       <c r="F38" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>116.44100000000002</v>
       </c>
       <c r="G38" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>151.37330000000003</v>
       </c>
       <c r="H38" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>196.78529000000003</v>
       </c>
       <c r="I38" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>255.82087700000005</v>
       </c>
       <c r="J38" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>332.56714010000007</v>
       </c>
       <c r="K38" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>432.33728213000012</v>
       </c>
       <c r="L38" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>562.03846676900014</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M38" s="17"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="18">
         <f>D18+D17</f>
@@ -1263,45 +1298,46 @@
         <v>1653.9</v>
       </c>
       <c r="D39" s="17">
-        <f t="shared" ref="D39:L39" si="4">C39*(1+$B$34)</f>
+        <f t="shared" ref="D39:L39" si="5">C39*(1+$B$34)</f>
         <v>2150.0700000000002</v>
       </c>
       <c r="E39" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2795.0910000000003</v>
       </c>
       <c r="F39" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3633.6183000000005</v>
       </c>
       <c r="G39" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4723.7037900000005</v>
       </c>
       <c r="H39" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6140.8149270000013</v>
       </c>
       <c r="I39" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7983.0594051000016</v>
       </c>
       <c r="J39" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10377.977226630002</v>
       </c>
       <c r="K39" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13491.370394619003</v>
       </c>
       <c r="L39" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17538.781513004706</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39" s="17"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="18">
         <f>D23</f>
@@ -1312,67 +1348,54 @@
         <v>24224.2</v>
       </c>
       <c r="D40" s="17">
-        <f t="shared" ref="D40:L40" si="5">C40*(1+$B$34)</f>
+        <f t="shared" ref="D40:L40" si="6">C40*(1+$B$34)</f>
         <v>31491.460000000003</v>
       </c>
       <c r="E40" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40938.898000000008</v>
       </c>
       <c r="F40" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>53220.567400000014</v>
       </c>
       <c r="G40" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>69186.737620000014</v>
       </c>
       <c r="H40" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>89942.758906000017</v>
       </c>
       <c r="I40" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>116925.58657780003</v>
       </c>
       <c r="J40" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>152003.26255114004</v>
       </c>
       <c r="K40" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>197604.24131648205</v>
       </c>
       <c r="L40" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>256885.51371142667</v>
       </c>
+      <c r="M40" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A17:A22"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -1583,24 +1606,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1617,4 +1638,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Deactivate UC capacity growth rate for 2050
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B695532-5D25-47C0-B833-E3869FD7DB96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451B63D4-64FF-4B12-8B28-7A07B452F05A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -195,7 +195,7 @@
     <t>UC_RHSRTS~2018</t>
   </si>
   <si>
-    <t>UC_RHSRTS~2050</t>
+    <t>*UC_RHSRTS~2050</t>
   </si>
 </sst>
 </file>
@@ -659,7 +659,7 @@
   <dimension ref="A2:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:M9"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,7 +848,7 @@
         <v>-3</v>
       </c>
       <c r="M7" s="19">
-        <f t="shared" ref="M7:M9" si="0">L7*200</f>
+        <f t="shared" ref="M7" si="0">L7*200</f>
         <v>-600</v>
       </c>
       <c r="N7" s="2">
@@ -1396,6 +1396,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -1606,22 +1621,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1638,21 +1655,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add UC growth rate for PHEVs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451B63D4-64FF-4B12-8B28-7A07B452F05A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A45986-2EC5-4B9C-B3EB-E9A8E85360EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -156,9 +156,6 @@
     <t>PC</t>
   </si>
   <si>
-    <t>UC_MaxGrowthPC</t>
-  </si>
-  <si>
     <t>UC_MaxGrowthLGT</t>
   </si>
   <si>
@@ -195,7 +192,13 @@
     <t>UC_RHSRTS~2018</t>
   </si>
   <si>
-    <t>*UC_RHSRTS~2050</t>
+    <t>UC_MaxGrowthBEVPC</t>
+  </si>
+  <si>
+    <t>UC_MaxGrowthPlugPC</t>
+  </si>
+  <si>
+    <t>T-CAR-PHEV*</t>
   </si>
 </sst>
 </file>
@@ -656,25 +659,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
-  <dimension ref="A2:O40"/>
+  <dimension ref="A2:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="34" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" customWidth="1"/>
     <col min="10" max="10" width="11.44140625" customWidth="1"/>
     <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="48.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -763,21 +766,18 @@
         <v>11</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -788,7 +788,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
@@ -803,23 +803,19 @@
         <v>1</v>
       </c>
       <c r="L6" s="19">
-        <f>-0.001*(D23/5)</f>
+        <f>-0.001*(D24/5)</f>
         <v>-24.2242</v>
       </c>
-      <c r="M6" s="19">
-        <f>L6*200</f>
-        <v>-4844.84</v>
-      </c>
-      <c r="N6" s="2">
+      <c r="M6" s="2">
         <v>5</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>44</v>
+      <c r="N6" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
@@ -830,10 +826,10 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H7" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>16</v>
@@ -845,22 +841,19 @@
         <v>1</v>
       </c>
       <c r="L7" s="19">
-        <v>-3</v>
-      </c>
-      <c r="M7" s="19">
-        <f t="shared" ref="M7" si="0">L7*200</f>
-        <v>-600</v>
-      </c>
-      <c r="N7" s="2">
+        <f>L6</f>
+        <v>-24.2242</v>
+      </c>
+      <c r="M7" s="2">
         <v>5</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>45</v>
+      <c r="N7" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
@@ -871,7 +864,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H8" s="2">
         <v>2018</v>
@@ -886,508 +879,535 @@
         <v>1</v>
       </c>
       <c r="L8" s="19">
-        <f>-0.001*((D19+D20)/10)</f>
-        <v>-5.2999999999999999E-2</v>
-      </c>
-      <c r="M8" s="19">
-        <f>L8*300</f>
-        <v>-15.9</v>
-      </c>
-      <c r="N8" s="2">
+        <v>-4</v>
+      </c>
+      <c r="M8" s="2">
         <v>5</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="N8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="19">
+        <v>-0.1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>5</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="20">
+        <v>1.3</v>
+      </c>
+      <c r="K10" s="20">
+        <v>1</v>
+      </c>
+      <c r="L10" s="21">
+        <v>-0.2</v>
+      </c>
+      <c r="M10" s="20">
+        <v>5</v>
+      </c>
+      <c r="N10" s="20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="20">
-        <v>2018</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="20">
-        <v>1.3</v>
-      </c>
-      <c r="K9" s="20">
-        <v>1</v>
-      </c>
-      <c r="L9" s="21">
-        <f>-0.001*((D21+D22)/10)</f>
-        <v>-0.15180000000000002</v>
-      </c>
-      <c r="M9" s="21">
-        <f>L9*300</f>
-        <v>-45.540000000000006</v>
-      </c>
-      <c r="N9" s="20">
-        <v>5</v>
-      </c>
-      <c r="O9" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="13" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E17" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C18" s="11">
         <v>228046</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D18" s="11">
         <v>9959</v>
       </c>
-      <c r="E17" s="14">
-        <f t="shared" ref="E17:E22" si="1">D17/C17</f>
+      <c r="E18" s="14">
+        <f t="shared" ref="E18:E23" si="0">D18/C18</f>
         <v>4.3671013742841359E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="11">
-        <v>100649</v>
-      </c>
-      <c r="D18" s="11">
-        <v>6580</v>
-      </c>
-      <c r="E18" s="14">
-        <f t="shared" si="1"/>
-        <v>6.5375711631511485E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
       <c r="B19" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" s="11">
-        <v>4546</v>
+        <v>100649</v>
       </c>
       <c r="D19" s="11">
-        <v>201</v>
+        <v>6580</v>
       </c>
       <c r="E19" s="14">
-        <f t="shared" si="1"/>
-        <v>4.4214694236691596E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.5375711631511485E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" s="11">
-        <v>6661</v>
+        <v>4546</v>
       </c>
       <c r="D20" s="11">
-        <v>329</v>
+        <v>201</v>
       </c>
       <c r="E20" s="14">
-        <f t="shared" si="1"/>
-        <v>4.9391983185707852E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.4214694236691596E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21" s="11">
-        <v>8424</v>
+        <v>6661</v>
       </c>
       <c r="D21" s="11">
-        <v>485</v>
+        <v>329</v>
       </c>
       <c r="E21" s="14">
-        <f t="shared" si="1"/>
-        <v>5.7573599240265907E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.9391983185707852E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="11">
+        <v>8424</v>
+      </c>
+      <c r="D22" s="11">
+        <v>485</v>
+      </c>
+      <c r="E22" s="14">
+        <f t="shared" si="0"/>
+        <v>5.7573599240265907E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="B23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C23" s="11">
         <v>14373</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D23" s="11">
         <v>1033</v>
       </c>
-      <c r="E22" s="14">
-        <f t="shared" si="1"/>
+      <c r="E23" s="14">
+        <f t="shared" si="0"/>
         <v>7.187086899046824E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="11">
-        <v>2168099</v>
-      </c>
-      <c r="D23" s="11">
-        <v>121121</v>
-      </c>
-      <c r="E23" s="14">
-        <f>D23/C23</f>
-        <v>5.5865068892149296E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" s="11">
-        <v>41471</v>
+        <v>2168099</v>
       </c>
       <c r="D24" s="11">
-        <v>2566</v>
+        <v>121121</v>
       </c>
       <c r="E24" s="14">
-        <f t="shared" ref="E24:E26" si="2">D24/C24</f>
-        <v>6.1874562947601935E-2</v>
+        <f>D24/C24</f>
+        <v>5.5865068892149296E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="11">
+        <v>41471</v>
+      </c>
+      <c r="D25" s="11">
+        <v>2566</v>
+      </c>
+      <c r="E25" s="14">
+        <f t="shared" ref="E25:E27" si="1">D25/C25</f>
+        <v>6.1874562947601935E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C26" s="11">
         <v>21457</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D26" s="11">
         <v>1224</v>
       </c>
-      <c r="E25" s="14">
-        <f t="shared" si="2"/>
+      <c r="E26" s="14">
+        <f t="shared" si="1"/>
         <v>5.7044321200540614E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C27" s="12">
         <v>11206</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D27" s="12">
         <v>551</v>
       </c>
-      <c r="E26" s="15">
-        <f t="shared" si="2"/>
+      <c r="E27" s="15">
+        <f t="shared" si="1"/>
         <v>4.9170087453150095E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B34" s="16">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B35" s="16">
         <v>0.3</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>1</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <v>2</v>
       </c>
-      <c r="E36">
+      <c r="E37">
         <v>3</v>
       </c>
-      <c r="F36">
+      <c r="F37">
         <v>4</v>
       </c>
-      <c r="G36">
+      <c r="G37">
         <v>5</v>
       </c>
-      <c r="H36">
+      <c r="H37">
         <v>6</v>
       </c>
-      <c r="I36">
+      <c r="I37">
         <v>7</v>
       </c>
-      <c r="J36">
+      <c r="J37">
         <v>8</v>
       </c>
-      <c r="K36">
+      <c r="K37">
         <v>9</v>
       </c>
-      <c r="L36">
+      <c r="L37">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="18">
-        <f>D22+D21</f>
-        <v>1518</v>
-      </c>
-      <c r="C37" s="17">
-        <f>B37/10</f>
-        <v>151.80000000000001</v>
-      </c>
-      <c r="D37" s="17">
-        <f t="shared" ref="D37:L37" si="3">C37*(1+$B$34)</f>
-        <v>197.34000000000003</v>
-      </c>
-      <c r="E37" s="17">
-        <f t="shared" si="3"/>
-        <v>256.54200000000003</v>
-      </c>
-      <c r="F37" s="17">
-        <f t="shared" si="3"/>
-        <v>333.50460000000004</v>
-      </c>
-      <c r="G37" s="17">
-        <f t="shared" si="3"/>
-        <v>433.55598000000009</v>
-      </c>
-      <c r="H37" s="17">
-        <f t="shared" si="3"/>
-        <v>563.62277400000016</v>
-      </c>
-      <c r="I37" s="17">
-        <f t="shared" si="3"/>
-        <v>732.70960620000028</v>
-      </c>
-      <c r="J37" s="17">
-        <f t="shared" si="3"/>
-        <v>952.52248806000034</v>
-      </c>
-      <c r="K37" s="17">
-        <f t="shared" si="3"/>
-        <v>1238.2792344780005</v>
-      </c>
-      <c r="L37" s="17">
-        <f t="shared" si="3"/>
-        <v>1609.7630048214007</v>
-      </c>
-      <c r="M37" s="17"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="18">
-        <f>D20+D19</f>
-        <v>530</v>
+        <f>D23+D22</f>
+        <v>1518</v>
       </c>
       <c r="C38" s="17">
         <f>B38/10</f>
-        <v>53</v>
+        <v>151.80000000000001</v>
       </c>
       <c r="D38" s="17">
-        <f t="shared" ref="D38:L38" si="4">C38*(1+$B$34)</f>
-        <v>68.900000000000006</v>
+        <f t="shared" ref="D38:L38" si="2">C38*(1+$B$35)</f>
+        <v>197.34000000000003</v>
       </c>
       <c r="E38" s="17">
-        <f t="shared" si="4"/>
-        <v>89.570000000000007</v>
+        <f t="shared" si="2"/>
+        <v>256.54200000000003</v>
       </c>
       <c r="F38" s="17">
-        <f t="shared" si="4"/>
-        <v>116.44100000000002</v>
+        <f t="shared" si="2"/>
+        <v>333.50460000000004</v>
       </c>
       <c r="G38" s="17">
-        <f t="shared" si="4"/>
-        <v>151.37330000000003</v>
+        <f t="shared" si="2"/>
+        <v>433.55598000000009</v>
       </c>
       <c r="H38" s="17">
-        <f t="shared" si="4"/>
-        <v>196.78529000000003</v>
+        <f t="shared" si="2"/>
+        <v>563.62277400000016</v>
       </c>
       <c r="I38" s="17">
-        <f t="shared" si="4"/>
-        <v>255.82087700000005</v>
+        <f t="shared" si="2"/>
+        <v>732.70960620000028</v>
       </c>
       <c r="J38" s="17">
-        <f t="shared" si="4"/>
-        <v>332.56714010000007</v>
+        <f t="shared" si="2"/>
+        <v>952.52248806000034</v>
       </c>
       <c r="K38" s="17">
-        <f t="shared" si="4"/>
-        <v>432.33728213000012</v>
+        <f t="shared" si="2"/>
+        <v>1238.2792344780005</v>
       </c>
       <c r="L38" s="17">
-        <f t="shared" si="4"/>
-        <v>562.03846676900014</v>
+        <f t="shared" si="2"/>
+        <v>1609.7630048214007</v>
       </c>
       <c r="M38" s="17"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="18">
-        <f>D18+D17</f>
-        <v>16539</v>
+        <f>D21+D20</f>
+        <v>530</v>
       </c>
       <c r="C39" s="17">
         <f>B39/10</f>
-        <v>1653.9</v>
+        <v>53</v>
       </c>
       <c r="D39" s="17">
-        <f t="shared" ref="D39:L39" si="5">C39*(1+$B$34)</f>
-        <v>2150.0700000000002</v>
+        <f t="shared" ref="D39:L39" si="3">C39*(1+$B$35)</f>
+        <v>68.900000000000006</v>
       </c>
       <c r="E39" s="17">
-        <f t="shared" si="5"/>
-        <v>2795.0910000000003</v>
+        <f t="shared" si="3"/>
+        <v>89.570000000000007</v>
       </c>
       <c r="F39" s="17">
-        <f t="shared" si="5"/>
-        <v>3633.6183000000005</v>
+        <f t="shared" si="3"/>
+        <v>116.44100000000002</v>
       </c>
       <c r="G39" s="17">
-        <f t="shared" si="5"/>
-        <v>4723.7037900000005</v>
+        <f t="shared" si="3"/>
+        <v>151.37330000000003</v>
       </c>
       <c r="H39" s="17">
-        <f t="shared" si="5"/>
-        <v>6140.8149270000013</v>
+        <f t="shared" si="3"/>
+        <v>196.78529000000003</v>
       </c>
       <c r="I39" s="17">
-        <f t="shared" si="5"/>
-        <v>7983.0594051000016</v>
+        <f t="shared" si="3"/>
+        <v>255.82087700000005</v>
       </c>
       <c r="J39" s="17">
-        <f t="shared" si="5"/>
-        <v>10377.977226630002</v>
+        <f t="shared" si="3"/>
+        <v>332.56714010000007</v>
       </c>
       <c r="K39" s="17">
-        <f t="shared" si="5"/>
-        <v>13491.370394619003</v>
+        <f t="shared" si="3"/>
+        <v>432.33728213000012</v>
       </c>
       <c r="L39" s="17">
-        <f t="shared" si="5"/>
-        <v>17538.781513004706</v>
+        <f t="shared" si="3"/>
+        <v>562.03846676900014</v>
       </c>
       <c r="M39" s="17"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="18">
+        <f>D19+D18</f>
+        <v>16539</v>
+      </c>
+      <c r="C40" s="17">
+        <f>B40/10</f>
+        <v>1653.9</v>
+      </c>
+      <c r="D40" s="17">
+        <f t="shared" ref="D40:L40" si="4">C40*(1+$B$35)</f>
+        <v>2150.0700000000002</v>
+      </c>
+      <c r="E40" s="17">
+        <f t="shared" si="4"/>
+        <v>2795.0910000000003</v>
+      </c>
+      <c r="F40" s="17">
+        <f t="shared" si="4"/>
+        <v>3633.6183000000005</v>
+      </c>
+      <c r="G40" s="17">
+        <f t="shared" si="4"/>
+        <v>4723.7037900000005</v>
+      </c>
+      <c r="H40" s="17">
+        <f t="shared" si="4"/>
+        <v>6140.8149270000013</v>
+      </c>
+      <c r="I40" s="17">
+        <f t="shared" si="4"/>
+        <v>7983.0594051000016</v>
+      </c>
+      <c r="J40" s="17">
+        <f t="shared" si="4"/>
+        <v>10377.977226630002</v>
+      </c>
+      <c r="K40" s="17">
+        <f t="shared" si="4"/>
+        <v>13491.370394619003</v>
+      </c>
+      <c r="L40" s="17">
+        <f t="shared" si="4"/>
+        <v>17538.781513004706</v>
+      </c>
+      <c r="M40" s="17"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="18">
-        <f>D23</f>
+      <c r="B41" s="18">
+        <f>D24</f>
         <v>121121</v>
       </c>
-      <c r="C40" s="17">
-        <f>B40/5</f>
+      <c r="C41" s="17">
+        <f>B41/5</f>
         <v>24224.2</v>
       </c>
-      <c r="D40" s="17">
-        <f t="shared" ref="D40:L40" si="6">C40*(1+$B$34)</f>
+      <c r="D41" s="17">
+        <f t="shared" ref="D41:L41" si="5">C41*(1+$B$35)</f>
         <v>31491.460000000003</v>
       </c>
-      <c r="E40" s="17">
-        <f t="shared" si="6"/>
+      <c r="E41" s="17">
+        <f t="shared" si="5"/>
         <v>40938.898000000008</v>
       </c>
-      <c r="F40" s="17">
-        <f t="shared" si="6"/>
+      <c r="F41" s="17">
+        <f t="shared" si="5"/>
         <v>53220.567400000014</v>
       </c>
-      <c r="G40" s="17">
-        <f t="shared" si="6"/>
+      <c r="G41" s="17">
+        <f t="shared" si="5"/>
         <v>69186.737620000014</v>
       </c>
-      <c r="H40" s="17">
-        <f t="shared" si="6"/>
+      <c r="H41" s="17">
+        <f t="shared" si="5"/>
         <v>89942.758906000017</v>
       </c>
-      <c r="I40" s="17">
-        <f t="shared" si="6"/>
+      <c r="I41" s="17">
+        <f t="shared" si="5"/>
         <v>116925.58657780003</v>
       </c>
-      <c r="J40" s="17">
-        <f t="shared" si="6"/>
+      <c r="J41" s="17">
+        <f t="shared" si="5"/>
         <v>152003.26255114004</v>
       </c>
-      <c r="K40" s="17">
-        <f t="shared" si="6"/>
+      <c r="K41" s="17">
+        <f t="shared" si="5"/>
         <v>197604.24131648205</v>
       </c>
-      <c r="L40" s="17">
-        <f t="shared" si="6"/>
+      <c r="L41" s="17">
+        <f t="shared" si="5"/>
         <v>256885.51371142667</v>
       </c>
-      <c r="M40" s="17"/>
+      <c r="M41" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A18:A23"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1396,21 +1416,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -1621,24 +1626,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1655,4 +1658,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modify Growth rate UC for diffusion of all vehicles
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A45986-2EC5-4B9C-B3EB-E9A8E85360EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874ABA08-2FA7-4CA9-BE51-22FD2CAFA3AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -156,27 +156,6 @@
     <t>PC</t>
   </si>
   <si>
-    <t>UC_MaxGrowthLGT</t>
-  </si>
-  <si>
-    <t>UC_MaxGrowthMGT</t>
-  </si>
-  <si>
-    <t>UC_MaxGrowthHGT</t>
-  </si>
-  <si>
-    <t>Maximum growth rate of advanced private cars</t>
-  </si>
-  <si>
-    <t>Maximum growth rate of advanced Light Goods Truck</t>
-  </si>
-  <si>
-    <t>Maximum growth rate of advanced Medium Goods Truck</t>
-  </si>
-  <si>
-    <t>Maximum growth rate of advanced Heavy Goods Truck</t>
-  </si>
-  <si>
     <t>T-LGT-BEV*</t>
   </si>
   <si>
@@ -192,24 +171,67 @@
     <t>UC_RHSRTS~2018</t>
   </si>
   <si>
-    <t>UC_MaxGrowthBEVPC</t>
-  </si>
-  <si>
-    <t>UC_MaxGrowthPlugPC</t>
-  </si>
-  <si>
     <t>T-CAR-PHEV*</t>
+  </si>
+  <si>
+    <t>HGT-Maximum growth rate of HEVs</t>
+  </si>
+  <si>
+    <t>HGT-Maximum growth rate of BEVs</t>
+  </si>
+  <si>
+    <t>UC-HGT_MaxGrowthBEV</t>
+  </si>
+  <si>
+    <t>UC-HGT_MaxGrowthHEV</t>
+  </si>
+  <si>
+    <t>T-HGT-HEV*</t>
+  </si>
+  <si>
+    <t>T-MGT-HEV*</t>
+  </si>
+  <si>
+    <t>UC-MGT-MaxGrowthBEV</t>
+  </si>
+  <si>
+    <t>UC-MGT-MaxGrowthHEV</t>
+  </si>
+  <si>
+    <t>MGT-Maximum growth rate of BEVs</t>
+  </si>
+  <si>
+    <t>MGT-Maximum growth rate of HEVs</t>
+  </si>
+  <si>
+    <t>UC-LGT_MaxGrowthBEV</t>
+  </si>
+  <si>
+    <t>LGT-Maximum growth rate of BEVs</t>
+  </si>
+  <si>
+    <t>UC-CAR_MaxGrowthBEV</t>
+  </si>
+  <si>
+    <t>UC-CAR_MaxGrowthPHEV</t>
+  </si>
+  <si>
+    <t>Cars-Maximum growth rate of BEVs</t>
+  </si>
+  <si>
+    <t>Cars-Maximum growth rate of PHEVs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +285,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +323,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -308,13 +348,226 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -338,16 +591,234 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="217">
+    <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
+    <cellStyle name="20% - Accent5 2 2" xfId="25" xr:uid="{11984554-9BCD-4991-A26E-8E4E32B379F3}"/>
+    <cellStyle name="20% - Accent5 2 2 2" xfId="80" xr:uid="{4053E826-B16E-4797-8175-121DE6309698}"/>
+    <cellStyle name="20% - Accent5 2 2 2 2" xfId="185" xr:uid="{60554CB6-C7FE-4DDB-8F65-E30B396779E1}"/>
+    <cellStyle name="20% - Accent5 2 2 3" xfId="132" xr:uid="{22EAA7F0-6D51-4237-88E7-CDFDDD6CC6CD}"/>
+    <cellStyle name="20% - Accent5 2 3" xfId="38" xr:uid="{ECE689CC-3A6C-4742-8416-DEA8E8323B79}"/>
+    <cellStyle name="20% - Accent5 2 3 2" xfId="93" xr:uid="{D756B8C4-6C46-4381-9E83-019B0600E541}"/>
+    <cellStyle name="20% - Accent5 2 3 2 2" xfId="198" xr:uid="{A0708BD6-428C-4641-8390-32A8A1F2D30E}"/>
+    <cellStyle name="20% - Accent5 2 3 3" xfId="145" xr:uid="{48AC7D55-0656-4540-9AE7-625393D58F89}"/>
+    <cellStyle name="20% - Accent5 2 4" xfId="51" xr:uid="{0245FBCC-EA98-45BC-B689-A7F068460447}"/>
+    <cellStyle name="20% - Accent5 2 4 2" xfId="106" xr:uid="{7C1FD2CD-79E1-4085-8FF1-B04CCC35C845}"/>
+    <cellStyle name="20% - Accent5 2 4 2 2" xfId="211" xr:uid="{2C928263-E4BB-4D32-BA0D-ED1DA0E4035F}"/>
+    <cellStyle name="20% - Accent5 2 4 3" xfId="158" xr:uid="{BEEEAD0A-8200-4A80-A59A-53F920FED21B}"/>
+    <cellStyle name="20% - Accent5 2 5" xfId="66" xr:uid="{2630F565-7C6A-439B-ACD5-E0ACBA1DF268}"/>
+    <cellStyle name="20% - Accent5 2 5 2" xfId="172" xr:uid="{61898455-0D5C-4576-B1DB-C00AE1322C0A}"/>
+    <cellStyle name="20% - Accent5 2 6" xfId="119" xr:uid="{B5C471D3-1FE7-4D06-9740-089D1F7D9DAB}"/>
+    <cellStyle name="20% - Accent5 3" xfId="14" xr:uid="{F609DE84-F47C-41C2-B577-FA90397BF740}"/>
+    <cellStyle name="20% - Accent5 3 2" xfId="29" xr:uid="{EE7F52B9-AA79-4CE7-B338-D23AFC2B0771}"/>
+    <cellStyle name="20% - Accent5 3 2 2" xfId="84" xr:uid="{C4C082C7-3040-455C-8122-CCFC8302854F}"/>
+    <cellStyle name="20% - Accent5 3 2 2 2" xfId="189" xr:uid="{D90D9644-A52C-40A7-8241-24DFDBA54804}"/>
+    <cellStyle name="20% - Accent5 3 2 3" xfId="136" xr:uid="{0C01763B-DBB7-4A3F-B0AC-0D5D554DB461}"/>
+    <cellStyle name="20% - Accent5 3 3" xfId="42" xr:uid="{D9C5F10A-2A39-45FD-9A43-48FFEEEC2AB6}"/>
+    <cellStyle name="20% - Accent5 3 3 2" xfId="97" xr:uid="{6A71DB6A-4154-472A-AF6B-27FD349E01E1}"/>
+    <cellStyle name="20% - Accent5 3 3 2 2" xfId="202" xr:uid="{590EA8C2-E8A4-4640-8089-8E58A0EADA2D}"/>
+    <cellStyle name="20% - Accent5 3 3 3" xfId="149" xr:uid="{FF192C5B-BF81-4F2B-AC6B-B251612853EC}"/>
+    <cellStyle name="20% - Accent5 3 4" xfId="55" xr:uid="{845206FD-B807-497E-834D-193E26AF789C}"/>
+    <cellStyle name="20% - Accent5 3 4 2" xfId="110" xr:uid="{63C1047A-E0ED-4BE6-9665-353E104AE219}"/>
+    <cellStyle name="20% - Accent5 3 4 2 2" xfId="215" xr:uid="{9DA4DEC7-7FC7-42C7-8DAB-9003EA64DFE3}"/>
+    <cellStyle name="20% - Accent5 3 4 3" xfId="162" xr:uid="{9CBD39AA-E2B1-4220-BF9D-4F7FA00418C5}"/>
+    <cellStyle name="20% - Accent5 3 5" xfId="70" xr:uid="{E7FA3618-5794-4F17-99A4-D54270E978AB}"/>
+    <cellStyle name="20% - Accent5 3 5 2" xfId="176" xr:uid="{EC35508F-3AF1-438A-8D38-E29D96A32F98}"/>
+    <cellStyle name="20% - Accent5 3 6" xfId="123" xr:uid="{33D390C7-D73A-42F9-834D-B69500D81776}"/>
+    <cellStyle name="20% - Accent5 4" xfId="18" xr:uid="{863EAC86-4DD0-44E4-9C89-723D946DD6C1}"/>
+    <cellStyle name="20% - Accent5 4 2" xfId="74" xr:uid="{FBBF1120-A2ED-4D2D-92BD-340E611F10AE}"/>
+    <cellStyle name="20% - Accent5 4 2 2" xfId="180" xr:uid="{3A6E54E0-75A4-4631-B926-8804A8C6DC1B}"/>
+    <cellStyle name="20% - Accent5 4 3" xfId="127" xr:uid="{4A4B5670-3D45-493A-8898-921A20B19A2A}"/>
+    <cellStyle name="20% - Accent5 5" xfId="33" xr:uid="{4087E6CD-999F-4901-851E-1D7378EF5F08}"/>
+    <cellStyle name="20% - Accent5 5 2" xfId="88" xr:uid="{C897A37A-836C-42E2-B20D-12E6A565C76B}"/>
+    <cellStyle name="20% - Accent5 5 2 2" xfId="193" xr:uid="{5EC463DA-7A01-483E-BA5E-FA3CB886AFB8}"/>
+    <cellStyle name="20% - Accent5 5 3" xfId="140" xr:uid="{2BD21D5B-2252-4DB7-9BD2-8C6B544FF004}"/>
+    <cellStyle name="20% - Accent5 6" xfId="46" xr:uid="{D89CA67E-77C0-43BB-B6A2-F2FBE2A7D6BD}"/>
+    <cellStyle name="20% - Accent5 6 2" xfId="101" xr:uid="{DA40EAF3-2B0E-4A78-918E-040CD0359758}"/>
+    <cellStyle name="20% - Accent5 6 2 2" xfId="206" xr:uid="{DC5819E0-D3F0-4003-91C0-24744F7158BE}"/>
+    <cellStyle name="20% - Accent5 6 3" xfId="153" xr:uid="{707D31F7-FC72-4C10-A515-F50A5A63F7CB}"/>
+    <cellStyle name="20% - Accent5 7" xfId="59" xr:uid="{B7DE35D2-5923-47D5-8064-2C04AE3B01BB}"/>
+    <cellStyle name="20% - Accent5 7 2" xfId="167" xr:uid="{874CF592-FD0E-4904-873C-C07FAEC322FE}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="8" xr:uid="{C47861FD-3E97-4744-A865-ACFD9DCC992D}"/>
+    <cellStyle name="Comma 2 2" xfId="23" xr:uid="{6FD8625A-7619-4301-8188-1E0AF0841F5E}"/>
+    <cellStyle name="Comma 2 2 2" xfId="78" xr:uid="{A71FA496-1E4A-4D5C-95F9-C213403D1372}"/>
+    <cellStyle name="Comma 2 2 2 2" xfId="183" xr:uid="{356500B6-3D45-44B3-9B7E-3AAB43000148}"/>
+    <cellStyle name="Comma 2 2 3" xfId="130" xr:uid="{CB4D2CEB-63D1-4770-9880-AD8E6C8E36DB}"/>
+    <cellStyle name="Comma 2 3" xfId="36" xr:uid="{90DE3579-1977-4C6B-847E-E92F15F9E0F1}"/>
+    <cellStyle name="Comma 2 3 2" xfId="91" xr:uid="{3CA1604E-8A06-4062-9104-8340F7183A16}"/>
+    <cellStyle name="Comma 2 3 2 2" xfId="196" xr:uid="{A7F5DA55-53CE-4422-BA06-89ABB3409010}"/>
+    <cellStyle name="Comma 2 3 3" xfId="143" xr:uid="{B8F801FD-5FC7-4F0B-88EC-EA43AE0A79B7}"/>
+    <cellStyle name="Comma 2 4" xfId="49" xr:uid="{59FC5B72-FAAC-4300-9DF1-2048D9CFC09A}"/>
+    <cellStyle name="Comma 2 4 2" xfId="104" xr:uid="{7F9BEF86-F7C9-47F6-B638-E029087F62EC}"/>
+    <cellStyle name="Comma 2 4 2 2" xfId="209" xr:uid="{DC4C781B-3ECA-42B1-94E6-01303C20BCE0}"/>
+    <cellStyle name="Comma 2 4 3" xfId="156" xr:uid="{928DA526-D1B2-4D7C-A0C2-989B566BF2CF}"/>
+    <cellStyle name="Comma 2 5" xfId="64" xr:uid="{18203036-49E3-4111-A041-C15EF8392F11}"/>
+    <cellStyle name="Comma 2 5 2" xfId="170" xr:uid="{69F7F36D-3C18-4C61-8F9E-13F178F3D6A0}"/>
+    <cellStyle name="Comma 2 6" xfId="117" xr:uid="{38D21344-41A3-4171-A298-3C4D16D5781D}"/>
+    <cellStyle name="Comma 3" xfId="12" xr:uid="{B4F90DA6-3CEF-4B5E-8E10-A29DAAC7E6E1}"/>
+    <cellStyle name="Comma 3 2" xfId="27" xr:uid="{22BBC824-B041-4306-BF3D-112FE089A6E4}"/>
+    <cellStyle name="Comma 3 2 2" xfId="82" xr:uid="{3B2B509C-A915-437B-8267-A638DE5102EC}"/>
+    <cellStyle name="Comma 3 2 2 2" xfId="187" xr:uid="{57955E9D-94F0-49A6-9F3F-5B3A06C4A25F}"/>
+    <cellStyle name="Comma 3 2 3" xfId="134" xr:uid="{B597C21C-04D6-4E66-99E2-E7521C0BF552}"/>
+    <cellStyle name="Comma 3 3" xfId="40" xr:uid="{BD92A8CD-1B04-42B0-A5EE-AD5991DE5F2B}"/>
+    <cellStyle name="Comma 3 3 2" xfId="95" xr:uid="{5B05ABBD-7F05-4B95-8433-D04FC429FFF6}"/>
+    <cellStyle name="Comma 3 3 2 2" xfId="200" xr:uid="{1181A999-A111-41F5-A8B6-A0A329A6282A}"/>
+    <cellStyle name="Comma 3 3 3" xfId="147" xr:uid="{431A9580-1EFC-4ADD-975F-AF3215B5DB60}"/>
+    <cellStyle name="Comma 3 4" xfId="53" xr:uid="{74EF9D46-89F5-4B02-BA6A-F228F73BCD51}"/>
+    <cellStyle name="Comma 3 4 2" xfId="108" xr:uid="{6E59CA5A-5039-4947-9E29-BC415D8C6D0E}"/>
+    <cellStyle name="Comma 3 4 2 2" xfId="213" xr:uid="{AC91527F-1468-44EF-99F2-A6476A77388E}"/>
+    <cellStyle name="Comma 3 4 3" xfId="160" xr:uid="{64ADE26D-B709-46AB-B1ED-D98440A98F28}"/>
+    <cellStyle name="Comma 3 5" xfId="68" xr:uid="{A984BC4E-032F-4E6C-8A39-C87842CFF2C7}"/>
+    <cellStyle name="Comma 3 5 2" xfId="174" xr:uid="{7839EEA7-157F-4562-A4BB-29503D37EA90}"/>
+    <cellStyle name="Comma 3 6" xfId="121" xr:uid="{5E507840-1D65-4E87-8D7F-4DEAC0461FD0}"/>
+    <cellStyle name="Comma 4" xfId="16" xr:uid="{CD4C481F-9382-4616-8DC5-80BECD555C1F}"/>
+    <cellStyle name="Comma 4 2" xfId="72" xr:uid="{1E03F2A1-21D4-49FC-B60C-E51F6DD1E52E}"/>
+    <cellStyle name="Comma 4 2 2" xfId="178" xr:uid="{5EE973C0-E52B-4051-8B2B-A870AF88C918}"/>
+    <cellStyle name="Comma 4 3" xfId="125" xr:uid="{BA46819D-2274-4B63-9822-8B2920FDE4A6}"/>
+    <cellStyle name="Comma 5" xfId="31" xr:uid="{8948A309-0A0B-4EDB-897E-DC68ADC888E5}"/>
+    <cellStyle name="Comma 5 2" xfId="86" xr:uid="{5F4FD49D-B720-479C-9506-386B5E33CC68}"/>
+    <cellStyle name="Comma 5 2 2" xfId="191" xr:uid="{9555B528-480C-43E9-848D-C76431DBFCDC}"/>
+    <cellStyle name="Comma 5 3" xfId="138" xr:uid="{F3A3DFF2-0391-488D-B790-383EFEFC2E88}"/>
+    <cellStyle name="Comma 6" xfId="44" xr:uid="{D215E70F-4FC9-4641-915E-57F29291582D}"/>
+    <cellStyle name="Comma 6 2" xfId="99" xr:uid="{A33A6D59-2FDE-4498-B148-2742AAA886D8}"/>
+    <cellStyle name="Comma 6 2 2" xfId="204" xr:uid="{8CB077BA-9B0C-4E28-B8F2-3F8DA5F6644F}"/>
+    <cellStyle name="Comma 6 3" xfId="151" xr:uid="{5FE6D830-212B-46FA-9213-E06AE57FD613}"/>
+    <cellStyle name="Comma 7" xfId="57" xr:uid="{B07F94D8-52D2-4210-96DC-5BE939614702}"/>
+    <cellStyle name="Comma 7 2" xfId="165" xr:uid="{59CC3575-535F-4640-8AA9-6860CE88644D}"/>
+    <cellStyle name="Comma 8" xfId="113" xr:uid="{D3049B2C-D006-4A03-BB47-B9A6F9D46786}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="56" xr:uid="{8FD9948C-E924-46F1-8C3F-BE68079CF0FB}"/>
+    <cellStyle name="Normal 10 2" xfId="164" xr:uid="{6EC5393C-9EE8-492E-83F0-05CD88BCF795}"/>
+    <cellStyle name="Normal 11" xfId="163" xr:uid="{35D2CCE6-F0E5-4CDF-A655-1461C9460DED}"/>
+    <cellStyle name="Normal 12" xfId="112" xr:uid="{9DEC65C4-D779-4C8A-A956-FB5E0551CC15}"/>
+    <cellStyle name="Normal 13" xfId="111" xr:uid="{4A4D0DE1-B7E2-43D6-B757-5CF5E4EA8606}"/>
+    <cellStyle name="Normal 13 2" xfId="216" xr:uid="{8ABA52A1-5844-4A31-A141-027FD6E20731}"/>
+    <cellStyle name="Normal 14" xfId="4" xr:uid="{43B4C573-954F-48A8-9646-FBB812C8F4E8}"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{B99A9728-4181-4E10-9A7D-F6FA2D41C1C2}"/>
+    <cellStyle name="Normal 2 2" xfId="21" xr:uid="{D245E550-6DC4-464E-BC9E-B8BB8FF47FFA}"/>
+    <cellStyle name="Normal 2 2 2" xfId="76" xr:uid="{418AE6B7-4883-40CF-B7E0-E8903843E3C8}"/>
+    <cellStyle name="Normal 2 2 2 2" xfId="181" xr:uid="{74AF0739-B6A2-4D63-AB95-D606EFCD5525}"/>
+    <cellStyle name="Normal 2 2 3" xfId="128" xr:uid="{1B2A998C-1465-4567-89F1-D49FA63A0558}"/>
+    <cellStyle name="Normal 2 3" xfId="34" xr:uid="{9959FB5A-92DC-4F5B-BA05-7578B72EA55C}"/>
+    <cellStyle name="Normal 2 3 2" xfId="89" xr:uid="{BA0BBB05-2276-40CE-9331-2F11DEDD566E}"/>
+    <cellStyle name="Normal 2 3 2 2" xfId="194" xr:uid="{40AF102A-6F84-4EA1-86AE-F21D3027B03C}"/>
+    <cellStyle name="Normal 2 3 3" xfId="141" xr:uid="{4A1230BE-DB43-4A26-AA0B-EC87742D0BB1}"/>
+    <cellStyle name="Normal 2 4" xfId="47" xr:uid="{C9EB474F-38CB-417B-BAFE-12FCAEB6B917}"/>
+    <cellStyle name="Normal 2 4 2" xfId="102" xr:uid="{756F70DA-A844-4C72-A5DB-49C8D28BABC2}"/>
+    <cellStyle name="Normal 2 4 2 2" xfId="207" xr:uid="{4A3C8C3D-66FD-4FCD-9EE1-0143CCFAC5EE}"/>
+    <cellStyle name="Normal 2 4 3" xfId="154" xr:uid="{D3850522-CAE2-4125-8A70-390D1953457C}"/>
+    <cellStyle name="Normal 2 5" xfId="62" xr:uid="{FEC486B2-72F3-4837-AABF-F208873D8282}"/>
+    <cellStyle name="Normal 2 5 2" xfId="168" xr:uid="{C3306601-716F-49BD-BF14-C567D899BBAB}"/>
+    <cellStyle name="Normal 2 6" xfId="115" xr:uid="{9F445F9F-682F-45FB-8EF4-82DA73F7116E}"/>
+    <cellStyle name="Normal 2 7" xfId="6" xr:uid="{572D363D-A58A-4852-94FE-C6E6523A396B}"/>
+    <cellStyle name="Normal 3" xfId="7" xr:uid="{9FCFF3A1-DEBF-4DF2-884D-337A0A280F03}"/>
+    <cellStyle name="Normal 3 2" xfId="22" xr:uid="{64823147-4DBC-4235-BEC9-C4FF6206EA70}"/>
+    <cellStyle name="Normal 3 2 2" xfId="77" xr:uid="{C696E8C7-37AD-4C70-9B4A-C34D33549A5F}"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="182" xr:uid="{B865EA29-4B9B-4C97-8E83-D4457302C6F6}"/>
+    <cellStyle name="Normal 3 2 3" xfId="129" xr:uid="{C9345BF7-CF94-4EAD-817E-79DC6639D891}"/>
+    <cellStyle name="Normal 3 3" xfId="35" xr:uid="{5E39A6F9-3B9D-42FC-942C-82396F68F64A}"/>
+    <cellStyle name="Normal 3 3 2" xfId="90" xr:uid="{B2F6894A-ABDF-43B5-ACB8-C9BB8FFA8254}"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="195" xr:uid="{B89BCBE0-1A73-47C0-9968-394D990CE44B}"/>
+    <cellStyle name="Normal 3 3 3" xfId="142" xr:uid="{0B4BD0D8-5EC2-4491-B0FE-EF1255690E88}"/>
+    <cellStyle name="Normal 3 4" xfId="48" xr:uid="{19BF5F99-8799-4E7C-8FB1-DEEB93186CD6}"/>
+    <cellStyle name="Normal 3 4 2" xfId="103" xr:uid="{FF00D113-D91D-4000-8A87-535BC8AA7275}"/>
+    <cellStyle name="Normal 3 4 2 2" xfId="208" xr:uid="{D8FF36A5-87F7-4102-A01E-341FDFB3DC50}"/>
+    <cellStyle name="Normal 3 4 3" xfId="155" xr:uid="{8973DE8E-A21D-4A67-AE7E-9BCCFEABD1D7}"/>
+    <cellStyle name="Normal 3 5" xfId="63" xr:uid="{6F24F798-C036-4FC7-B10A-6F202581A2CC}"/>
+    <cellStyle name="Normal 3 5 2" xfId="169" xr:uid="{353F0A7F-7ABF-4972-950E-E5EB28AC0136}"/>
+    <cellStyle name="Normal 3 6" xfId="116" xr:uid="{E3D319F9-E9CF-40F2-90B9-FE6BA93125B8}"/>
+    <cellStyle name="Normal 4" xfId="11" xr:uid="{52ED5DC7-210A-445A-915C-A2E1BF4F8C59}"/>
+    <cellStyle name="Normal 4 2" xfId="26" xr:uid="{20B018E7-FDD2-4D64-AF83-7566BF3BC845}"/>
+    <cellStyle name="Normal 4 2 2" xfId="81" xr:uid="{6178EC38-A062-46C3-BBDA-1F030D7D4CD1}"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="186" xr:uid="{8C125171-9CD0-4D07-966B-D69CBEB140C2}"/>
+    <cellStyle name="Normal 4 2 3" xfId="133" xr:uid="{00FC95A5-2941-4A9A-8D15-985B00991972}"/>
+    <cellStyle name="Normal 4 3" xfId="39" xr:uid="{EEA1B992-496D-4D09-B5A5-C93195F8259C}"/>
+    <cellStyle name="Normal 4 3 2" xfId="94" xr:uid="{D9A8C5DA-CF6B-4C37-B9FA-1B4D9EB6CA5E}"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="199" xr:uid="{1C29C5AF-57AE-4CF5-A536-06218088DB3A}"/>
+    <cellStyle name="Normal 4 3 3" xfId="146" xr:uid="{0E7F66CE-3CE3-4E80-A053-2D3830CC49B6}"/>
+    <cellStyle name="Normal 4 4" xfId="52" xr:uid="{81CD0E6C-08B3-474E-9036-C846BA89C4DF}"/>
+    <cellStyle name="Normal 4 4 2" xfId="107" xr:uid="{0E22EDF5-01B4-4706-9EAB-D01AACA1D958}"/>
+    <cellStyle name="Normal 4 4 2 2" xfId="212" xr:uid="{73CD0AFB-63E6-47D8-BDDB-D751FFB60CDB}"/>
+    <cellStyle name="Normal 4 4 3" xfId="159" xr:uid="{600F8E78-9F3F-4DCB-8BBA-E571C692EDF0}"/>
+    <cellStyle name="Normal 4 5" xfId="67" xr:uid="{0E130F97-0EB5-444C-A205-F58418115BD4}"/>
+    <cellStyle name="Normal 4 5 2" xfId="173" xr:uid="{20286E43-B33A-466B-B905-CA3B8D96BB98}"/>
+    <cellStyle name="Normal 4 6" xfId="120" xr:uid="{9425644B-9165-4A5C-8E86-AF1E7D81D0FF}"/>
+    <cellStyle name="Normal 5" xfId="19" xr:uid="{8C177EFE-557B-4BF8-B113-860388016769}"/>
+    <cellStyle name="Normal 5 2" xfId="75" xr:uid="{E339B932-AE50-4479-AC49-EF84DAEB367F}"/>
+    <cellStyle name="Normal 6" xfId="15" xr:uid="{7BD16B33-6930-4198-A6F1-8E4EAC20364B}"/>
+    <cellStyle name="Normal 6 2" xfId="71" xr:uid="{BEEDA6E6-2F0A-4FD9-B680-5652C04B4245}"/>
+    <cellStyle name="Normal 6 2 2" xfId="177" xr:uid="{A41F7CA7-EB0E-4346-85BA-26B66233784E}"/>
+    <cellStyle name="Normal 6 3" xfId="124" xr:uid="{1A2C9E8F-E339-487E-ADB7-653CAF2283B3}"/>
+    <cellStyle name="Normal 7" xfId="30" xr:uid="{A0527DB1-859B-47D9-8AF4-7E6FBB24C293}"/>
+    <cellStyle name="Normal 7 2" xfId="85" xr:uid="{4309EB4E-D133-4BB8-8C9F-F55DF1E295AF}"/>
+    <cellStyle name="Normal 7 2 2" xfId="190" xr:uid="{4070A2FD-CB1D-46D6-AFEE-D53E679E461E}"/>
+    <cellStyle name="Normal 7 3" xfId="137" xr:uid="{676DAAF5-AC0B-4A24-A15C-AA0472388AC5}"/>
+    <cellStyle name="Normal 8" xfId="43" xr:uid="{88AA4B56-5212-4625-8A57-DAA15B88DCB4}"/>
+    <cellStyle name="Normal 8 2" xfId="98" xr:uid="{EA3E8B42-E850-4A76-9DE5-EDEB909C927A}"/>
+    <cellStyle name="Normal 8 2 2" xfId="203" xr:uid="{B3554D9C-7423-46A1-AC75-E8AC3DB91AF5}"/>
+    <cellStyle name="Normal 8 3" xfId="150" xr:uid="{B6AF7096-7495-40F8-8DFB-CBA837E78CF6}"/>
+    <cellStyle name="Normal 9" xfId="60" xr:uid="{E867A79A-5FDB-4F45-A8F9-B6AC5B9D7569}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent 10" xfId="114" xr:uid="{7868A223-7A62-4040-8A1F-697609DDA337}"/>
+    <cellStyle name="Percent 11" xfId="5" xr:uid="{EE941A09-82F0-45C0-B10F-76FC07DAEEFD}"/>
+    <cellStyle name="Percent 2" xfId="9" xr:uid="{8BFD9FCD-CF3F-4946-9791-AAC37770C517}"/>
+    <cellStyle name="Percent 2 2" xfId="24" xr:uid="{5B4A32BC-2D03-4598-9EC9-ACA78BA94BFB}"/>
+    <cellStyle name="Percent 2 2 2" xfId="79" xr:uid="{FC5F31F7-54FD-4F4F-9317-7C1E75E9E3BB}"/>
+    <cellStyle name="Percent 2 2 2 2" xfId="184" xr:uid="{2A8E32BE-C94A-4DD2-90C9-94112466EF41}"/>
+    <cellStyle name="Percent 2 2 3" xfId="131" xr:uid="{425A8DD2-6A22-4039-97EE-D53CA44B19DD}"/>
+    <cellStyle name="Percent 2 3" xfId="37" xr:uid="{236B8580-D7D1-469D-AF95-E1CFD5B41119}"/>
+    <cellStyle name="Percent 2 3 2" xfId="92" xr:uid="{1ACB8966-E39F-4D01-82FF-A65C66A0ADC8}"/>
+    <cellStyle name="Percent 2 3 2 2" xfId="197" xr:uid="{B7AD31B6-D449-4CBE-9939-81318ABAF046}"/>
+    <cellStyle name="Percent 2 3 3" xfId="144" xr:uid="{83E4070D-767C-4F53-87F3-4898969296F8}"/>
+    <cellStyle name="Percent 2 4" xfId="50" xr:uid="{9260B4DB-A3D4-4976-97AA-4E5A1AD23684}"/>
+    <cellStyle name="Percent 2 4 2" xfId="105" xr:uid="{513B06AF-3ADE-4F9B-A6DA-37039A14F880}"/>
+    <cellStyle name="Percent 2 4 2 2" xfId="210" xr:uid="{5CA3032B-99B7-405F-9C8E-54DA37CFB930}"/>
+    <cellStyle name="Percent 2 4 3" xfId="157" xr:uid="{B15AD370-0144-4FDD-84AB-6482C09A230B}"/>
+    <cellStyle name="Percent 2 5" xfId="65" xr:uid="{6AF70087-790D-4B7D-90C0-B1FB37759188}"/>
+    <cellStyle name="Percent 2 5 2" xfId="171" xr:uid="{5FEAA66B-5EE7-49B3-9640-DAC60CE307E6}"/>
+    <cellStyle name="Percent 2 6" xfId="118" xr:uid="{B47EBB9B-C7EE-487E-9594-D1AA29CB900A}"/>
+    <cellStyle name="Percent 3" xfId="13" xr:uid="{FBA9ADE3-D1A0-43B5-910C-82408F637899}"/>
+    <cellStyle name="Percent 3 2" xfId="28" xr:uid="{C59C35C1-9ADF-4FA7-A3BF-AE805C05C2EE}"/>
+    <cellStyle name="Percent 3 2 2" xfId="83" xr:uid="{D27A9B6B-A7EA-42C6-BD8E-04E433A5147B}"/>
+    <cellStyle name="Percent 3 2 2 2" xfId="188" xr:uid="{3D7A89B1-364B-4297-8204-F2F0F302D138}"/>
+    <cellStyle name="Percent 3 2 3" xfId="135" xr:uid="{66C59DF8-BFE3-4813-9EF4-1B7D4885D29A}"/>
+    <cellStyle name="Percent 3 3" xfId="41" xr:uid="{A165D081-EC3D-46B1-B6C7-D2787E38FC85}"/>
+    <cellStyle name="Percent 3 3 2" xfId="96" xr:uid="{9A7797D2-6BE5-4468-80C1-DBA9C4DBD0B8}"/>
+    <cellStyle name="Percent 3 3 2 2" xfId="201" xr:uid="{55650E75-BD4B-47C4-9459-264441E678D9}"/>
+    <cellStyle name="Percent 3 3 3" xfId="148" xr:uid="{34A27936-BBD0-4531-8BCA-4FDA1F42E5CD}"/>
+    <cellStyle name="Percent 3 4" xfId="54" xr:uid="{B54C68FC-EB06-46F6-9510-89CE54A34328}"/>
+    <cellStyle name="Percent 3 4 2" xfId="109" xr:uid="{A7363051-84E2-4CF7-881B-AF8B10C784B6}"/>
+    <cellStyle name="Percent 3 4 2 2" xfId="214" xr:uid="{D5BDB50F-7EA3-4600-A2F9-0E928AC40357}"/>
+    <cellStyle name="Percent 3 4 3" xfId="161" xr:uid="{5D60557C-7C0D-409C-8700-B400A80F074E}"/>
+    <cellStyle name="Percent 3 5" xfId="69" xr:uid="{478AC944-C28B-42EF-B1D4-35E86AB9B888}"/>
+    <cellStyle name="Percent 3 5 2" xfId="175" xr:uid="{DAEB3EB4-FC2F-44C2-8625-94DE60249A15}"/>
+    <cellStyle name="Percent 3 6" xfId="122" xr:uid="{E4A0ED59-7C2B-4A39-8FA2-72C1551C2E75}"/>
+    <cellStyle name="Percent 4" xfId="20" xr:uid="{6A195803-FDB9-4226-97AE-B51FCAC37BB6}"/>
+    <cellStyle name="Percent 5" xfId="17" xr:uid="{B6A5AAB7-CBDE-4019-91D3-58A64847BAFD}"/>
+    <cellStyle name="Percent 5 2" xfId="73" xr:uid="{8DA4AE56-FA32-4F43-A95E-3B1A83EC0870}"/>
+    <cellStyle name="Percent 5 2 2" xfId="179" xr:uid="{BBCE41A6-0308-4EF4-978D-EA668BF3FD8F}"/>
+    <cellStyle name="Percent 5 3" xfId="126" xr:uid="{28179A12-E6CB-4974-A2A4-BCF0E056DBB4}"/>
+    <cellStyle name="Percent 6" xfId="32" xr:uid="{C9D84FF9-1809-4F65-8E73-C3A7C7682976}"/>
+    <cellStyle name="Percent 6 2" xfId="87" xr:uid="{E7BCB055-AEE1-44E1-8BAB-9ECA40EAEA2C}"/>
+    <cellStyle name="Percent 6 2 2" xfId="192" xr:uid="{FB1CC11A-1D55-493F-BB70-8FCF18B0AAA6}"/>
+    <cellStyle name="Percent 6 3" xfId="139" xr:uid="{F8B6D391-7AA8-4784-B01C-0628B603A2A6}"/>
+    <cellStyle name="Percent 7" xfId="45" xr:uid="{EC099B8F-9555-4D95-B8DF-DDA73C6646D9}"/>
+    <cellStyle name="Percent 7 2" xfId="100" xr:uid="{78254F7A-EAAD-4DA4-A0CC-1C925142EB15}"/>
+    <cellStyle name="Percent 7 2 2" xfId="205" xr:uid="{C4FB9B98-DF70-4314-893E-D6EBB23D9170}"/>
+    <cellStyle name="Percent 7 3" xfId="152" xr:uid="{92CF761C-1BBE-4D94-BF6D-AD7667227CE2}"/>
+    <cellStyle name="Percent 8" xfId="61" xr:uid="{1848715F-DE88-40CD-98AC-0CB6E56A7642}"/>
+    <cellStyle name="Percent 9" xfId="58" xr:uid="{657D1467-14DF-4F62-A66C-89876345DB56}"/>
+    <cellStyle name="Percent 9 2" xfId="166" xr:uid="{D3945A79-ED19-4CA5-8845-823608947536}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -659,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
-  <dimension ref="A2:O41"/>
+  <dimension ref="A2:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,7 +1151,7 @@
     <col min="15" max="15" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +1169,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -716,7 +1187,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -734,7 +1205,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -766,7 +1237,7 @@
         <v>11</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>12</v>
@@ -775,9 +1246,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -788,7 +1259,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
@@ -803,19 +1274,19 @@
         <v>1</v>
       </c>
       <c r="L6" s="19">
-        <f>-0.001*(D24/5)</f>
+        <f>-0.001*(D25/5)</f>
         <v>-24.2242</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N6" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
@@ -826,7 +1297,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="H7" s="2">
         <v>2019</v>
@@ -837,23 +1308,23 @@
       <c r="J7" s="2">
         <v>1.3</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="24">
         <v>1</v>
       </c>
-      <c r="L7" s="19">
+      <c r="L7" s="25">
         <f>L6</f>
         <v>-24.2242</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="24">
         <v>5</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N7" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
@@ -864,7 +1335,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H8" s="2">
         <v>2018</v>
@@ -875,539 +1346,635 @@
       <c r="J8" s="2">
         <v>1.3</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="24">
         <v>1</v>
       </c>
-      <c r="L8" s="19">
-        <v>-4</v>
-      </c>
-      <c r="M8" s="2">
+      <c r="L8" s="26">
+        <f>-H41/1000</f>
+        <v>-6.140814927000001</v>
+      </c>
+      <c r="M8" s="24">
         <v>5</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
+      <c r="N8" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="H9" s="24">
+        <v>2018</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="24">
+        <v>1.3</v>
+      </c>
+      <c r="K9" s="24">
+        <v>1</v>
+      </c>
+      <c r="L9" s="26">
+        <f>-H40/1000</f>
+        <v>-0.19678529000000003</v>
+      </c>
+      <c r="M9" s="24">
+        <v>5</v>
+      </c>
+      <c r="N9" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="24">
+        <v>2018</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="24">
+        <v>1.3</v>
+      </c>
+      <c r="K10" s="24">
+        <v>1</v>
+      </c>
+      <c r="L10" s="26">
+        <f>-H40/1000</f>
+        <v>-0.19678529000000003</v>
+      </c>
+      <c r="M10" s="27">
+        <v>5</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="2">
+      <c r="C11" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="24">
         <v>2018</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I11" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J11" s="24">
         <v>1.3</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K11" s="24">
         <v>1</v>
       </c>
-      <c r="L9" s="19">
-        <v>-0.1</v>
-      </c>
-      <c r="M9" s="2">
+      <c r="L11" s="26">
+        <f>-H39/1000</f>
+        <v>-0.56362277400000016</v>
+      </c>
+      <c r="M11" s="24">
         <v>5</v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="20" t="s">
+      <c r="N11" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="20">
-        <v>2018</v>
-      </c>
-      <c r="I10" s="20" t="s">
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J12" s="20">
         <v>1.3</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K12" s="20">
         <v>1</v>
       </c>
-      <c r="L10" s="21">
-        <v>-0.2</v>
-      </c>
-      <c r="M10" s="20">
+      <c r="L12" s="23">
+        <f>-H39/1000</f>
+        <v>-0.56362277400000016</v>
+      </c>
+      <c r="M12" s="20">
         <v>5</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="N12" s="20" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="O12" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="13" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E18" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C19" s="11">
         <v>228046</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D19" s="11">
         <v>9959</v>
       </c>
-      <c r="E18" s="14">
-        <f t="shared" ref="E18:E23" si="0">D18/C18</f>
+      <c r="E19" s="14">
+        <f t="shared" ref="E19:E24" si="0">D19/C19</f>
         <v>4.3671013742841359E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="6" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="21"/>
+      <c r="B20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C20" s="11">
         <v>100649</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D20" s="11">
         <v>6580</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E20" s="14">
         <f t="shared" si="0"/>
         <v>6.5375711631511485E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
-      <c r="B20" s="6" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
+      <c r="B21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C21" s="11">
         <v>4546</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D21" s="11">
         <v>201</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E21" s="14">
         <f t="shared" si="0"/>
         <v>4.4214694236691596E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
-      <c r="B21" s="6" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="21"/>
+      <c r="B22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C22" s="11">
         <v>6661</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D22" s="11">
         <v>329</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E22" s="14">
         <f t="shared" si="0"/>
         <v>4.9391983185707852E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="6" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="21"/>
+      <c r="B23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C23" s="11">
         <v>8424</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D23" s="11">
         <v>485</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E23" s="14">
         <f t="shared" si="0"/>
         <v>5.7573599240265907E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="6" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="21"/>
+      <c r="B24" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C24" s="11">
         <v>14373</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D24" s="11">
         <v>1033</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E24" s="14">
         <f t="shared" si="0"/>
         <v>7.187086899046824E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="11">
-        <v>2168099</v>
-      </c>
-      <c r="D24" s="11">
-        <v>121121</v>
-      </c>
-      <c r="E24" s="14">
-        <f>D24/C24</f>
-        <v>5.5865068892149296E-2</v>
-      </c>
-    </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C25" s="11">
-        <v>41471</v>
+        <v>2168099</v>
       </c>
       <c r="D25" s="11">
-        <v>2566</v>
+        <v>121121</v>
       </c>
       <c r="E25" s="14">
-        <f t="shared" ref="E25:E27" si="1">D25/C25</f>
-        <v>6.1874562947601935E-2</v>
+        <f>D25/C25</f>
+        <v>5.5865068892149296E-2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="11">
+        <v>41471</v>
+      </c>
+      <c r="D26" s="11">
+        <v>2566</v>
+      </c>
+      <c r="E26" s="14">
+        <f t="shared" ref="E26:E28" si="1">D26/C26</f>
+        <v>6.1874562947601935E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C27" s="11">
         <v>21457</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D27" s="11">
         <v>1224</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E27" s="14">
         <f t="shared" si="1"/>
         <v>5.7044321200540614E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C28" s="12">
         <v>11206</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D28" s="12">
         <v>551</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E28" s="15">
         <f t="shared" si="1"/>
         <v>4.9170087453150095E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B35" s="16">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B36" s="16">
         <v>0.3</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+      <c r="C37">
+        <v>2020</v>
+      </c>
+      <c r="D37">
+        <v>2021</v>
+      </c>
+      <c r="E37">
+        <v>2022</v>
+      </c>
+      <c r="F37">
+        <v>2023</v>
+      </c>
+      <c r="G37">
+        <v>2024</v>
+      </c>
+      <c r="H37">
+        <v>2025</v>
+      </c>
+      <c r="I37">
+        <v>2026</v>
+      </c>
+      <c r="J37">
+        <v>2027</v>
+      </c>
+      <c r="K37">
+        <v>2028</v>
+      </c>
+      <c r="L37">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>35</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>1</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <v>2</v>
       </c>
-      <c r="E37">
+      <c r="E38">
         <v>3</v>
       </c>
-      <c r="F37">
+      <c r="F38">
         <v>4</v>
       </c>
-      <c r="G37">
+      <c r="G38">
         <v>5</v>
       </c>
-      <c r="H37">
+      <c r="H38">
         <v>6</v>
       </c>
-      <c r="I37">
+      <c r="I38">
         <v>7</v>
       </c>
-      <c r="J37">
+      <c r="J38">
         <v>8</v>
       </c>
-      <c r="K37">
+      <c r="K38">
         <v>9</v>
       </c>
-      <c r="L37">
+      <c r="L38">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="18">
-        <f>D23+D22</f>
+      <c r="B39" s="18">
+        <f>D24+D23</f>
         <v>1518</v>
       </c>
-      <c r="C38" s="17">
-        <f>B38/10</f>
+      <c r="C39" s="17">
+        <f>B39/10</f>
         <v>151.80000000000001</v>
       </c>
-      <c r="D38" s="17">
-        <f t="shared" ref="D38:L38" si="2">C38*(1+$B$35)</f>
+      <c r="D39" s="17">
+        <f t="shared" ref="D39:L39" si="2">C39*(1+$B$36)</f>
         <v>197.34000000000003</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E39" s="17">
         <f t="shared" si="2"/>
         <v>256.54200000000003</v>
       </c>
-      <c r="F38" s="17">
+      <c r="F39" s="17">
         <f t="shared" si="2"/>
         <v>333.50460000000004</v>
       </c>
-      <c r="G38" s="17">
+      <c r="G39" s="17">
         <f t="shared" si="2"/>
         <v>433.55598000000009</v>
       </c>
-      <c r="H38" s="17">
+      <c r="H39" s="22">
         <f t="shared" si="2"/>
         <v>563.62277400000016</v>
       </c>
-      <c r="I38" s="17">
+      <c r="I39" s="17">
         <f t="shared" si="2"/>
         <v>732.70960620000028</v>
       </c>
-      <c r="J38" s="17">
+      <c r="J39" s="17">
         <f t="shared" si="2"/>
         <v>952.52248806000034</v>
       </c>
-      <c r="K38" s="17">
+      <c r="K39" s="17">
         <f t="shared" si="2"/>
         <v>1238.2792344780005</v>
       </c>
-      <c r="L38" s="17">
+      <c r="L39" s="17">
         <f t="shared" si="2"/>
         <v>1609.7630048214007</v>
       </c>
-      <c r="M38" s="17"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="M39" s="17"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="18">
-        <f>D21+D20</f>
+      <c r="B40" s="18">
+        <f>D22+D21</f>
         <v>530</v>
       </c>
-      <c r="C39" s="17">
-        <f>B39/10</f>
+      <c r="C40" s="17">
+        <f>B40/10</f>
         <v>53</v>
       </c>
-      <c r="D39" s="17">
-        <f t="shared" ref="D39:L39" si="3">C39*(1+$B$35)</f>
+      <c r="D40" s="17">
+        <f t="shared" ref="D40:L40" si="3">C40*(1+$B$36)</f>
         <v>68.900000000000006</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E40" s="17">
         <f t="shared" si="3"/>
         <v>89.570000000000007</v>
       </c>
-      <c r="F39" s="17">
+      <c r="F40" s="17">
         <f t="shared" si="3"/>
         <v>116.44100000000002</v>
       </c>
-      <c r="G39" s="17">
+      <c r="G40" s="17">
         <f t="shared" si="3"/>
         <v>151.37330000000003</v>
       </c>
-      <c r="H39" s="17">
+      <c r="H40" s="22">
         <f t="shared" si="3"/>
         <v>196.78529000000003</v>
       </c>
-      <c r="I39" s="17">
+      <c r="I40" s="17">
         <f t="shared" si="3"/>
         <v>255.82087700000005</v>
       </c>
-      <c r="J39" s="17">
+      <c r="J40" s="17">
         <f t="shared" si="3"/>
         <v>332.56714010000007</v>
       </c>
-      <c r="K39" s="17">
+      <c r="K40" s="17">
         <f t="shared" si="3"/>
         <v>432.33728213000012</v>
       </c>
-      <c r="L39" s="17">
+      <c r="L40" s="17">
         <f t="shared" si="3"/>
         <v>562.03846676900014</v>
       </c>
-      <c r="M39" s="17"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="M40" s="17"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="18">
-        <f>D19+D18</f>
+      <c r="B41" s="18">
+        <f>D20+D19</f>
         <v>16539</v>
       </c>
-      <c r="C40" s="17">
-        <f>B40/10</f>
+      <c r="C41" s="17">
+        <f>B41/10</f>
         <v>1653.9</v>
       </c>
-      <c r="D40" s="17">
-        <f t="shared" ref="D40:L40" si="4">C40*(1+$B$35)</f>
+      <c r="D41" s="17">
+        <f t="shared" ref="D41:L41" si="4">C41*(1+$B$36)</f>
         <v>2150.0700000000002</v>
       </c>
-      <c r="E40" s="17">
+      <c r="E41" s="17">
         <f t="shared" si="4"/>
         <v>2795.0910000000003</v>
       </c>
-      <c r="F40" s="17">
+      <c r="F41" s="17">
         <f t="shared" si="4"/>
         <v>3633.6183000000005</v>
       </c>
-      <c r="G40" s="17">
+      <c r="G41" s="17">
         <f t="shared" si="4"/>
         <v>4723.7037900000005</v>
       </c>
-      <c r="H40" s="17">
+      <c r="H41" s="22">
         <f t="shared" si="4"/>
         <v>6140.8149270000013</v>
       </c>
-      <c r="I40" s="17">
+      <c r="I41" s="17">
         <f t="shared" si="4"/>
         <v>7983.0594051000016</v>
       </c>
-      <c r="J40" s="17">
+      <c r="J41" s="17">
         <f t="shared" si="4"/>
         <v>10377.977226630002</v>
       </c>
-      <c r="K40" s="17">
+      <c r="K41" s="17">
         <f t="shared" si="4"/>
         <v>13491.370394619003</v>
       </c>
-      <c r="L40" s="17">
+      <c r="L41" s="17">
         <f t="shared" si="4"/>
         <v>17538.781513004706</v>
       </c>
-      <c r="M40" s="17"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="M41" s="17"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="18">
-        <f>D24</f>
+      <c r="B42" s="18">
+        <f>D25</f>
         <v>121121</v>
       </c>
-      <c r="C41" s="17">
-        <f>B41/5</f>
+      <c r="C42" s="17">
+        <f>B42/5</f>
         <v>24224.2</v>
       </c>
-      <c r="D41" s="17">
-        <f t="shared" ref="D41:L41" si="5">C41*(1+$B$35)</f>
+      <c r="D42" s="17">
+        <f t="shared" ref="D42:L42" si="5">C42*(1+$B$36)</f>
         <v>31491.460000000003</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E42" s="17">
         <f t="shared" si="5"/>
         <v>40938.898000000008</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F42" s="17">
         <f t="shared" si="5"/>
         <v>53220.567400000014</v>
       </c>
-      <c r="G41" s="17">
+      <c r="G42" s="17">
         <f t="shared" si="5"/>
         <v>69186.737620000014</v>
       </c>
-      <c r="H41" s="17">
+      <c r="H42" s="22">
         <f t="shared" si="5"/>
         <v>89942.758906000017</v>
       </c>
-      <c r="I41" s="17">
+      <c r="I42" s="17">
         <f t="shared" si="5"/>
         <v>116925.58657780003</v>
       </c>
-      <c r="J41" s="17">
+      <c r="J42" s="17">
         <f t="shared" si="5"/>
         <v>152003.26255114004</v>
       </c>
-      <c r="K41" s="17">
+      <c r="K42" s="17">
         <f t="shared" si="5"/>
         <v>197604.24131648205</v>
       </c>
-      <c r="L41" s="17">
+      <c r="L42" s="17">
         <f t="shared" si="5"/>
         <v>256885.51371142667</v>
       </c>
-      <c r="M41" s="17"/>
+      <c r="M42" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="A19:A24"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1416,6 +1983,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -1626,22 +2208,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1658,21 +2242,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add UC growth rate for other technologies
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874ABA08-2FA7-4CA9-BE51-22FD2CAFA3AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FE6E35-D99C-4D15-9649-1782EBE7C636}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -220,6 +220,51 @@
   </si>
   <si>
     <t>Cars-Maximum growth rate of PHEVs</t>
+  </si>
+  <si>
+    <t>UC-HGT_MaxGrowthFCV</t>
+  </si>
+  <si>
+    <t>T-HGT-FCV*</t>
+  </si>
+  <si>
+    <t>HGT-Maximum growth rate of FCVs</t>
+  </si>
+  <si>
+    <t>MGT-Maximum growth rate of FCVs</t>
+  </si>
+  <si>
+    <t>T-MGT-FCV*</t>
+  </si>
+  <si>
+    <t>UC-MGT-MaxGrowthFCV</t>
+  </si>
+  <si>
+    <t>T-CAR-FCV*</t>
+  </si>
+  <si>
+    <t>UC-CAR_MaxGrowthFCV</t>
+  </si>
+  <si>
+    <t>Cars-Maximum growth rate of FCVs</t>
+  </si>
+  <si>
+    <t>LGT-Maximum growth rate of PHEVs</t>
+  </si>
+  <si>
+    <t>LGT-Maximum growth rate of FCVs</t>
+  </si>
+  <si>
+    <t>T-LGT-PHEV*</t>
+  </si>
+  <si>
+    <t>T-LGT-FCV*</t>
+  </si>
+  <si>
+    <t>UC-LGT_MaxGrowthPHEV</t>
+  </si>
+  <si>
+    <t>UC-LGT_MaxGrowthFCV</t>
   </si>
 </sst>
 </file>
@@ -567,13 +612,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -589,17 +631,15 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="217">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -1130,15 +1170,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
-  <dimension ref="A2:O42"/>
+  <dimension ref="A2:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.21875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
@@ -1147,7 +1187,7 @@
     <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.5546875" customWidth="1"/>
-    <col min="14" max="14" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.88671875" customWidth="1"/>
     <col min="15" max="15" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1206,277 +1246,277 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="20">
         <v>2018</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="20">
         <v>1.3</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="20">
         <v>1</v>
       </c>
-      <c r="L6" s="19">
-        <f>-0.001*(D25/5)</f>
+      <c r="L6" s="21">
+        <f>-0.001*(D29/5)</f>
         <v>-24.2242</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="20">
         <v>5</v>
       </c>
-      <c r="N6" s="24" t="s">
+      <c r="N6" s="20" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="2">
-        <v>2019</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="H7" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="20">
         <v>1.3</v>
       </c>
-      <c r="K7" s="24">
+      <c r="K7" s="20">
         <v>1</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="21">
         <f>L6</f>
         <v>-24.2242</v>
       </c>
-      <c r="M7" s="24">
+      <c r="M7" s="20">
         <v>5</v>
       </c>
-      <c r="N7" s="24" t="s">
+      <c r="N7" s="20" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="20">
+        <v>1.3</v>
+      </c>
+      <c r="K8" s="20">
+        <v>1</v>
+      </c>
+      <c r="L8" s="21">
+        <f>L7</f>
+        <v>-24.2242</v>
+      </c>
+      <c r="M8" s="20">
+        <v>5</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H9" s="20">
         <v>2018</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J9" s="20">
         <v>1.3</v>
       </c>
-      <c r="K8" s="24">
+      <c r="K9" s="20">
         <v>1</v>
       </c>
-      <c r="L8" s="26">
-        <f>-H41/1000</f>
+      <c r="L9" s="22">
+        <f>-H45/1000</f>
         <v>-6.140814927000001</v>
       </c>
-      <c r="M8" s="24">
+      <c r="M9" s="20">
         <v>5</v>
       </c>
-      <c r="N8" s="24" t="s">
+      <c r="N9" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="24" t="s">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="24">
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="20">
         <v>2018</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J10" s="20">
         <v>1.3</v>
       </c>
-      <c r="K9" s="24">
+      <c r="K10" s="20">
         <v>1</v>
       </c>
-      <c r="L9" s="26">
-        <f>-H40/1000</f>
-        <v>-0.19678529000000003</v>
-      </c>
-      <c r="M9" s="24">
+      <c r="L10" s="22">
+        <f>L9</f>
+        <v>-6.140814927000001</v>
+      </c>
+      <c r="M10" s="20">
         <v>5</v>
       </c>
-      <c r="N9" s="24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="24" t="s">
+      <c r="N10" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="24">
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="20">
         <v>2018</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J11" s="20">
         <v>1.3</v>
       </c>
-      <c r="K10" s="24">
+      <c r="K11" s="20">
         <v>1</v>
       </c>
-      <c r="L10" s="26">
-        <f>-H40/1000</f>
-        <v>-0.19678529000000003</v>
-      </c>
-      <c r="M10" s="27">
+      <c r="L11" s="22">
+        <f>L10</f>
+        <v>-6.140814927000001</v>
+      </c>
+      <c r="M11" s="20">
         <v>5</v>
       </c>
-      <c r="N10" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="24">
-        <v>2018</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="24">
-        <v>1.3</v>
-      </c>
-      <c r="K11" s="24">
-        <v>1</v>
-      </c>
-      <c r="L11" s="26">
-        <f>-H39/1000</f>
-        <v>-0.56362277400000016</v>
-      </c>
-      <c r="M11" s="24">
-        <v>5</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>47</v>
+      <c r="N11" s="20" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="20" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>14</v>
@@ -1487,10 +1527,10 @@
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H12" s="20">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="I12" s="20" t="s">
         <v>16</v>
@@ -1501,480 +1541,670 @@
       <c r="K12" s="20">
         <v>1</v>
       </c>
-      <c r="L12" s="23">
-        <f>-H39/1000</f>
-        <v>-0.56362277400000016</v>
+      <c r="L12" s="22">
+        <f>-H44/1000</f>
+        <v>-0.19678529000000003</v>
       </c>
       <c r="M12" s="20">
         <v>5</v>
       </c>
       <c r="N12" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="20">
+        <v>1.3</v>
+      </c>
+      <c r="K13" s="20">
+        <v>1</v>
+      </c>
+      <c r="L13" s="22">
+        <f>-H44/1000</f>
+        <v>-0.19678529000000003</v>
+      </c>
+      <c r="M13" s="20">
+        <v>5</v>
+      </c>
+      <c r="N13" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="20">
+        <v>1.3</v>
+      </c>
+      <c r="K14" s="20">
+        <v>1</v>
+      </c>
+      <c r="L14" s="22">
+        <f>-H44/1000</f>
+        <v>-0.19678529000000003</v>
+      </c>
+      <c r="M14" s="20">
+        <v>5</v>
+      </c>
+      <c r="N14" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="20">
+        <v>1.3</v>
+      </c>
+      <c r="K15" s="20">
+        <v>1</v>
+      </c>
+      <c r="L15" s="22">
+        <f>-H43/1000</f>
+        <v>-0.56362277400000016</v>
+      </c>
+      <c r="M15" s="20">
+        <v>5</v>
+      </c>
+      <c r="N15" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="20">
+        <v>1.3</v>
+      </c>
+      <c r="K16" s="20">
+        <v>1</v>
+      </c>
+      <c r="L16" s="22">
+        <f>-H43/1000</f>
+        <v>-0.56362277400000016</v>
+      </c>
+      <c r="M16" s="20">
+        <v>5</v>
+      </c>
+      <c r="N16" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="O12" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="20">
+        <v>2018</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="20">
+        <v>1.3</v>
+      </c>
+      <c r="K17" s="20">
+        <v>1</v>
+      </c>
+      <c r="L17" s="22">
+        <f>-H43/1000</f>
+        <v>-0.56362277400000016</v>
+      </c>
+      <c r="M17" s="20">
+        <v>5</v>
+      </c>
+      <c r="N17" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="13" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E22" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C23" s="8">
         <v>228046</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D23" s="8">
         <v>9959</v>
       </c>
-      <c r="E19" s="14">
-        <f t="shared" ref="E19:E24" si="0">D19/C19</f>
+      <c r="E23" s="11">
+        <f t="shared" ref="E23:E28" si="0">D23/C23</f>
         <v>4.3671013742841359E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="6" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="19"/>
+      <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C24" s="8">
         <v>100649</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D24" s="8">
         <v>6580</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E24" s="11">
         <f t="shared" si="0"/>
         <v>6.5375711631511485E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="6" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="19"/>
+      <c r="B25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C25" s="8">
         <v>4546</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D25" s="8">
         <v>201</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E25" s="11">
         <f t="shared" si="0"/>
         <v>4.4214694236691596E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
-      <c r="B22" s="6" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="19"/>
+      <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C26" s="8">
         <v>6661</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D26" s="8">
         <v>329</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E26" s="11">
         <f t="shared" si="0"/>
         <v>4.9391983185707852E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="6" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="19"/>
+      <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C27" s="8">
         <v>8424</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D27" s="8">
         <v>485</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E27" s="11">
         <f t="shared" si="0"/>
         <v>5.7573599240265907E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="6" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="19"/>
+      <c r="B28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C28" s="8">
         <v>14373</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D28" s="8">
         <v>1033</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E28" s="11">
         <f t="shared" si="0"/>
         <v>7.187086899046824E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C29" s="8">
         <v>2168099</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D29" s="8">
         <v>121121</v>
       </c>
-      <c r="E25" s="14">
-        <f>D25/C25</f>
+      <c r="E29" s="11">
+        <f>D29/C29</f>
         <v>5.5865068892149296E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C30" s="8">
         <v>41471</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D30" s="8">
         <v>2566</v>
       </c>
-      <c r="E26" s="14">
-        <f t="shared" ref="E26:E28" si="1">D26/C26</f>
+      <c r="E30" s="11">
+        <f t="shared" ref="E30:E32" si="1">D30/C30</f>
         <v>6.1874562947601935E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="6" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C31" s="8">
         <v>21457</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D31" s="8">
         <v>1224</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E31" s="11">
         <f t="shared" si="1"/>
         <v>5.7044321200540614E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C32" s="9">
         <v>11206</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D32" s="9">
         <v>551</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E32" s="12">
         <f t="shared" si="1"/>
         <v>4.9170087453150095E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B36" s="16">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B40" s="13">
         <v>0.3</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C37">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C41">
         <v>2020</v>
       </c>
-      <c r="D37">
+      <c r="D41">
         <v>2021</v>
       </c>
-      <c r="E37">
+      <c r="E41">
         <v>2022</v>
       </c>
-      <c r="F37">
+      <c r="F41">
         <v>2023</v>
       </c>
-      <c r="G37">
+      <c r="G41">
         <v>2024</v>
       </c>
-      <c r="H37">
+      <c r="H41">
         <v>2025</v>
       </c>
-      <c r="I37">
+      <c r="I41">
         <v>2026</v>
       </c>
-      <c r="J37">
+      <c r="J41">
         <v>2027</v>
       </c>
-      <c r="K37">
+      <c r="K41">
         <v>2028</v>
       </c>
-      <c r="L37">
+      <c r="L41">
         <v>2029</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>35</v>
       </c>
-      <c r="C38">
+      <c r="C42">
         <v>1</v>
       </c>
-      <c r="D38">
+      <c r="D42">
         <v>2</v>
       </c>
-      <c r="E38">
+      <c r="E42">
         <v>3</v>
       </c>
-      <c r="F38">
+      <c r="F42">
         <v>4</v>
       </c>
-      <c r="G38">
+      <c r="G42">
         <v>5</v>
       </c>
-      <c r="H38">
+      <c r="H42">
         <v>6</v>
       </c>
-      <c r="I38">
+      <c r="I42">
         <v>7</v>
       </c>
-      <c r="J38">
+      <c r="J42">
         <v>8</v>
       </c>
-      <c r="K38">
+      <c r="K42">
         <v>9</v>
       </c>
-      <c r="L38">
+      <c r="L42">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="18">
-        <f>D24+D23</f>
+      <c r="B43" s="15">
+        <f>D28+D27</f>
         <v>1518</v>
       </c>
-      <c r="C39" s="17">
-        <f>B39/10</f>
+      <c r="C43" s="14">
+        <f>B43/10</f>
         <v>151.80000000000001</v>
       </c>
-      <c r="D39" s="17">
-        <f t="shared" ref="D39:L39" si="2">C39*(1+$B$36)</f>
+      <c r="D43" s="14">
+        <f t="shared" ref="D43:L43" si="2">C43*(1+$B$40)</f>
         <v>197.34000000000003</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E43" s="14">
         <f t="shared" si="2"/>
         <v>256.54200000000003</v>
       </c>
-      <c r="F39" s="17">
+      <c r="F43" s="14">
         <f t="shared" si="2"/>
         <v>333.50460000000004</v>
       </c>
-      <c r="G39" s="17">
+      <c r="G43" s="14">
         <f t="shared" si="2"/>
         <v>433.55598000000009</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H43" s="16">
         <f t="shared" si="2"/>
         <v>563.62277400000016</v>
       </c>
-      <c r="I39" s="17">
+      <c r="I43" s="14">
         <f t="shared" si="2"/>
         <v>732.70960620000028</v>
       </c>
-      <c r="J39" s="17">
+      <c r="J43" s="14">
         <f t="shared" si="2"/>
         <v>952.52248806000034</v>
       </c>
-      <c r="K39" s="17">
+      <c r="K43" s="14">
         <f t="shared" si="2"/>
         <v>1238.2792344780005</v>
       </c>
-      <c r="L39" s="17">
+      <c r="L43" s="14">
         <f t="shared" si="2"/>
         <v>1609.7630048214007</v>
       </c>
-      <c r="M39" s="17"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="M43" s="14"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="18">
-        <f>D22+D21</f>
+      <c r="B44" s="15">
+        <f>D26+D25</f>
         <v>530</v>
       </c>
-      <c r="C40" s="17">
-        <f>B40/10</f>
+      <c r="C44" s="14">
+        <f>B44/10</f>
         <v>53</v>
       </c>
-      <c r="D40" s="17">
-        <f t="shared" ref="D40:L40" si="3">C40*(1+$B$36)</f>
+      <c r="D44" s="14">
+        <f t="shared" ref="D44:L44" si="3">C44*(1+$B$40)</f>
         <v>68.900000000000006</v>
       </c>
-      <c r="E40" s="17">
+      <c r="E44" s="14">
         <f t="shared" si="3"/>
         <v>89.570000000000007</v>
       </c>
-      <c r="F40" s="17">
+      <c r="F44" s="14">
         <f t="shared" si="3"/>
         <v>116.44100000000002</v>
       </c>
-      <c r="G40" s="17">
+      <c r="G44" s="14">
         <f t="shared" si="3"/>
         <v>151.37330000000003</v>
       </c>
-      <c r="H40" s="22">
+      <c r="H44" s="16">
         <f t="shared" si="3"/>
         <v>196.78529000000003</v>
       </c>
-      <c r="I40" s="17">
+      <c r="I44" s="14">
         <f t="shared" si="3"/>
         <v>255.82087700000005</v>
       </c>
-      <c r="J40" s="17">
+      <c r="J44" s="14">
         <f t="shared" si="3"/>
         <v>332.56714010000007</v>
       </c>
-      <c r="K40" s="17">
+      <c r="K44" s="14">
         <f t="shared" si="3"/>
         <v>432.33728213000012</v>
       </c>
-      <c r="L40" s="17">
+      <c r="L44" s="14">
         <f t="shared" si="3"/>
         <v>562.03846676900014</v>
       </c>
-      <c r="M40" s="17"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="M44" s="14"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="18">
-        <f>D20+D19</f>
+      <c r="B45" s="15">
+        <f>D24+D23</f>
         <v>16539</v>
       </c>
-      <c r="C41" s="17">
-        <f>B41/10</f>
+      <c r="C45" s="14">
+        <f>B45/10</f>
         <v>1653.9</v>
       </c>
-      <c r="D41" s="17">
-        <f t="shared" ref="D41:L41" si="4">C41*(1+$B$36)</f>
+      <c r="D45" s="14">
+        <f t="shared" ref="D45:L45" si="4">C45*(1+$B$40)</f>
         <v>2150.0700000000002</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E45" s="14">
         <f t="shared" si="4"/>
         <v>2795.0910000000003</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F45" s="14">
         <f t="shared" si="4"/>
         <v>3633.6183000000005</v>
       </c>
-      <c r="G41" s="17">
+      <c r="G45" s="14">
         <f t="shared" si="4"/>
         <v>4723.7037900000005</v>
       </c>
-      <c r="H41" s="22">
+      <c r="H45" s="16">
         <f t="shared" si="4"/>
         <v>6140.8149270000013</v>
       </c>
-      <c r="I41" s="17">
+      <c r="I45" s="14">
         <f t="shared" si="4"/>
         <v>7983.0594051000016</v>
       </c>
-      <c r="J41" s="17">
+      <c r="J45" s="14">
         <f t="shared" si="4"/>
         <v>10377.977226630002</v>
       </c>
-      <c r="K41" s="17">
+      <c r="K45" s="14">
         <f t="shared" si="4"/>
         <v>13491.370394619003</v>
       </c>
-      <c r="L41" s="17">
+      <c r="L45" s="14">
         <f t="shared" si="4"/>
         <v>17538.781513004706</v>
       </c>
-      <c r="M41" s="17"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="M45" s="14"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="18">
-        <f>D25</f>
+      <c r="B46" s="15">
+        <f>D29</f>
         <v>121121</v>
       </c>
-      <c r="C42" s="17">
-        <f>B42/5</f>
+      <c r="C46" s="14">
+        <f>B46/5</f>
         <v>24224.2</v>
       </c>
-      <c r="D42" s="17">
-        <f t="shared" ref="D42:L42" si="5">C42*(1+$B$36)</f>
+      <c r="D46" s="14">
+        <f t="shared" ref="D46:L46" si="5">C46*(1+$B$40)</f>
         <v>31491.460000000003</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E46" s="14">
         <f t="shared" si="5"/>
         <v>40938.898000000008</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F46" s="14">
         <f t="shared" si="5"/>
         <v>53220.567400000014</v>
       </c>
-      <c r="G42" s="17">
+      <c r="G46" s="14">
         <f t="shared" si="5"/>
         <v>69186.737620000014</v>
       </c>
-      <c r="H42" s="22">
+      <c r="H46" s="16">
         <f t="shared" si="5"/>
         <v>89942.758906000017</v>
       </c>
-      <c r="I42" s="17">
+      <c r="I46" s="14">
         <f t="shared" si="5"/>
         <v>116925.58657780003</v>
       </c>
-      <c r="J42" s="17">
+      <c r="J46" s="14">
         <f t="shared" si="5"/>
         <v>152003.26255114004</v>
       </c>
-      <c r="K42" s="17">
+      <c r="K46" s="14">
         <f t="shared" si="5"/>
         <v>197604.24131648205</v>
       </c>
-      <c r="L42" s="17">
+      <c r="L46" s="14">
         <f t="shared" si="5"/>
         <v>256885.51371142667</v>
       </c>
-      <c r="M42" s="17"/>
+      <c r="M46" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A23:A28"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adjust seed value in UC growth rate for different technologies
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FE6E35-D99C-4D15-9649-1782EBE7C636}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE65335-E98B-49FB-9C7C-AD634799C326}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -276,7 +276,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +342,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -612,7 +619,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -634,12 +641,13 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="217">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -1172,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1287,459 +1295,459 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20" t="s">
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="19">
         <v>2018</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="19">
         <v>1.3</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="19">
         <v>1</v>
       </c>
-      <c r="L6" s="21">
-        <f>-0.001*(D29/5)</f>
+      <c r="L6" s="20">
+        <f>-J46/1000</f>
+        <v>-152.00326255114004</v>
+      </c>
+      <c r="M6" s="19">
+        <v>5</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="19">
+        <v>2018</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="19">
+        <v>1.3</v>
+      </c>
+      <c r="K7" s="19">
+        <v>1</v>
+      </c>
+      <c r="L7" s="20">
+        <f>-J46/1000</f>
+        <v>-152.00326255114004</v>
+      </c>
+      <c r="M7" s="19">
+        <v>5</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="19">
+        <v>2018</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="19">
+        <v>1.3</v>
+      </c>
+      <c r="K8" s="19">
+        <v>1</v>
+      </c>
+      <c r="L8" s="20">
+        <f>-C46/1000</f>
         <v>-24.2242</v>
       </c>
-      <c r="M6" s="20">
+      <c r="M8" s="19">
         <v>5</v>
       </c>
-      <c r="N6" s="20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="20" t="s">
+      <c r="N8" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="20">
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="19">
         <v>2018</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J9" s="19">
         <v>1.3</v>
       </c>
-      <c r="K7" s="20">
+      <c r="K9" s="19">
         <v>1</v>
       </c>
-      <c r="L7" s="21">
-        <f>L6</f>
-        <v>-24.2242</v>
-      </c>
-      <c r="M7" s="20">
+      <c r="L9" s="20">
+        <f>-J45/1000</f>
+        <v>-10.377977226630003</v>
+      </c>
+      <c r="M9" s="19">
         <v>5</v>
       </c>
-      <c r="N7" s="20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="20" t="s">
+      <c r="N9" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="20">
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="19">
         <v>2018</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J10" s="19">
         <v>1.3</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K10" s="19">
         <v>1</v>
       </c>
-      <c r="L8" s="21">
-        <f>L7</f>
-        <v>-24.2242</v>
-      </c>
-      <c r="M8" s="20">
+      <c r="L10" s="20">
+        <f>-J45/1000</f>
+        <v>-10.377977226630003</v>
+      </c>
+      <c r="M10" s="19">
         <v>5</v>
       </c>
-      <c r="N8" s="20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="20" t="s">
+      <c r="N10" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="20">
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="19">
         <v>2018</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J11" s="19">
         <v>1.3</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K11" s="19">
         <v>1</v>
       </c>
-      <c r="L9" s="22">
-        <f>-H45/1000</f>
-        <v>-6.140814927000001</v>
-      </c>
-      <c r="M9" s="20">
+      <c r="L11" s="20">
+        <f>-C45/1000</f>
+        <v>-1.6539000000000001</v>
+      </c>
+      <c r="M11" s="19">
         <v>5</v>
       </c>
-      <c r="N9" s="20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="20" t="s">
+      <c r="N11" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="20">
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="19">
         <v>2018</v>
       </c>
-      <c r="I10" s="20" t="s">
+      <c r="I12" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J12" s="19">
         <v>1.3</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K12" s="19">
         <v>1</v>
       </c>
-      <c r="L10" s="22">
-        <f>L9</f>
-        <v>-6.140814927000001</v>
-      </c>
-      <c r="M10" s="20">
+      <c r="L12" s="20">
+        <f>-J44/1000</f>
+        <v>-0.33256714010000005</v>
+      </c>
+      <c r="M12" s="19">
         <v>5</v>
       </c>
-      <c r="N10" s="20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="20" t="s">
+      <c r="N12" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" s="20">
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="19">
         <v>2018</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I13" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J13" s="19">
         <v>1.3</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K13" s="19">
         <v>1</v>
       </c>
-      <c r="L11" s="22">
-        <f>L10</f>
-        <v>-6.140814927000001</v>
-      </c>
-      <c r="M11" s="20">
+      <c r="L13" s="20">
+        <f>-J44/1000</f>
+        <v>-0.33256714010000005</v>
+      </c>
+      <c r="M13" s="19">
         <v>5</v>
       </c>
-      <c r="N11" s="20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="20" t="s">
+      <c r="N13" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="20">
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="19">
         <v>2018</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J14" s="19">
         <v>1.3</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K14" s="19">
         <v>1</v>
       </c>
-      <c r="L12" s="22">
-        <f>-H44/1000</f>
-        <v>-0.19678529000000003</v>
-      </c>
-      <c r="M12" s="20">
+      <c r="L14" s="20">
+        <f>-C44/1000</f>
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="M14" s="19">
         <v>5</v>
       </c>
-      <c r="N12" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="20" t="s">
+      <c r="N14" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D15" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="20">
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="19">
         <v>2018</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I15" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J15" s="19">
         <v>1.3</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K15" s="19">
         <v>1</v>
       </c>
-      <c r="L13" s="22">
-        <f>-H44/1000</f>
-        <v>-0.19678529000000003</v>
-      </c>
-      <c r="M13" s="20">
+      <c r="L15" s="20">
+        <f>-J43/1000</f>
+        <v>-0.95252248806000039</v>
+      </c>
+      <c r="M15" s="19">
         <v>5</v>
       </c>
-      <c r="N13" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="20" t="s">
+      <c r="N15" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D16" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="20">
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="19">
         <v>2018</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="I16" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J16" s="19">
         <v>1.3</v>
       </c>
-      <c r="K14" s="20">
+      <c r="K16" s="19">
         <v>1</v>
       </c>
-      <c r="L14" s="22">
-        <f>-H44/1000</f>
-        <v>-0.19678529000000003</v>
-      </c>
-      <c r="M14" s="20">
+      <c r="L16" s="20">
+        <f>L15</f>
+        <v>-0.95252248806000039</v>
+      </c>
+      <c r="M16" s="19">
         <v>5</v>
       </c>
-      <c r="N14" s="20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="20" t="s">
+      <c r="N16" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="20">
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="19">
         <v>2018</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I17" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J17" s="19">
         <v>1.3</v>
       </c>
-      <c r="K15" s="20">
+      <c r="K17" s="19">
         <v>1</v>
       </c>
-      <c r="L15" s="22">
-        <f>-H43/1000</f>
-        <v>-0.56362277400000016</v>
-      </c>
-      <c r="M15" s="20">
+      <c r="L17" s="20">
+        <f>-C43/1000</f>
+        <v>-0.15180000000000002</v>
+      </c>
+      <c r="M17" s="19">
         <v>5</v>
       </c>
-      <c r="N15" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" s="20">
-        <v>2018</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="20">
-        <v>1.3</v>
-      </c>
-      <c r="K16" s="20">
-        <v>1</v>
-      </c>
-      <c r="L16" s="22">
-        <f>-H43/1000</f>
-        <v>-0.56362277400000016</v>
-      </c>
-      <c r="M16" s="20">
-        <v>5</v>
-      </c>
-      <c r="N16" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="20">
-        <v>2018</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="20">
-        <v>1.3</v>
-      </c>
-      <c r="K17" s="20">
-        <v>1</v>
-      </c>
-      <c r="L17" s="22">
-        <f>-H43/1000</f>
-        <v>-0.56362277400000016</v>
-      </c>
-      <c r="M17" s="20">
-        <v>5</v>
-      </c>
-      <c r="N17" s="20" t="s">
+      <c r="N17" s="19" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1762,7 +1770,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1780,7 +1788,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
@@ -1796,7 +1804,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="3" t="s">
         <v>25</v>
       </c>
@@ -1812,7 +1820,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="19"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
@@ -1828,7 +1836,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="19"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
@@ -1844,7 +1852,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="19"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="3" t="s">
         <v>22</v>
       </c>
@@ -1937,34 +1945,34 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C41">
+        <v>2018</v>
+      </c>
+      <c r="D41">
+        <v>2019</v>
+      </c>
+      <c r="E41">
         <v>2020</v>
       </c>
-      <c r="D41">
+      <c r="F41">
         <v>2021</v>
       </c>
-      <c r="E41">
+      <c r="G41">
         <v>2022</v>
       </c>
-      <c r="F41">
+      <c r="H41">
         <v>2023</v>
       </c>
-      <c r="G41">
+      <c r="I41">
         <v>2024</v>
       </c>
-      <c r="H41">
+      <c r="J41">
         <v>2025</v>
       </c>
-      <c r="I41">
+      <c r="K41">
         <v>2026</v>
       </c>
-      <c r="J41">
+      <c r="L41">
         <v>2027</v>
-      </c>
-      <c r="K41">
-        <v>2028</v>
-      </c>
-      <c r="L41">
-        <v>2029</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -1992,7 +2000,7 @@
       <c r="I42">
         <v>7</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="22">
         <v>8</v>
       </c>
       <c r="K42">
@@ -2038,7 +2046,7 @@
         <f t="shared" si="2"/>
         <v>732.70960620000028</v>
       </c>
-      <c r="J43" s="14">
+      <c r="J43" s="23">
         <f t="shared" si="2"/>
         <v>952.52248806000034</v>
       </c>
@@ -2088,7 +2096,7 @@
         <f t="shared" si="3"/>
         <v>255.82087700000005</v>
       </c>
-      <c r="J44" s="14">
+      <c r="J44" s="23">
         <f t="shared" si="3"/>
         <v>332.56714010000007</v>
       </c>
@@ -2138,7 +2146,7 @@
         <f t="shared" si="4"/>
         <v>7983.0594051000016</v>
       </c>
-      <c r="J45" s="14">
+      <c r="J45" s="23">
         <f t="shared" si="4"/>
         <v>10377.977226630002</v>
       </c>
@@ -2188,7 +2196,7 @@
         <f t="shared" si="5"/>
         <v>116925.58657780003</v>
       </c>
-      <c r="J46" s="14">
+      <c r="J46" s="23">
         <f t="shared" si="5"/>
         <v>152003.26255114004</v>
       </c>
@@ -2213,21 +2221,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -2438,24 +2431,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2472,4 +2463,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add seed value for FCV for 2030 in UC growth rate
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE65335-E98B-49FB-9C7C-AD634799C326}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE69AF6-E84D-4015-A9D5-84A74DBF30EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>UC-LGT_MaxGrowthFCV</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS~2030</t>
   </si>
 </sst>
 </file>
@@ -276,7 +279,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,13 +329,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -405,78 +401,78 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -619,7 +615,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -638,16 +634,15 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="217">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -1178,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
-  <dimension ref="A2:O46"/>
+  <dimension ref="A2:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1194,12 +1189,12 @@
     <col min="10" max="10" width="11.44140625" customWidth="1"/>
     <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" customWidth="1"/>
-    <col min="14" max="14" width="35.88671875" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" customWidth="1"/>
+    <col min="13" max="14" width="17.5546875" customWidth="1"/>
+    <col min="15" max="15" width="33.109375" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1216,8 +1211,9 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1234,8 +1230,9 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1252,30 +1249,31 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="17" t="s">
         <v>9</v>
       </c>
       <c r="J5" s="5" t="s">
@@ -1288,475 +1286,490 @@
         <v>44</v>
       </c>
       <c r="M5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="19" t="s">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19" t="s">
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="18">
         <v>2018</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="18">
         <v>1.3</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="18">
         <v>1</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="19">
         <f>-J46/1000</f>
         <v>-152.00326255114004</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="19"/>
+      <c r="N6" s="18">
         <v>5</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="O6" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19" t="s">
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="18">
         <v>2018</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="18">
         <v>1.3</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="18">
         <v>1</v>
       </c>
-      <c r="L7" s="20">
+      <c r="L7" s="19">
         <f>-J46/1000</f>
         <v>-152.00326255114004</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="19"/>
+      <c r="N7" s="18">
         <v>5</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="O7" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19" t="s">
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="18">
         <v>2018</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="18">
         <v>1.3</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="18">
         <v>1</v>
       </c>
-      <c r="L8" s="20">
-        <f>-C46/1000</f>
-        <v>-24.2242</v>
-      </c>
+      <c r="L8" s="19"/>
       <c r="M8" s="19">
+        <f>-E46/1000</f>
+        <v>-40.938898000000009</v>
+      </c>
+      <c r="N8" s="18">
         <v>5</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="O8" s="18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="19" t="s">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19" t="s">
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="18">
         <v>2018</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="18">
         <v>1.3</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="18">
         <v>1</v>
       </c>
-      <c r="L9" s="20">
+      <c r="L9" s="19">
         <f>-J45/1000</f>
         <v>-10.377977226630003</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="19"/>
+      <c r="N9" s="18">
         <v>5</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="O9" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="19" t="s">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19" t="s">
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="18">
         <v>2018</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="18">
         <v>1.3</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="18">
         <v>1</v>
       </c>
-      <c r="L10" s="20">
+      <c r="L10" s="19">
         <f>-J45/1000</f>
         <v>-10.377977226630003</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="19"/>
+      <c r="N10" s="18">
         <v>5</v>
       </c>
-      <c r="N10" s="19" t="s">
+      <c r="O10" s="18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="19" t="s">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19" t="s">
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="18">
         <v>2018</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="18">
         <v>1.3</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="18">
         <v>1</v>
       </c>
-      <c r="L11" s="20">
-        <f>-C45/1000</f>
-        <v>-1.6539000000000001</v>
-      </c>
+      <c r="L11" s="19"/>
       <c r="M11" s="19">
+        <f>-E45/1000</f>
+        <v>-2.7950910000000002</v>
+      </c>
+      <c r="N11" s="18">
         <v>5</v>
       </c>
-      <c r="N11" s="19" t="s">
+      <c r="O11" s="18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19" t="s">
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="18">
         <v>2018</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="18">
         <v>1.3</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="18">
         <v>1</v>
       </c>
-      <c r="L12" s="20">
+      <c r="L12" s="19">
         <f>-J44/1000</f>
         <v>-0.33256714010000005</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="19"/>
+      <c r="N12" s="18">
         <v>5</v>
       </c>
-      <c r="N12" s="19" t="s">
+      <c r="O12" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="19" t="s">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19" t="s">
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <v>2018</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="18">
         <v>1.3</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="18">
         <v>1</v>
       </c>
-      <c r="L13" s="20">
-        <f>-J44/1000</f>
-        <v>-0.33256714010000005</v>
-      </c>
-      <c r="M13" s="19">
+      <c r="L13" s="19">
+        <f>-L44/1000</f>
+        <v>-0.56203846676900016</v>
+      </c>
+      <c r="M13" s="19"/>
+      <c r="N13" s="18">
         <v>5</v>
       </c>
-      <c r="N13" s="19" t="s">
+      <c r="O13" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="19" t="s">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19" t="s">
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="18">
         <v>2018</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="18">
         <v>1.3</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="18">
         <v>1</v>
       </c>
-      <c r="L14" s="20">
-        <f>-C44/1000</f>
-        <v>-5.2999999999999999E-2</v>
-      </c>
+      <c r="L14" s="19"/>
       <c r="M14" s="19">
+        <f>-E44/1000</f>
+        <v>-8.9570000000000011E-2</v>
+      </c>
+      <c r="N14" s="18">
         <v>5</v>
       </c>
-      <c r="N14" s="19" t="s">
+      <c r="O14" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19" t="s">
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="18">
         <v>2018</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="18">
         <v>1.3</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="18">
         <v>1</v>
       </c>
-      <c r="L15" s="20">
+      <c r="L15" s="19">
         <f>-J43/1000</f>
         <v>-0.95252248806000039</v>
       </c>
-      <c r="M15" s="19">
+      <c r="M15" s="19"/>
+      <c r="N15" s="18">
         <v>5</v>
       </c>
-      <c r="N15" s="19" t="s">
+      <c r="O15" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="19" t="s">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19" t="s">
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="18">
         <v>2018</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="18">
         <v>1.3</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="18">
         <v>1</v>
       </c>
-      <c r="L16" s="20">
-        <f>L15</f>
-        <v>-0.95252248806000039</v>
-      </c>
-      <c r="M16" s="19">
+      <c r="L16" s="19">
+        <f>-L43/1000</f>
+        <v>-1.6097630048214007</v>
+      </c>
+      <c r="M16" s="19"/>
+      <c r="N16" s="18">
         <v>5</v>
       </c>
-      <c r="N16" s="19" t="s">
+      <c r="O16" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="19" t="s">
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19" t="s">
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="18">
         <v>2018</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="18">
         <v>1.3</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="18">
         <v>1</v>
       </c>
-      <c r="L17" s="20">
-        <f>-C43/1000</f>
-        <v>-0.15180000000000002</v>
-      </c>
+      <c r="L17" s="19"/>
       <c r="M17" s="19">
+        <f>-E43/1000</f>
+        <v>-0.25654200000000005</v>
+      </c>
+      <c r="N17" s="18">
         <v>5</v>
       </c>
-      <c r="N17" s="19" t="s">
+      <c r="O17" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="10" t="s">
@@ -1769,8 +1782,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1787,8 +1800,8 @@
         <v>4.3671013742841359E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
       <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
@@ -1803,8 +1816,8 @@
         <v>6.5375711631511485E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
       <c r="B25" s="3" t="s">
         <v>25</v>
       </c>
@@ -1819,8 +1832,8 @@
         <v>4.4214694236691596E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="21"/>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
       <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
@@ -1835,8 +1848,8 @@
         <v>4.9391983185707852E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
       <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
@@ -1851,8 +1864,8 @@
         <v>5.7573599240265907E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="22"/>
       <c r="B28" s="3" t="s">
         <v>22</v>
       </c>
@@ -1867,7 +1880,7 @@
         <v>7.187086899046824E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>21</v>
       </c>
@@ -1882,7 +1895,7 @@
         <v>5.5865068892149296E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>20</v>
       </c>
@@ -1897,7 +1910,7 @@
         <v>6.1874562947601935E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>19</v>
       </c>
@@ -1912,7 +1925,7 @@
         <v>5.7044321200540614E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="7" t="s">
         <v>18</v>
@@ -1928,22 +1941,22 @@
         <v>4.9170087453150095E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B40" s="13">
         <v>0.3</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>2018</v>
       </c>
@@ -1975,7 +1988,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>35</v>
       </c>
@@ -2000,7 +2013,7 @@
       <c r="I42">
         <v>7</v>
       </c>
-      <c r="J42" s="22">
+      <c r="J42" s="20">
         <v>8</v>
       </c>
       <c r="K42">
@@ -2010,7 +2023,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2038,7 +2051,7 @@
         <f t="shared" si="2"/>
         <v>433.55598000000009</v>
       </c>
-      <c r="H43" s="16">
+      <c r="H43" s="14">
         <f t="shared" si="2"/>
         <v>563.62277400000016</v>
       </c>
@@ -2046,7 +2059,7 @@
         <f t="shared" si="2"/>
         <v>732.70960620000028</v>
       </c>
-      <c r="J43" s="23">
+      <c r="J43" s="21">
         <f t="shared" si="2"/>
         <v>952.52248806000034</v>
       </c>
@@ -2059,8 +2072,9 @@
         <v>1609.7630048214007</v>
       </c>
       <c r="M43" s="14"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N43" s="14"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -2088,7 +2102,7 @@
         <f t="shared" si="3"/>
         <v>151.37330000000003</v>
       </c>
-      <c r="H44" s="16">
+      <c r="H44" s="14">
         <f t="shared" si="3"/>
         <v>196.78529000000003</v>
       </c>
@@ -2096,7 +2110,7 @@
         <f t="shared" si="3"/>
         <v>255.82087700000005</v>
       </c>
-      <c r="J44" s="23">
+      <c r="J44" s="21">
         <f t="shared" si="3"/>
         <v>332.56714010000007</v>
       </c>
@@ -2109,8 +2123,9 @@
         <v>562.03846676900014</v>
       </c>
       <c r="M44" s="14"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N44" s="14"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -2138,7 +2153,7 @@
         <f t="shared" si="4"/>
         <v>4723.7037900000005</v>
       </c>
-      <c r="H45" s="16">
+      <c r="H45" s="14">
         <f t="shared" si="4"/>
         <v>6140.8149270000013</v>
       </c>
@@ -2146,7 +2161,7 @@
         <f t="shared" si="4"/>
         <v>7983.0594051000016</v>
       </c>
-      <c r="J45" s="23">
+      <c r="J45" s="21">
         <f t="shared" si="4"/>
         <v>10377.977226630002</v>
       </c>
@@ -2159,8 +2174,9 @@
         <v>17538.781513004706</v>
       </c>
       <c r="M45" s="14"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N45" s="14"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -2188,7 +2204,7 @@
         <f t="shared" si="5"/>
         <v>69186.737620000014</v>
       </c>
-      <c r="H46" s="16">
+      <c r="H46" s="14">
         <f t="shared" si="5"/>
         <v>89942.758906000017</v>
       </c>
@@ -2196,7 +2212,7 @@
         <f t="shared" si="5"/>
         <v>116925.58657780003</v>
       </c>
-      <c r="J46" s="23">
+      <c r="J46" s="21">
         <f t="shared" si="5"/>
         <v>152003.26255114004</v>
       </c>
@@ -2209,6 +2225,7 @@
         <v>256885.51371142667</v>
       </c>
       <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2221,6 +2238,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -2431,22 +2463,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2463,21 +2497,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modify growth rate for FCV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE69AF6-E84D-4015-A9D5-84A74DBF30EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F031B651-A366-4AD9-A3F0-9843698A0548}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -265,9 +265,6 @@
   </si>
   <si>
     <t>UC-LGT_MaxGrowthFCV</t>
-  </si>
-  <si>
-    <t>UC_RHSRTS~2030</t>
   </si>
 </sst>
 </file>
@@ -615,7 +612,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -643,6 +640,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="217">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -1173,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
-  <dimension ref="A2:P46"/>
+  <dimension ref="A2:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,12 +1188,12 @@
     <col min="10" max="10" width="11.44140625" customWidth="1"/>
     <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="17.5546875" customWidth="1"/>
-    <col min="15" max="15" width="33.109375" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="14" max="14" width="33.109375" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1211,9 +1210,8 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1230,9 +1228,8 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1249,9 +1246,8 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1286,16 +1282,13 @@
         <v>44</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
         <v>58</v>
       </c>
@@ -1326,15 +1319,14 @@
         <f>-J46/1000</f>
         <v>-152.00326255114004</v>
       </c>
-      <c r="M6" s="19"/>
-      <c r="N6" s="18">
+      <c r="M6" s="18">
         <v>5</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="N6" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="18" t="s">
         <v>59</v>
       </c>
@@ -1365,54 +1357,52 @@
         <f>-J46/1000</f>
         <v>-152.00326255114004</v>
       </c>
-      <c r="M7" s="19"/>
-      <c r="N7" s="18">
+      <c r="M7" s="18">
         <v>5</v>
       </c>
-      <c r="O7" s="18" t="s">
+      <c r="N7" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="23">
         <v>2018</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="18">
-        <v>1.3</v>
-      </c>
-      <c r="K8" s="18">
+      <c r="J8" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="K8" s="23">
         <v>1</v>
       </c>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19">
-        <f>-E46/1000</f>
-        <v>-40.938898000000009</v>
-      </c>
-      <c r="N8" s="18">
+      <c r="L8" s="24">
+        <f>-C46/1000</f>
+        <v>-24.2242</v>
+      </c>
+      <c r="M8" s="23">
         <v>5</v>
       </c>
-      <c r="O8" s="18" t="s">
+      <c r="N8" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>56</v>
       </c>
@@ -1443,15 +1433,14 @@
         <f>-J45/1000</f>
         <v>-10.377977226630003</v>
       </c>
-      <c r="M9" s="19"/>
-      <c r="N9" s="18">
+      <c r="M9" s="18">
         <v>5</v>
       </c>
-      <c r="O9" s="18" t="s">
+      <c r="N9" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>75</v>
       </c>
@@ -1482,54 +1471,52 @@
         <f>-J45/1000</f>
         <v>-10.377977226630003</v>
       </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="18">
+      <c r="M10" s="18">
         <v>5</v>
       </c>
-      <c r="O10" s="18" t="s">
+      <c r="N10" s="18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="18" t="s">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18" t="s">
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="23">
         <v>2018</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="18">
-        <v>1.3</v>
-      </c>
-      <c r="K11" s="18">
+      <c r="J11" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="K11" s="23">
         <v>1</v>
       </c>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19">
-        <f>-E45/1000</f>
-        <v>-2.7950910000000002</v>
-      </c>
-      <c r="N11" s="18">
+      <c r="L11" s="24">
+        <f>-C45/1000</f>
+        <v>-1.6539000000000001</v>
+      </c>
+      <c r="M11" s="23">
         <v>5</v>
       </c>
-      <c r="O11" s="18" t="s">
+      <c r="N11" s="23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
         <v>52</v>
       </c>
@@ -1560,15 +1547,14 @@
         <f>-J44/1000</f>
         <v>-0.33256714010000005</v>
       </c>
-      <c r="M12" s="19"/>
-      <c r="N12" s="18">
+      <c r="M12" s="18">
         <v>5</v>
       </c>
-      <c r="O12" s="18" t="s">
+      <c r="N12" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
         <v>53</v>
       </c>
@@ -1599,54 +1585,52 @@
         <f>-L44/1000</f>
         <v>-0.56203846676900016</v>
       </c>
-      <c r="M13" s="19"/>
-      <c r="N13" s="18">
+      <c r="M13" s="18">
         <v>5</v>
       </c>
-      <c r="O13" s="18" t="s">
+      <c r="N13" s="18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="18" t="s">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18" t="s">
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="23">
         <v>2018</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="18">
-        <v>1.3</v>
-      </c>
-      <c r="K14" s="18">
+      <c r="J14" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="K14" s="23">
         <v>1</v>
       </c>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19">
-        <f>-E44/1000</f>
-        <v>-8.9570000000000011E-2</v>
-      </c>
-      <c r="N14" s="18">
+      <c r="L14" s="24">
+        <f>-C44/1000</f>
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="M14" s="23">
         <v>5</v>
       </c>
-      <c r="O14" s="18" t="s">
+      <c r="N14" s="23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
         <v>48</v>
       </c>
@@ -1677,15 +1661,14 @@
         <f>-J43/1000</f>
         <v>-0.95252248806000039</v>
       </c>
-      <c r="M15" s="19"/>
-      <c r="N15" s="18">
+      <c r="M15" s="18">
         <v>5</v>
       </c>
-      <c r="O15" s="18" t="s">
+      <c r="N15" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>49</v>
       </c>
@@ -1716,60 +1699,58 @@
         <f>-L43/1000</f>
         <v>-1.6097630048214007</v>
       </c>
-      <c r="M16" s="19"/>
-      <c r="N16" s="18">
+      <c r="M16" s="18">
         <v>5</v>
       </c>
-      <c r="O16" s="18" t="s">
+      <c r="N16" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="18" t="s">
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18" t="s">
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="23">
         <v>2018</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="I17" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="18">
-        <v>1.3</v>
-      </c>
-      <c r="K17" s="18">
+      <c r="J17" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="K17" s="23">
         <v>1</v>
       </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19">
-        <f>-E43/1000</f>
-        <v>-0.25654200000000005</v>
-      </c>
-      <c r="N17" s="18">
+      <c r="L17" s="24">
+        <f>-C43/1000</f>
+        <v>-0.15180000000000002</v>
+      </c>
+      <c r="M17" s="23">
         <v>5</v>
       </c>
-      <c r="O17" s="18" t="s">
+      <c r="N17" s="23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="10" t="s">
@@ -1782,7 +1763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>28</v>
       </c>
@@ -1800,7 +1781,7 @@
         <v>4.3671013742841359E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="3" t="s">
         <v>26</v>
@@ -1816,7 +1797,7 @@
         <v>6.5375711631511485E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="3" t="s">
         <v>25</v>
@@ -1832,7 +1813,7 @@
         <v>4.4214694236691596E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="3" t="s">
         <v>24</v>
@@ -1848,7 +1829,7 @@
         <v>4.9391983185707852E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="22"/>
       <c r="B27" s="3" t="s">
         <v>23</v>
@@ -1864,7 +1845,7 @@
         <v>5.7573599240265907E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="22"/>
       <c r="B28" s="3" t="s">
         <v>22</v>
@@ -1880,7 +1861,7 @@
         <v>7.187086899046824E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>21</v>
       </c>
@@ -1895,7 +1876,7 @@
         <v>5.5865068892149296E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>20</v>
       </c>
@@ -1910,7 +1891,7 @@
         <v>6.1874562947601935E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>19</v>
       </c>
@@ -1925,7 +1906,7 @@
         <v>5.7044321200540614E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="7" t="s">
         <v>18</v>
@@ -1941,22 +1922,22 @@
         <v>4.9170087453150095E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B40" s="13">
         <v>0.3</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>2018</v>
       </c>
@@ -1988,7 +1969,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>35</v>
       </c>
@@ -2023,7 +2004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2072,9 +2053,8 @@
         <v>1609.7630048214007</v>
       </c>
       <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -2123,9 +2103,8 @@
         <v>562.03846676900014</v>
       </c>
       <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -2174,9 +2153,8 @@
         <v>17538.781513004706</v>
       </c>
       <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -2225,7 +2203,6 @@
         <v>256885.51371142667</v>
       </c>
       <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Change seed value for UC growth rate
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F031B651-A366-4AD9-A3F0-9843698A0548}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0073FCF-AE3C-4F39-87E0-0A4878422B78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -637,11 +637,11 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="217">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -1174,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,40 +1365,40 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23" t="s">
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="22">
         <v>2018</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="23">
+      <c r="J8" s="22">
         <v>1.2</v>
       </c>
-      <c r="K8" s="23">
+      <c r="K8" s="22">
         <v>1</v>
       </c>
-      <c r="L8" s="24">
+      <c r="L8" s="23">
         <f>-C46/1000</f>
         <v>-24.2242</v>
       </c>
-      <c r="M8" s="23">
+      <c r="M8" s="22">
         <v>5</v>
       </c>
-      <c r="N8" s="23" t="s">
+      <c r="N8" s="22" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1479,40 +1479,40 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23" t="s">
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="22">
         <v>2018</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="22">
         <v>1.2</v>
       </c>
-      <c r="K11" s="23">
+      <c r="K11" s="22">
         <v>1</v>
       </c>
-      <c r="L11" s="24">
+      <c r="L11" s="23">
         <f>-C45/1000</f>
         <v>-1.6539000000000001</v>
       </c>
-      <c r="M11" s="23">
+      <c r="M11" s="22">
         <v>5</v>
       </c>
-      <c r="N11" s="23" t="s">
+      <c r="N11" s="22" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1544,8 +1544,8 @@
         <v>1</v>
       </c>
       <c r="L12" s="19">
-        <f>-J44/1000</f>
-        <v>-0.33256714010000005</v>
+        <f>-L44/1000</f>
+        <v>-0.56203846676900016</v>
       </c>
       <c r="M12" s="18">
         <v>5</v>
@@ -1593,40 +1593,40 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23" t="s">
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="22">
         <v>2018</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="22">
         <v>1.2</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="22">
         <v>1</v>
       </c>
-      <c r="L14" s="24">
+      <c r="L14" s="23">
         <f>-C44/1000</f>
         <v>-5.2999999999999999E-2</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="22">
         <v>5</v>
       </c>
-      <c r="N14" s="23" t="s">
+      <c r="N14" s="22" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1658,8 +1658,8 @@
         <v>1</v>
       </c>
       <c r="L15" s="19">
-        <f>-J43/1000</f>
-        <v>-0.95252248806000039</v>
+        <f>-L43/1000</f>
+        <v>-1.6097630048214007</v>
       </c>
       <c r="M15" s="18">
         <v>5</v>
@@ -1708,40 +1708,40 @@
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23" t="s">
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="22">
         <v>2018</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="I17" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="23">
+      <c r="J17" s="22">
         <v>1.2</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17" s="22">
         <v>1</v>
       </c>
-      <c r="L17" s="24">
+      <c r="L17" s="23">
         <f>-C43/1000</f>
         <v>-0.15180000000000002</v>
       </c>
-      <c r="M17" s="23">
+      <c r="M17" s="22">
         <v>5</v>
       </c>
-      <c r="N17" s="23" t="s">
+      <c r="N17" s="22" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1764,7 +1764,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="24" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1782,7 +1782,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
@@ -1798,7 +1798,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="3" t="s">
         <v>25</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
@@ -1830,7 +1830,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
@@ -1846,7 +1846,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="3" t="s">
         <v>22</v>
       </c>
@@ -2215,21 +2215,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -2440,24 +2425,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2474,4 +2457,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change Max Growth Rate constraint for EVs from 30% to 20%
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9524487E-C876-4708-8C9F-489642785E77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8351E01-90C8-494C-8DD2-2C3C4B56086E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -1174,7 +1174,7 @@
   <dimension ref="A2:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1309,7 +1309,7 @@
         <v>16</v>
       </c>
       <c r="J6" s="18">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="K6" s="18">
         <v>1</v>
@@ -1347,7 +1347,7 @@
         <v>16</v>
       </c>
       <c r="J7" s="18">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="K7" s="18">
         <v>1</v>
@@ -1423,7 +1423,7 @@
         <v>16</v>
       </c>
       <c r="J9" s="18">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="K9" s="18">
         <v>1</v>
@@ -1461,7 +1461,7 @@
         <v>16</v>
       </c>
       <c r="J10" s="18">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="K10" s="18">
         <v>1</v>
@@ -1537,7 +1537,7 @@
         <v>16</v>
       </c>
       <c r="J12" s="18">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="K12" s="18">
         <v>1</v>
@@ -1575,7 +1575,7 @@
         <v>16</v>
       </c>
       <c r="J13" s="18">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="K13" s="18">
         <v>1</v>
@@ -1651,7 +1651,7 @@
         <v>16</v>
       </c>
       <c r="J15" s="18">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="K15" s="18">
         <v>1</v>
@@ -1689,7 +1689,7 @@
         <v>16</v>
       </c>
       <c r="J16" s="18">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="K16" s="18">
         <v>1</v>
@@ -2120,7 +2120,7 @@
         <v>2150.0700000000002</v>
       </c>
       <c r="E45" s="20">
-        <f t="shared" ref="D45:L45" si="4">D45*(1+$B$40)</f>
+        <f t="shared" ref="E45:L45" si="4">D45*(1+$B$40)</f>
         <v>2795.0910000000003</v>
       </c>
       <c r="F45" s="14">
@@ -2214,21 +2214,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -2439,24 +2424,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2473,4 +2456,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modify seed value for Max Growth Rate Constraint
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8351E01-90C8-494C-8DD2-2C3C4B56086E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1784CD42-3C16-47AF-8B81-C47FBAD21E2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -1173,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,8 +1315,8 @@
         <v>1</v>
       </c>
       <c r="L6" s="19">
-        <f>-J46/1000</f>
-        <v>-152.00326255114004</v>
+        <f>-H46/1000</f>
+        <v>-89.942758906000023</v>
       </c>
       <c r="M6" s="18">
         <v>5</v>
@@ -1353,8 +1353,8 @@
         <v>1</v>
       </c>
       <c r="L7" s="19">
-        <f>-J46/1000</f>
-        <v>-152.00326255114004</v>
+        <f>-H46/1000</f>
+        <v>-89.942758906000023</v>
       </c>
       <c r="M7" s="18">
         <v>5</v>
@@ -1429,8 +1429,8 @@
         <v>1</v>
       </c>
       <c r="L9" s="19">
-        <f>-E45/1000</f>
-        <v>-2.7950910000000002</v>
+        <f>-C45/1000</f>
+        <v>-1.6539000000000001</v>
       </c>
       <c r="M9" s="18">
         <v>5</v>
@@ -1467,8 +1467,8 @@
         <v>1</v>
       </c>
       <c r="L10" s="19">
-        <f>-E45/1000</f>
-        <v>-2.7950910000000002</v>
+        <f>-C45/1000</f>
+        <v>-1.6539000000000001</v>
       </c>
       <c r="M10" s="18">
         <v>5</v>
@@ -1505,8 +1505,8 @@
         <v>1</v>
       </c>
       <c r="L11" s="22">
-        <f>-E45/1000</f>
-        <v>-2.7950910000000002</v>
+        <f>-C45/1000</f>
+        <v>-1.6539000000000001</v>
       </c>
       <c r="M11" s="21">
         <v>5</v>
@@ -1543,8 +1543,8 @@
         <v>1</v>
       </c>
       <c r="L12" s="19">
-        <f>-E44/1000</f>
-        <v>-8.9570000000000011E-2</v>
+        <f>-C44/1000</f>
+        <v>-5.2999999999999999E-2</v>
       </c>
       <c r="M12" s="18">
         <v>5</v>
@@ -1581,8 +1581,8 @@
         <v>1</v>
       </c>
       <c r="L13" s="19">
-        <f>-E44/1000</f>
-        <v>-8.9570000000000011E-2</v>
+        <f>-C44/1000</f>
+        <v>-5.2999999999999999E-2</v>
       </c>
       <c r="M13" s="18">
         <v>5</v>
@@ -1619,8 +1619,8 @@
         <v>1</v>
       </c>
       <c r="L14" s="22">
-        <f>-E44/1000</f>
-        <v>-8.9570000000000011E-2</v>
+        <f>-C44/1000</f>
+        <v>-5.2999999999999999E-2</v>
       </c>
       <c r="M14" s="21">
         <v>5</v>
@@ -1657,8 +1657,8 @@
         <v>1</v>
       </c>
       <c r="L15" s="19">
-        <f>-E43/1000</f>
-        <v>-0.25654200000000005</v>
+        <f>-C43/1000</f>
+        <v>-0.15180000000000002</v>
       </c>
       <c r="M15" s="18">
         <v>5</v>
@@ -1695,8 +1695,8 @@
         <v>1</v>
       </c>
       <c r="L16" s="19">
-        <f>-E43/1000</f>
-        <v>-0.25654200000000005</v>
+        <f>-C43/1000</f>
+        <v>-0.15180000000000002</v>
       </c>
       <c r="M16" s="18">
         <v>5</v>
@@ -1734,8 +1734,8 @@
         <v>1</v>
       </c>
       <c r="L17" s="22">
-        <f>-E43/1000</f>
-        <v>-0.25654200000000005</v>
+        <f>-C43/1000</f>
+        <v>-0.15180000000000002</v>
       </c>
       <c r="M17" s="21">
         <v>5</v>
@@ -2214,6 +2214,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -2424,22 +2439,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2456,21 +2473,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TRA: apply growth constraint only to the regions with transport demand; close #118
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -1,20 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1784CD42-3C16-47AF-8B81-C47FBAD21E2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53C8F5B-7107-4AB0-A020-D181E9B02275}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Regions" sheetId="2" r:id="rId1"/>
+    <sheet name="UC_Growth" sheetId="1" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
+    <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
+    <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,11 +48,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
-  <si>
-    <t>~UC_Sets: R_E: AllRegions</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="136">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -265,6 +299,206 @@
   </si>
   <si>
     <t>UC-LGT_MaxGrowthFCV</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>*National</t>
+  </si>
+  <si>
+    <t>Single-region</t>
+  </si>
+  <si>
+    <t>Multi-region</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>County name</t>
+  </si>
+  <si>
+    <t>IE-CW</t>
+  </si>
+  <si>
+    <t>Carlow</t>
+  </si>
+  <si>
+    <t>IE-CN</t>
+  </si>
+  <si>
+    <t>Cavan</t>
+  </si>
+  <si>
+    <t>IE-CE</t>
+  </si>
+  <si>
+    <t>Clare</t>
+  </si>
+  <si>
+    <t>IE-CO</t>
+  </si>
+  <si>
+    <t>Cork</t>
+  </si>
+  <si>
+    <t>IE-DL</t>
+  </si>
+  <si>
+    <t>Donegal</t>
+  </si>
+  <si>
+    <t>IE-D</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>IE-G</t>
+  </si>
+  <si>
+    <t>Galway</t>
+  </si>
+  <si>
+    <t>IE-KY</t>
+  </si>
+  <si>
+    <t>Kerry</t>
+  </si>
+  <si>
+    <t>IE-KE</t>
+  </si>
+  <si>
+    <t>Kildare</t>
+  </si>
+  <si>
+    <t>IE-KK</t>
+  </si>
+  <si>
+    <t>Kilkenny</t>
+  </si>
+  <si>
+    <t>IE-LS</t>
+  </si>
+  <si>
+    <t>Laois</t>
+  </si>
+  <si>
+    <t>IE-LM</t>
+  </si>
+  <si>
+    <t>Leitrim</t>
+  </si>
+  <si>
+    <t>IE-LK</t>
+  </si>
+  <si>
+    <t>Limerick</t>
+  </si>
+  <si>
+    <t>IE-LD</t>
+  </si>
+  <si>
+    <t>Longford</t>
+  </si>
+  <si>
+    <t>IE-LH</t>
+  </si>
+  <si>
+    <t>Louth</t>
+  </si>
+  <si>
+    <t>IE-MO</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>IE-MH</t>
+  </si>
+  <si>
+    <t>Meath</t>
+  </si>
+  <si>
+    <t>IE-MN</t>
+  </si>
+  <si>
+    <t>Monaghan</t>
+  </si>
+  <si>
+    <t>IE-OY</t>
+  </si>
+  <si>
+    <t>Offaly</t>
+  </si>
+  <si>
+    <t>IE-RN</t>
+  </si>
+  <si>
+    <t>Roscommon</t>
+  </si>
+  <si>
+    <t>IE-SO</t>
+  </si>
+  <si>
+    <t>Sligo</t>
+  </si>
+  <si>
+    <t>IE-TA</t>
+  </si>
+  <si>
+    <t>Tipperary</t>
+  </si>
+  <si>
+    <t>IE-WD</t>
+  </si>
+  <si>
+    <t>Waterford</t>
+  </si>
+  <si>
+    <t>IE-WH</t>
+  </si>
+  <si>
+    <t>Westmeath</t>
+  </si>
+  <si>
+    <t>IE-WX</t>
+  </si>
+  <si>
+    <t>Wexford</t>
+  </si>
+  <si>
+    <t>IE-WW</t>
+  </si>
+  <si>
+    <t>Wicklow</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://en.wikipedia.org/wiki/ISO_3166-2:IE</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -272,9 +506,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -343,7 +577,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,8 +608,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -392,227 +638,277 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -621,8 +917,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -630,17 +926,28 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="217">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -872,6 +1179,96 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="39" fmlaLink="$A$4" fmlaRange="$A$5:$A$7" noThreeD="1" sel="1" val="0"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Drop Down 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AADFBB5-A5E4-4977-8F4D-421FF25333EB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Regions"/>
+      <sheetName val="EB2018"/>
+      <sheetName val="FT_Single"/>
+      <sheetName val="FT_Multi"/>
+      <sheetName val="Setup"/>
+      <sheetName val="Conversions"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1170,31 +1567,796 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E206C345-0D8E-4CDB-A3D4-9EEBCC27251E}">
+  <dimension ref="A3:AD37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C3" s="24" t="str" cm="1">
+        <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
+        <v>IE</v>
+      </c>
+      <c r="D3" s="24" t="str" cm="1">
+        <f t="array" ref="D3">IF(LEFT(INDEX(D5:D7,$A$4),1)&lt;&gt;"*",INDEX(D5:D7,$A$4),"")</f>
+        <v/>
+      </c>
+      <c r="E3" s="24" t="str" cm="1">
+        <f t="array" ref="E3">IF(LEFT(INDEX(E5:E7,$A$4),1)&lt;&gt;"*",INDEX(E5:E7,$A$4),"")</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F3" s="24" t="str" cm="1">
+        <f t="array" ref="F3">IF(LEFT(INDEX(F5:F7,$A$4),1)&lt;&gt;"*",INDEX(F5:F7,$A$4),"")</f>
+        <v>IE-D</v>
+      </c>
+      <c r="G3" s="24" t="str" cm="1">
+        <f t="array" ref="G3">IF(LEFT(INDEX(G5:G7,$A$4),1)&lt;&gt;"*",INDEX(G5:G7,$A$4),"")</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="H3" s="24" t="str" cm="1">
+        <f t="array" ref="H3">IF(LEFT(INDEX(H5:H7,$A$4),1)&lt;&gt;"*",INDEX(H5:H7,$A$4),"")</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="I3" s="24" t="str" cm="1">
+        <f t="array" ref="I3">IF(LEFT(INDEX(I5:I7,$A$4),1)&lt;&gt;"*",INDEX(I5:I7,$A$4),"")</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="J3" s="24" t="str" cm="1">
+        <f t="array" ref="J3">IF(LEFT(INDEX(J5:J7,$A$4),1)&lt;&gt;"*",INDEX(J5:J7,$A$4),"")</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="K3" s="24" t="str" cm="1">
+        <f t="array" ref="K3">IF(LEFT(INDEX(K5:K7,$A$4),1)&lt;&gt;"*",INDEX(K5:K7,$A$4),"")</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="L3" s="24" t="str" cm="1">
+        <f t="array" ref="L3">IF(LEFT(INDEX(L5:L7,$A$4),1)&lt;&gt;"*",INDEX(L5:L7,$A$4),"")</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="M3" s="24" t="str" cm="1">
+        <f t="array" ref="M3">IF(LEFT(INDEX(M5:M7,$A$4),1)&lt;&gt;"*",INDEX(M5:M7,$A$4),"")</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="N3" s="24" t="str" cm="1">
+        <f t="array" ref="N3">IF(LEFT(INDEX(N5:N7,$A$4),1)&lt;&gt;"*",INDEX(N5:N7,$A$4),"")</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="O3" s="24" t="str" cm="1">
+        <f t="array" ref="O3">IF(LEFT(INDEX(O5:O7,$A$4),1)&lt;&gt;"*",INDEX(O5:O7,$A$4),"")</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="P3" s="24" t="str" cm="1">
+        <f t="array" ref="P3">IF(LEFT(INDEX(P5:P7,$A$4),1)&lt;&gt;"*",INDEX(P5:P7,$A$4),"")</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q3" s="24" t="str" cm="1">
+        <f t="array" ref="Q3">IF(LEFT(INDEX(Q5:Q7,$A$4),1)&lt;&gt;"*",INDEX(Q5:Q7,$A$4),"")</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="R3" s="24" t="str" cm="1">
+        <f t="array" ref="R3">IF(LEFT(INDEX(R5:R7,$A$4),1)&lt;&gt;"*",INDEX(R5:R7,$A$4),"")</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="S3" s="24" t="str" cm="1">
+        <f t="array" ref="S3">IF(LEFT(INDEX(S5:S7,$A$4),1)&lt;&gt;"*",INDEX(S5:S7,$A$4),"")</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="T3" s="24" t="str" cm="1">
+        <f t="array" ref="T3">IF(LEFT(INDEX(T5:T7,$A$4),1)&lt;&gt;"*",INDEX(T5:T7,$A$4),"")</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="U3" s="24" t="str" cm="1">
+        <f t="array" ref="U3">IF(LEFT(INDEX(U5:U7,$A$4),1)&lt;&gt;"*",INDEX(U5:U7,$A$4),"")</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="V3" s="24" t="str" cm="1">
+        <f t="array" ref="V3">IF(LEFT(INDEX(V5:V7,$A$4),1)&lt;&gt;"*",INDEX(V5:V7,$A$4),"")</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="W3" s="24" t="str" cm="1">
+        <f t="array" ref="W3">IF(LEFT(INDEX(W5:W7,$A$4),1)&lt;&gt;"*",INDEX(W5:W7,$A$4),"")</f>
+        <v>IE-G</v>
+      </c>
+      <c r="X3" s="24" t="str" cm="1">
+        <f t="array" ref="X3">IF(LEFT(INDEX(X5:X7,$A$4),1)&lt;&gt;"*",INDEX(X5:X7,$A$4),"")</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y3" s="24" t="str" cm="1">
+        <f t="array" ref="Y3">IF(LEFT(INDEX(Y5:Y7,$A$4),1)&lt;&gt;"*",INDEX(Y5:Y7,$A$4),"")</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z3" s="24" t="str" cm="1">
+        <f t="array" ref="Z3">IF(LEFT(INDEX(Z5:Z7,$A$4),1)&lt;&gt;"*",INDEX(Z5:Z7,$A$4),"")</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA3" s="24" t="str" cm="1">
+        <f t="array" ref="AA3">IF(LEFT(INDEX(AA5:AA7,$A$4),1)&lt;&gt;"*",INDEX(AA5:AA7,$A$4),"")</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB3" s="24" t="str" cm="1">
+        <f t="array" ref="AB3">IF(LEFT(INDEX(AB5:AB7,$A$4),1)&lt;&gt;"*",INDEX(AB5:AB7,$A$4),"")</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC3" s="24" t="str" cm="1">
+        <f t="array" ref="AC3">IF(LEFT(INDEX(AC5:AC7,$A$4),1)&lt;&gt;"*",INDEX(AC5:AC7,$A$4),"")</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD3" s="24" t="str" cm="1">
+        <f t="array" ref="AD3">IF(LEFT(INDEX(AD5:AD7,$A$4),1)&lt;&gt;"*",INDEX(AD5:AD7,$A$4),"")</f>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="24" t="str">
+        <f>Regions!A11</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F5" s="24" t="str">
+        <f>Regions!A16</f>
+        <v>IE-D</v>
+      </c>
+      <c r="G5" s="24" t="str">
+        <f>Regions!A19</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="H5" s="24" t="str">
+        <f>Regions!A20</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="I5" s="24" t="str">
+        <f>Regions!A21</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="J5" s="24" t="str">
+        <f>Regions!A24</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="K5" s="24" t="str">
+        <f>Regions!A25</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="L5" s="24" t="str">
+        <f>Regions!A27</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="M5" s="24" t="str">
+        <f>Regions!A29</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="N5" s="24" t="str">
+        <f>Regions!A34</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="O5" s="24" t="str">
+        <f>Regions!A35</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="P5" s="24" t="str">
+        <f>Regions!A36</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q5" s="24" t="str">
+        <f>Regions!A13</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="R5" s="24" t="str">
+        <f>Regions!A14</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="S5" s="24" t="str">
+        <f>Regions!A18</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="T5" s="24" t="str">
+        <f>Regions!A23</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="U5" s="24" t="str">
+        <f>Regions!A32</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="V5" s="24" t="str">
+        <f>Regions!A33</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="W5" s="24" t="str">
+        <f>Regions!A17</f>
+        <v>IE-G</v>
+      </c>
+      <c r="X5" s="24" t="str">
+        <f>Regions!A22</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y5" s="24" t="str">
+        <f>Regions!A26</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z5" s="24" t="str">
+        <f>Regions!A30</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA5" s="24" t="str">
+        <f>Regions!A31</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB5" s="24" t="str">
+        <f>Regions!A12</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC5" s="24" t="str">
+        <f>Regions!A15</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD5" s="24" t="str">
+        <f>Regions!A28</f>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="24" t="str">
+        <f>C5</f>
+        <v>IE</v>
+      </c>
+      <c r="D6" s="24" t="str">
+        <f>IF(LEFT(D5,1)&lt;&gt;"*","*"&amp;D5,D5)</f>
+        <v>*National</v>
+      </c>
+      <c r="E6" s="24" t="str">
+        <f t="shared" ref="E6:AD6" si="0">IF(LEFT(E5,1)&lt;&gt;"*","*"&amp;E5,E5)</f>
+        <v>*IE-CW</v>
+      </c>
+      <c r="F6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-D</v>
+      </c>
+      <c r="G6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-KE</v>
+      </c>
+      <c r="H6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-KK</v>
+      </c>
+      <c r="I6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LS</v>
+      </c>
+      <c r="J6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LD</v>
+      </c>
+      <c r="K6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LH</v>
+      </c>
+      <c r="L6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-MH</v>
+      </c>
+      <c r="M6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-OY</v>
+      </c>
+      <c r="N6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WH</v>
+      </c>
+      <c r="O6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WX</v>
+      </c>
+      <c r="P6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WW</v>
+      </c>
+      <c r="Q6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-CE</v>
+      </c>
+      <c r="R6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-CO</v>
+      </c>
+      <c r="S6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-KY</v>
+      </c>
+      <c r="T6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LK</v>
+      </c>
+      <c r="U6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-TA</v>
+      </c>
+      <c r="V6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WD</v>
+      </c>
+      <c r="W6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-G</v>
+      </c>
+      <c r="X6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LM</v>
+      </c>
+      <c r="Y6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-MO</v>
+      </c>
+      <c r="Z6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-RN</v>
+      </c>
+      <c r="AA6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-SO</v>
+      </c>
+      <c r="AB6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-CN</v>
+      </c>
+      <c r="AC6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-DL</v>
+      </c>
+      <c r="AD6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-MN</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="24" t="str">
+        <f>"*"&amp;C5</f>
+        <v>*IE</v>
+      </c>
+      <c r="D7" s="24" t="str">
+        <f>D5</f>
+        <v>*National</v>
+      </c>
+      <c r="E7" s="24" t="str">
+        <f t="shared" ref="E7:AD7" si="1">E5</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-D</v>
+      </c>
+      <c r="G7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-KE</v>
+      </c>
+      <c r="H7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-KK</v>
+      </c>
+      <c r="I7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LS</v>
+      </c>
+      <c r="J7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LD</v>
+      </c>
+      <c r="K7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LH</v>
+      </c>
+      <c r="L7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-MH</v>
+      </c>
+      <c r="M7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-OY</v>
+      </c>
+      <c r="N7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WH</v>
+      </c>
+      <c r="O7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WX</v>
+      </c>
+      <c r="P7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-CE</v>
+      </c>
+      <c r="R7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-CO</v>
+      </c>
+      <c r="S7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-KY</v>
+      </c>
+      <c r="T7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LK</v>
+      </c>
+      <c r="U7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-TA</v>
+      </c>
+      <c r="V7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WD</v>
+      </c>
+      <c r="W7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-G</v>
+      </c>
+      <c r="X7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId3" name="Drop Down 1">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>38100</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <dimension ref="A2:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" customWidth="1"/>
-    <col min="14" max="14" width="33.109375" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="14" max="14" width="33.140625" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:AD3)</f>
+        <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1210,9 +2372,9 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1228,7 +2390,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1237,7 +2399,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -1246,67 +2408,67 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="G5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="H5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="I5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="J5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="5" t="s">
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="18">
         <v>2018</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" s="18">
         <v>1.2</v>
@@ -1322,29 +2484,29 @@
         <v>5</v>
       </c>
       <c r="N6" s="18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>15</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
       <c r="G7" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H7" s="18">
         <v>2018</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="18">
         <v>1.2</v>
@@ -1360,29 +2522,29 @@
         <v>5</v>
       </c>
       <c r="N7" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>15</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H8" s="21">
         <v>2018</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" s="21">
         <v>1.2</v>
@@ -1398,29 +2560,29 @@
         <v>5</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>15</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H9" s="18">
         <v>2018</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" s="18">
         <v>1.2</v>
@@ -1436,29 +2598,29 @@
         <v>5</v>
       </c>
       <c r="N9" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>15</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H10" s="18">
         <v>2018</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J10" s="18">
         <v>1.2</v>
@@ -1474,29 +2636,29 @@
         <v>5</v>
       </c>
       <c r="N10" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>14</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>15</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H11" s="21">
         <v>2018</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J11" s="21">
         <v>1.2</v>
@@ -1512,29 +2674,29 @@
         <v>5</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>15</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12" s="18">
         <v>2018</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J12" s="18">
         <v>1.2</v>
@@ -1550,29 +2712,29 @@
         <v>5</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>15</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H13" s="18">
         <v>2018</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J13" s="18">
         <v>1.2</v>
@@ -1588,29 +2750,29 @@
         <v>5</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>14</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>15</v>
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H14" s="21">
         <v>2018</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J14" s="21">
         <v>1.2</v>
@@ -1626,29 +2788,29 @@
         <v>5</v>
       </c>
       <c r="N14" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>15</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H15" s="18">
         <v>2018</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J15" s="18">
         <v>1.2</v>
@@ -1664,29 +2826,29 @@
         <v>5</v>
       </c>
       <c r="N15" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>14</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>15</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H16" s="18">
         <v>2018</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J16" s="18">
         <v>1.2</v>
@@ -1702,30 +2864,30 @@
         <v>5</v>
       </c>
       <c r="N16" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>14</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>15</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
       <c r="G17" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H17" s="21">
         <v>2018</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J17" s="21">
         <v>1.2</v>
@@ -1741,33 +2903,33 @@
         <v>5</v>
       </c>
       <c r="N17" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="8">
         <v>228046</v>
@@ -1780,10 +2942,10 @@
         <v>4.3671013742841359E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="8">
         <v>100649</v>
@@ -1796,10 +2958,10 @@
         <v>6.5375711631511485E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="8">
         <v>4546</v>
@@ -1812,10 +2974,10 @@
         <v>4.4214694236691596E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="8">
         <v>6661</v>
@@ -1828,10 +2990,10 @@
         <v>4.9391983185707852E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="8">
         <v>8424</v>
@@ -1844,10 +3006,10 @@
         <v>5.7573599240265907E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="8">
         <v>14373</v>
@@ -1860,9 +3022,9 @@
         <v>7.187086899046824E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29" s="8">
         <v>2168099</v>
@@ -1875,9 +3037,9 @@
         <v>5.5865068892149296E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="8">
         <v>41471</v>
@@ -1890,9 +3052,9 @@
         <v>6.1874562947601935E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="8">
         <v>21457</v>
@@ -1905,10 +3067,10 @@
         <v>5.7044321200540614E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" s="9">
         <v>11206</v>
@@ -1921,22 +3083,22 @@
         <v>4.9170087453150095E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B40" s="13">
         <v>0.3</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>2018</v>
       </c>
@@ -1968,9 +3130,9 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2003,9 +3165,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B43" s="15">
         <f>D28+D27</f>
@@ -2053,9 +3215,9 @@
       </c>
       <c r="M43" s="14"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="15">
         <f>D26+D25</f>
@@ -2103,9 +3265,9 @@
       </c>
       <c r="M44" s="14"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="15">
         <f>D24+D23</f>
@@ -2153,9 +3315,9 @@
       </c>
       <c r="M45" s="14"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="15">
         <f>D29</f>
@@ -2214,21 +3376,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -2439,24 +3586,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2473,4 +3618,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modify growth rate for new BEVs and add growth rate for NG fueled MGTs and HGTs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -5,20 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53C8F5B-7107-4AB0-A020-D181E9B02275}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A4E627-0154-4378-94C9-296A6B03B3E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
     <sheet name="UC_Growth" sheetId="1" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
@@ -71,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="148">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -500,15 +497,51 @@
       <t>https://en.wikipedia.org/wiki/ISO_3166-2:IE</t>
     </r>
   </si>
+  <si>
+    <t>UC-HGT_MaxGrowthNGICE</t>
+  </si>
+  <si>
+    <t>UC-MGT-MaxGrowthNGICE</t>
+  </si>
+  <si>
+    <t>T-MGT-ICE_NG*</t>
+  </si>
+  <si>
+    <t>MGT-Maximum growth rate of NG-ICEs</t>
+  </si>
+  <si>
+    <t>HGT-Maximum growth rate of NG-ICEs</t>
+  </si>
+  <si>
+    <t>T-HGT-ICE-NG*</t>
+  </si>
+  <si>
+    <t>UC-HGT_MaxGrowthLNGICE</t>
+  </si>
+  <si>
+    <t>T-HGT-ICE-LNG*</t>
+  </si>
+  <si>
+    <t>HGT-Maximum growth rate of LNG-ICEs</t>
+  </si>
+  <si>
+    <t>UC-MGT-MaxGrowthLNGICE</t>
+  </si>
+  <si>
+    <t>T-MGT-ICE_LNG*</t>
+  </si>
+  <si>
+    <t>MGT-Maximum growth rate of LNG-ICEs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -691,219 +724,219 @@
   </borders>
   <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -917,8 +950,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -926,17 +959,14 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -948,6 +978,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="217">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -1210,7 +1243,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AADFBB5-A5E4-4977-8F4D-421FF25333EB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1246,29 +1279,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Regions"/>
-      <sheetName val="EB2018"/>
-      <sheetName val="FT_Single"/>
-      <sheetName val="FT_Multi"/>
-      <sheetName val="Setup"/>
-      <sheetName val="Conversions"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1574,724 +1584,724 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="C3" s="24" t="str" cm="1">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C3" s="23" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
       </c>
-      <c r="D3" s="24" t="str" cm="1">
+      <c r="D3" s="23" t="str" cm="1">
         <f t="array" ref="D3">IF(LEFT(INDEX(D5:D7,$A$4),1)&lt;&gt;"*",INDEX(D5:D7,$A$4),"")</f>
         <v/>
       </c>
-      <c r="E3" s="24" t="str" cm="1">
+      <c r="E3" s="23" t="str" cm="1">
         <f t="array" ref="E3">IF(LEFT(INDEX(E5:E7,$A$4),1)&lt;&gt;"*",INDEX(E5:E7,$A$4),"")</f>
         <v>IE-CW</v>
       </c>
-      <c r="F3" s="24" t="str" cm="1">
+      <c r="F3" s="23" t="str" cm="1">
         <f t="array" ref="F3">IF(LEFT(INDEX(F5:F7,$A$4),1)&lt;&gt;"*",INDEX(F5:F7,$A$4),"")</f>
         <v>IE-D</v>
       </c>
-      <c r="G3" s="24" t="str" cm="1">
+      <c r="G3" s="23" t="str" cm="1">
         <f t="array" ref="G3">IF(LEFT(INDEX(G5:G7,$A$4),1)&lt;&gt;"*",INDEX(G5:G7,$A$4),"")</f>
         <v>IE-KE</v>
       </c>
-      <c r="H3" s="24" t="str" cm="1">
+      <c r="H3" s="23" t="str" cm="1">
         <f t="array" ref="H3">IF(LEFT(INDEX(H5:H7,$A$4),1)&lt;&gt;"*",INDEX(H5:H7,$A$4),"")</f>
         <v>IE-KK</v>
       </c>
-      <c r="I3" s="24" t="str" cm="1">
+      <c r="I3" s="23" t="str" cm="1">
         <f t="array" ref="I3">IF(LEFT(INDEX(I5:I7,$A$4),1)&lt;&gt;"*",INDEX(I5:I7,$A$4),"")</f>
         <v>IE-LS</v>
       </c>
-      <c r="J3" s="24" t="str" cm="1">
+      <c r="J3" s="23" t="str" cm="1">
         <f t="array" ref="J3">IF(LEFT(INDEX(J5:J7,$A$4),1)&lt;&gt;"*",INDEX(J5:J7,$A$4),"")</f>
         <v>IE-LD</v>
       </c>
-      <c r="K3" s="24" t="str" cm="1">
+      <c r="K3" s="23" t="str" cm="1">
         <f t="array" ref="K3">IF(LEFT(INDEX(K5:K7,$A$4),1)&lt;&gt;"*",INDEX(K5:K7,$A$4),"")</f>
         <v>IE-LH</v>
       </c>
-      <c r="L3" s="24" t="str" cm="1">
+      <c r="L3" s="23" t="str" cm="1">
         <f t="array" ref="L3">IF(LEFT(INDEX(L5:L7,$A$4),1)&lt;&gt;"*",INDEX(L5:L7,$A$4),"")</f>
         <v>IE-MH</v>
       </c>
-      <c r="M3" s="24" t="str" cm="1">
+      <c r="M3" s="23" t="str" cm="1">
         <f t="array" ref="M3">IF(LEFT(INDEX(M5:M7,$A$4),1)&lt;&gt;"*",INDEX(M5:M7,$A$4),"")</f>
         <v>IE-OY</v>
       </c>
-      <c r="N3" s="24" t="str" cm="1">
+      <c r="N3" s="23" t="str" cm="1">
         <f t="array" ref="N3">IF(LEFT(INDEX(N5:N7,$A$4),1)&lt;&gt;"*",INDEX(N5:N7,$A$4),"")</f>
         <v>IE-WH</v>
       </c>
-      <c r="O3" s="24" t="str" cm="1">
+      <c r="O3" s="23" t="str" cm="1">
         <f t="array" ref="O3">IF(LEFT(INDEX(O5:O7,$A$4),1)&lt;&gt;"*",INDEX(O5:O7,$A$4),"")</f>
         <v>IE-WX</v>
       </c>
-      <c r="P3" s="24" t="str" cm="1">
+      <c r="P3" s="23" t="str" cm="1">
         <f t="array" ref="P3">IF(LEFT(INDEX(P5:P7,$A$4),1)&lt;&gt;"*",INDEX(P5:P7,$A$4),"")</f>
         <v>IE-WW</v>
       </c>
-      <c r="Q3" s="24" t="str" cm="1">
+      <c r="Q3" s="23" t="str" cm="1">
         <f t="array" ref="Q3">IF(LEFT(INDEX(Q5:Q7,$A$4),1)&lt;&gt;"*",INDEX(Q5:Q7,$A$4),"")</f>
         <v>IE-CE</v>
       </c>
-      <c r="R3" s="24" t="str" cm="1">
+      <c r="R3" s="23" t="str" cm="1">
         <f t="array" ref="R3">IF(LEFT(INDEX(R5:R7,$A$4),1)&lt;&gt;"*",INDEX(R5:R7,$A$4),"")</f>
         <v>IE-CO</v>
       </c>
-      <c r="S3" s="24" t="str" cm="1">
+      <c r="S3" s="23" t="str" cm="1">
         <f t="array" ref="S3">IF(LEFT(INDEX(S5:S7,$A$4),1)&lt;&gt;"*",INDEX(S5:S7,$A$4),"")</f>
         <v>IE-KY</v>
       </c>
-      <c r="T3" s="24" t="str" cm="1">
+      <c r="T3" s="23" t="str" cm="1">
         <f t="array" ref="T3">IF(LEFT(INDEX(T5:T7,$A$4),1)&lt;&gt;"*",INDEX(T5:T7,$A$4),"")</f>
         <v>IE-LK</v>
       </c>
-      <c r="U3" s="24" t="str" cm="1">
+      <c r="U3" s="23" t="str" cm="1">
         <f t="array" ref="U3">IF(LEFT(INDEX(U5:U7,$A$4),1)&lt;&gt;"*",INDEX(U5:U7,$A$4),"")</f>
         <v>IE-TA</v>
       </c>
-      <c r="V3" s="24" t="str" cm="1">
+      <c r="V3" s="23" t="str" cm="1">
         <f t="array" ref="V3">IF(LEFT(INDEX(V5:V7,$A$4),1)&lt;&gt;"*",INDEX(V5:V7,$A$4),"")</f>
         <v>IE-WD</v>
       </c>
-      <c r="W3" s="24" t="str" cm="1">
+      <c r="W3" s="23" t="str" cm="1">
         <f t="array" ref="W3">IF(LEFT(INDEX(W5:W7,$A$4),1)&lt;&gt;"*",INDEX(W5:W7,$A$4),"")</f>
         <v>IE-G</v>
       </c>
-      <c r="X3" s="24" t="str" cm="1">
+      <c r="X3" s="23" t="str" cm="1">
         <f t="array" ref="X3">IF(LEFT(INDEX(X5:X7,$A$4),1)&lt;&gt;"*",INDEX(X5:X7,$A$4),"")</f>
         <v>IE-LM</v>
       </c>
-      <c r="Y3" s="24" t="str" cm="1">
+      <c r="Y3" s="23" t="str" cm="1">
         <f t="array" ref="Y3">IF(LEFT(INDEX(Y5:Y7,$A$4),1)&lt;&gt;"*",INDEX(Y5:Y7,$A$4),"")</f>
         <v>IE-MO</v>
       </c>
-      <c r="Z3" s="24" t="str" cm="1">
+      <c r="Z3" s="23" t="str" cm="1">
         <f t="array" ref="Z3">IF(LEFT(INDEX(Z5:Z7,$A$4),1)&lt;&gt;"*",INDEX(Z5:Z7,$A$4),"")</f>
         <v>IE-RN</v>
       </c>
-      <c r="AA3" s="24" t="str" cm="1">
+      <c r="AA3" s="23" t="str" cm="1">
         <f t="array" ref="AA3">IF(LEFT(INDEX(AA5:AA7,$A$4),1)&lt;&gt;"*",INDEX(AA5:AA7,$A$4),"")</f>
         <v>IE-SO</v>
       </c>
-      <c r="AB3" s="24" t="str" cm="1">
+      <c r="AB3" s="23" t="str" cm="1">
         <f t="array" ref="AB3">IF(LEFT(INDEX(AB5:AB7,$A$4),1)&lt;&gt;"*",INDEX(AB5:AB7,$A$4),"")</f>
         <v>IE-CN</v>
       </c>
-      <c r="AC3" s="24" t="str" cm="1">
+      <c r="AC3" s="23" t="str" cm="1">
         <f t="array" ref="AC3">IF(LEFT(INDEX(AC5:AC7,$A$4),1)&lt;&gt;"*",INDEX(AC5:AC7,$A$4),"")</f>
         <v>IE-DL</v>
       </c>
-      <c r="AD3" s="24" t="str" cm="1">
+      <c r="AD3" s="23" t="str" cm="1">
         <f t="array" ref="AD3">IF(LEFT(INDEX(AD5:AD7,$A$4),1)&lt;&gt;"*",INDEX(AD5:AD7,$A$4),"")</f>
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="24" t="str">
+      <c r="E5" s="23" t="str">
         <f>Regions!A11</f>
         <v>IE-CW</v>
       </c>
-      <c r="F5" s="24" t="str">
+      <c r="F5" s="23" t="str">
         <f>Regions!A16</f>
         <v>IE-D</v>
       </c>
-      <c r="G5" s="24" t="str">
+      <c r="G5" s="23" t="str">
         <f>Regions!A19</f>
         <v>IE-KE</v>
       </c>
-      <c r="H5" s="24" t="str">
+      <c r="H5" s="23" t="str">
         <f>Regions!A20</f>
         <v>IE-KK</v>
       </c>
-      <c r="I5" s="24" t="str">
+      <c r="I5" s="23" t="str">
         <f>Regions!A21</f>
         <v>IE-LS</v>
       </c>
-      <c r="J5" s="24" t="str">
+      <c r="J5" s="23" t="str">
         <f>Regions!A24</f>
         <v>IE-LD</v>
       </c>
-      <c r="K5" s="24" t="str">
+      <c r="K5" s="23" t="str">
         <f>Regions!A25</f>
         <v>IE-LH</v>
       </c>
-      <c r="L5" s="24" t="str">
+      <c r="L5" s="23" t="str">
         <f>Regions!A27</f>
         <v>IE-MH</v>
       </c>
-      <c r="M5" s="24" t="str">
+      <c r="M5" s="23" t="str">
         <f>Regions!A29</f>
         <v>IE-OY</v>
       </c>
-      <c r="N5" s="24" t="str">
+      <c r="N5" s="23" t="str">
         <f>Regions!A34</f>
         <v>IE-WH</v>
       </c>
-      <c r="O5" s="24" t="str">
+      <c r="O5" s="23" t="str">
         <f>Regions!A35</f>
         <v>IE-WX</v>
       </c>
-      <c r="P5" s="24" t="str">
+      <c r="P5" s="23" t="str">
         <f>Regions!A36</f>
         <v>IE-WW</v>
       </c>
-      <c r="Q5" s="24" t="str">
+      <c r="Q5" s="23" t="str">
         <f>Regions!A13</f>
         <v>IE-CE</v>
       </c>
-      <c r="R5" s="24" t="str">
+      <c r="R5" s="23" t="str">
         <f>Regions!A14</f>
         <v>IE-CO</v>
       </c>
-      <c r="S5" s="24" t="str">
+      <c r="S5" s="23" t="str">
         <f>Regions!A18</f>
         <v>IE-KY</v>
       </c>
-      <c r="T5" s="24" t="str">
+      <c r="T5" s="23" t="str">
         <f>Regions!A23</f>
         <v>IE-LK</v>
       </c>
-      <c r="U5" s="24" t="str">
+      <c r="U5" s="23" t="str">
         <f>Regions!A32</f>
         <v>IE-TA</v>
       </c>
-      <c r="V5" s="24" t="str">
+      <c r="V5" s="23" t="str">
         <f>Regions!A33</f>
         <v>IE-WD</v>
       </c>
-      <c r="W5" s="24" t="str">
+      <c r="W5" s="23" t="str">
         <f>Regions!A17</f>
         <v>IE-G</v>
       </c>
-      <c r="X5" s="24" t="str">
+      <c r="X5" s="23" t="str">
         <f>Regions!A22</f>
         <v>IE-LM</v>
       </c>
-      <c r="Y5" s="24" t="str">
+      <c r="Y5" s="23" t="str">
         <f>Regions!A26</f>
         <v>IE-MO</v>
       </c>
-      <c r="Z5" s="24" t="str">
+      <c r="Z5" s="23" t="str">
         <f>Regions!A30</f>
         <v>IE-RN</v>
       </c>
-      <c r="AA5" s="24" t="str">
+      <c r="AA5" s="23" t="str">
         <f>Regions!A31</f>
         <v>IE-SO</v>
       </c>
-      <c r="AB5" s="24" t="str">
+      <c r="AB5" s="23" t="str">
         <f>Regions!A12</f>
         <v>IE-CN</v>
       </c>
-      <c r="AC5" s="24" t="str">
+      <c r="AC5" s="23" t="str">
         <f>Regions!A15</f>
         <v>IE-DL</v>
       </c>
-      <c r="AD5" s="24" t="str">
+      <c r="AD5" s="23" t="str">
         <f>Regions!A28</f>
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="24" t="str">
+      <c r="C6" s="23" t="str">
         <f>C5</f>
         <v>IE</v>
       </c>
-      <c r="D6" s="24" t="str">
+      <c r="D6" s="23" t="str">
         <f>IF(LEFT(D5,1)&lt;&gt;"*","*"&amp;D5,D5)</f>
         <v>*National</v>
       </c>
-      <c r="E6" s="24" t="str">
+      <c r="E6" s="23" t="str">
         <f t="shared" ref="E6:AD6" si="0">IF(LEFT(E5,1)&lt;&gt;"*","*"&amp;E5,E5)</f>
         <v>*IE-CW</v>
       </c>
-      <c r="F6" s="24" t="str">
+      <c r="F6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-D</v>
       </c>
-      <c r="G6" s="24" t="str">
+      <c r="G6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-KE</v>
       </c>
-      <c r="H6" s="24" t="str">
+      <c r="H6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-KK</v>
       </c>
-      <c r="I6" s="24" t="str">
+      <c r="I6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-LS</v>
       </c>
-      <c r="J6" s="24" t="str">
+      <c r="J6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-LD</v>
       </c>
-      <c r="K6" s="24" t="str">
+      <c r="K6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-LH</v>
       </c>
-      <c r="L6" s="24" t="str">
+      <c r="L6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-MH</v>
       </c>
-      <c r="M6" s="24" t="str">
+      <c r="M6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-OY</v>
       </c>
-      <c r="N6" s="24" t="str">
+      <c r="N6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-WH</v>
       </c>
-      <c r="O6" s="24" t="str">
+      <c r="O6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-WX</v>
       </c>
-      <c r="P6" s="24" t="str">
+      <c r="P6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-WW</v>
       </c>
-      <c r="Q6" s="24" t="str">
+      <c r="Q6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-CE</v>
       </c>
-      <c r="R6" s="24" t="str">
+      <c r="R6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-CO</v>
       </c>
-      <c r="S6" s="24" t="str">
+      <c r="S6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-KY</v>
       </c>
-      <c r="T6" s="24" t="str">
+      <c r="T6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-LK</v>
       </c>
-      <c r="U6" s="24" t="str">
+      <c r="U6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-TA</v>
       </c>
-      <c r="V6" s="24" t="str">
+      <c r="V6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-WD</v>
       </c>
-      <c r="W6" s="24" t="str">
+      <c r="W6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-G</v>
       </c>
-      <c r="X6" s="24" t="str">
+      <c r="X6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-LM</v>
       </c>
-      <c r="Y6" s="24" t="str">
+      <c r="Y6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-MO</v>
       </c>
-      <c r="Z6" s="24" t="str">
+      <c r="Z6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-RN</v>
       </c>
-      <c r="AA6" s="24" t="str">
+      <c r="AA6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-SO</v>
       </c>
-      <c r="AB6" s="24" t="str">
+      <c r="AB6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-CN</v>
       </c>
-      <c r="AC6" s="24" t="str">
+      <c r="AC6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-DL</v>
       </c>
-      <c r="AD6" s="24" t="str">
+      <c r="AD6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="24" t="str">
+      <c r="C7" s="23" t="str">
         <f>"*"&amp;C5</f>
         <v>*IE</v>
       </c>
-      <c r="D7" s="24" t="str">
+      <c r="D7" s="23" t="str">
         <f>D5</f>
         <v>*National</v>
       </c>
-      <c r="E7" s="24" t="str">
+      <c r="E7" s="23" t="str">
         <f t="shared" ref="E7:AD7" si="1">E5</f>
         <v>IE-CW</v>
       </c>
-      <c r="F7" s="24" t="str">
+      <c r="F7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-D</v>
       </c>
-      <c r="G7" s="24" t="str">
+      <c r="G7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-KE</v>
       </c>
-      <c r="H7" s="24" t="str">
+      <c r="H7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-KK</v>
       </c>
-      <c r="I7" s="24" t="str">
+      <c r="I7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-LS</v>
       </c>
-      <c r="J7" s="24" t="str">
+      <c r="J7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-LD</v>
       </c>
-      <c r="K7" s="24" t="str">
+      <c r="K7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-LH</v>
       </c>
-      <c r="L7" s="24" t="str">
+      <c r="L7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-MH</v>
       </c>
-      <c r="M7" s="24" t="str">
+      <c r="M7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-OY</v>
       </c>
-      <c r="N7" s="24" t="str">
+      <c r="N7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-WH</v>
       </c>
-      <c r="O7" s="24" t="str">
+      <c r="O7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-WX</v>
       </c>
-      <c r="P7" s="24" t="str">
+      <c r="P7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-WW</v>
       </c>
-      <c r="Q7" s="24" t="str">
+      <c r="Q7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-CE</v>
       </c>
-      <c r="R7" s="24" t="str">
+      <c r="R7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-CO</v>
       </c>
-      <c r="S7" s="24" t="str">
+      <c r="S7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-KY</v>
       </c>
-      <c r="T7" s="24" t="str">
+      <c r="T7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-LK</v>
       </c>
-      <c r="U7" s="24" t="str">
+      <c r="U7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-TA</v>
       </c>
-      <c r="V7" s="24" t="str">
+      <c r="V7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-WD</v>
       </c>
-      <c r="W7" s="24" t="str">
+      <c r="W7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-G</v>
       </c>
-      <c r="X7" s="24" t="str">
+      <c r="X7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-LM</v>
       </c>
-      <c r="Y7" s="24" t="str">
+      <c r="Y7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-MO</v>
       </c>
-      <c r="Z7" s="24" t="str">
+      <c r="Z7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-RN</v>
       </c>
-      <c r="AA7" s="24" t="str">
+      <c r="AA7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-SO</v>
       </c>
-      <c r="AB7" s="24" t="str">
+      <c r="AB7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-CN</v>
       </c>
-      <c r="AC7" s="24" t="str">
+      <c r="AC7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-DL</v>
       </c>
-      <c r="AD7" s="24" t="str">
+      <c r="AD7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="27" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="27" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="27" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="27" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="27" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="27" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="27" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="27" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="27" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="27" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="27" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="27" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="27" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="27" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="27" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="27" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="27" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="28" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2332,28 +2342,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
-  <dimension ref="A2:O46"/>
+  <dimension ref="A2:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="33.140625" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="14" max="14" width="34" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:AD3)</f>
         <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
@@ -2372,7 +2382,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2390,7 +2400,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2408,7 +2418,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -2449,7 +2459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
         <v>57</v>
       </c>
@@ -2477,8 +2487,8 @@
         <v>1</v>
       </c>
       <c r="L6" s="19">
-        <f>-H46/1000</f>
-        <v>-89.942758906000023</v>
+        <f>-C50/1000</f>
+        <v>-24.2242</v>
       </c>
       <c r="M6" s="18">
         <v>5</v>
@@ -2487,7 +2497,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="18" t="s">
         <v>58</v>
       </c>
@@ -2515,8 +2525,8 @@
         <v>1</v>
       </c>
       <c r="L7" s="19">
-        <f>-H46/1000</f>
-        <v>-89.942758906000023</v>
+        <f>-C50/1000</f>
+        <v>-24.2242</v>
       </c>
       <c r="M7" s="18">
         <v>5</v>
@@ -2525,7 +2535,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="21" t="s">
         <v>68</v>
       </c>
@@ -2553,7 +2563,7 @@
         <v>1</v>
       </c>
       <c r="L8" s="22">
-        <f>-C46/1000</f>
+        <f>-C50/1000</f>
         <v>-24.2242</v>
       </c>
       <c r="M8" s="21">
@@ -2563,7 +2573,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>55</v>
       </c>
@@ -2591,7 +2601,7 @@
         <v>1</v>
       </c>
       <c r="L9" s="19">
-        <f>-C45/1000</f>
+        <f>-C49/1000</f>
         <v>-1.6539000000000001</v>
       </c>
       <c r="M9" s="18">
@@ -2601,7 +2611,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>74</v>
       </c>
@@ -2629,7 +2639,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="19">
-        <f>-C45/1000</f>
+        <f>-C49/1000</f>
         <v>-1.6539000000000001</v>
       </c>
       <c r="M10" s="18">
@@ -2639,7 +2649,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="21" t="s">
         <v>75</v>
       </c>
@@ -2667,7 +2677,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="22">
-        <f>-C45/1000</f>
+        <f>-C49/1000</f>
         <v>-1.6539000000000001</v>
       </c>
       <c r="M11" s="21">
@@ -2677,7 +2687,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
         <v>51</v>
       </c>
@@ -2705,7 +2715,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="19">
-        <f>-C44/1000</f>
+        <f>-C48/1000</f>
         <v>-5.2999999999999999E-2</v>
       </c>
       <c r="M12" s="18">
@@ -2715,9 +2725,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>13</v>
@@ -2728,7 +2738,7 @@
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="H13" s="18">
         <v>2018</v>
@@ -2743,57 +2753,57 @@
         <v>1</v>
       </c>
       <c r="L13" s="19">
-        <f>-C44/1000</f>
+        <f>-C48/1000</f>
         <v>-5.2999999999999999E-2</v>
       </c>
       <c r="M13" s="18">
         <v>5</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="21">
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="18">
         <v>2018</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="18">
         <v>1.2</v>
       </c>
-      <c r="K14" s="21">
+      <c r="K14" s="18">
         <v>1</v>
       </c>
-      <c r="L14" s="22">
-        <f>-C44/1000</f>
+      <c r="L14" s="19">
+        <f>-C48/1000</f>
         <v>-5.2999999999999999E-2</v>
       </c>
-      <c r="M14" s="21">
+      <c r="M14" s="18">
         <v>5</v>
       </c>
-      <c r="N14" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>13</v>
@@ -2804,7 +2814,7 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="H15" s="18">
         <v>2018</v>
@@ -2819,555 +2829,707 @@
         <v>1</v>
       </c>
       <c r="L15" s="19">
-        <f>-C43/1000</f>
-        <v>-0.15180000000000002</v>
+        <f>-C48/1000</f>
+        <v>-5.2999999999999999E-2</v>
       </c>
       <c r="M15" s="18">
         <v>5</v>
       </c>
       <c r="N15" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="21">
+        <v>2018</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="K16" s="21">
+        <v>1</v>
+      </c>
+      <c r="L16" s="22">
+        <f>-C48/1000</f>
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="M16" s="21">
+        <v>5</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="18">
+        <v>2018</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="18">
+        <v>1.2</v>
+      </c>
+      <c r="K17" s="18">
+        <v>1</v>
+      </c>
+      <c r="L17" s="19">
+        <f>-C47/1000</f>
+        <v>-0.15180000000000002</v>
+      </c>
+      <c r="M17" s="18">
+        <v>5</v>
+      </c>
+      <c r="N17" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B18" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="H18" s="18">
+        <v>2018</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="18">
+        <v>1.2</v>
+      </c>
+      <c r="K18" s="18">
+        <v>1</v>
+      </c>
+      <c r="L18" s="19">
+        <f>-C47/1000</f>
+        <v>-0.15180000000000002</v>
+      </c>
+      <c r="M18" s="18">
+        <v>5</v>
+      </c>
+      <c r="N18" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B19" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="18">
+        <v>2018</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="18">
+        <v>1.2</v>
+      </c>
+      <c r="K19" s="18">
+        <v>1</v>
+      </c>
+      <c r="L19" s="19">
+        <f>-C47/1000</f>
+        <v>-0.15180000000000002</v>
+      </c>
+      <c r="M19" s="18">
+        <v>5</v>
+      </c>
+      <c r="N19" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C20" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D20" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18" t="s">
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H20" s="18">
         <v>2018</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I20" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J20" s="18">
         <v>1.2</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K20" s="18">
         <v>1</v>
       </c>
-      <c r="L16" s="19">
-        <f>-C43/1000</f>
+      <c r="L20" s="19">
+        <f>-C47/1000</f>
         <v>-0.15180000000000002</v>
       </c>
-      <c r="M16" s="18">
+      <c r="M20" s="18">
         <v>5</v>
       </c>
-      <c r="N16" s="18" t="s">
+      <c r="N20" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B21" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C21" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D21" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21" t="s">
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H21" s="21">
         <v>2018</v>
       </c>
-      <c r="I17" s="21" t="s">
+      <c r="I21" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J21" s="21">
         <v>1.2</v>
       </c>
-      <c r="K17" s="21">
+      <c r="K21" s="21">
         <v>1</v>
       </c>
-      <c r="L17" s="22">
-        <f>-C43/1000</f>
+      <c r="L21" s="22">
+        <f>-C47/1000</f>
         <v>-0.15180000000000002</v>
       </c>
-      <c r="M17" s="21">
+      <c r="M21" s="21">
         <v>5</v>
       </c>
-      <c r="N17" s="21" t="s">
+      <c r="N21" s="21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="10" t="s">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E26" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C27" s="8">
         <v>228046</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D27" s="8">
         <v>9959</v>
       </c>
-      <c r="E23" s="11">
-        <f t="shared" ref="E23:E28" si="0">D23/C23</f>
+      <c r="E27" s="11">
+        <f t="shared" ref="E27:E32" si="0">D27/C27</f>
         <v>4.3671013742841359E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="3" t="s">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="29"/>
+      <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C28" s="8">
         <v>100649</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D28" s="8">
         <v>6580</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E28" s="11">
         <f t="shared" si="0"/>
         <v>6.5375711631511485E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="3" t="s">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="29"/>
+      <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C29" s="8">
         <v>4546</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D29" s="8">
         <v>201</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E29" s="11">
         <f t="shared" si="0"/>
         <v>4.4214694236691596E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="3" t="s">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="29"/>
+      <c r="B30" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C30" s="8">
         <v>6661</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D30" s="8">
         <v>329</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E30" s="11">
         <f t="shared" si="0"/>
         <v>4.9391983185707852E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="3" t="s">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="29"/>
+      <c r="B31" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C31" s="8">
         <v>8424</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D31" s="8">
         <v>485</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E31" s="11">
         <f t="shared" si="0"/>
         <v>5.7573599240265907E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="3" t="s">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="29"/>
+      <c r="B32" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C32" s="8">
         <v>14373</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D32" s="8">
         <v>1033</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E32" s="11">
         <f t="shared" si="0"/>
         <v>7.187086899046824E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C33" s="8">
         <v>2168099</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D33" s="8">
         <v>121121</v>
       </c>
-      <c r="E29" s="11">
-        <f>D29/C29</f>
+      <c r="E33" s="11">
+        <f>D33/C33</f>
         <v>5.5865068892149296E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C34" s="8">
         <v>41471</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D34" s="8">
         <v>2566</v>
       </c>
-      <c r="E30" s="11">
-        <f t="shared" ref="E30:E32" si="1">D30/C30</f>
+      <c r="E34" s="11">
+        <f t="shared" ref="E34:E36" si="1">D34/C34</f>
         <v>6.1874562947601935E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C35" s="8">
         <v>21457</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D35" s="8">
         <v>1224</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E35" s="11">
         <f t="shared" si="1"/>
         <v>5.7044321200540614E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="7" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C36" s="9">
         <v>11206</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D36" s="9">
         <v>551</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E36" s="12">
         <f t="shared" si="1"/>
         <v>4.9170087453150095E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="13">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C41">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B44" s="13">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C45">
         <v>2018</v>
       </c>
-      <c r="D41">
+      <c r="D45">
         <v>2019</v>
       </c>
-      <c r="E41">
+      <c r="E45">
         <v>2020</v>
       </c>
-      <c r="F41">
+      <c r="F45">
         <v>2021</v>
       </c>
-      <c r="G41">
+      <c r="G45">
         <v>2022</v>
       </c>
-      <c r="H41">
+      <c r="H45">
         <v>2023</v>
       </c>
-      <c r="I41">
+      <c r="I45">
         <v>2024</v>
       </c>
-      <c r="J41">
+      <c r="J45">
         <v>2025</v>
       </c>
-      <c r="K41">
+      <c r="K45">
         <v>2026</v>
       </c>
-      <c r="L41">
+      <c r="L45">
         <v>2027</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
         <v>34</v>
       </c>
-      <c r="C42">
+      <c r="C46">
         <v>1</v>
       </c>
-      <c r="D42">
+      <c r="D46">
         <v>2</v>
       </c>
-      <c r="E42">
+      <c r="E46">
         <v>3</v>
       </c>
-      <c r="F42">
+      <c r="F46">
         <v>4</v>
       </c>
-      <c r="G42">
+      <c r="G46">
         <v>5</v>
       </c>
-      <c r="H42">
+      <c r="H46">
         <v>6</v>
       </c>
-      <c r="I42">
+      <c r="I46">
         <v>7</v>
       </c>
-      <c r="J42" s="14">
+      <c r="J46" s="14">
         <v>8</v>
       </c>
-      <c r="K42">
+      <c r="K46">
         <v>9</v>
       </c>
-      <c r="L42">
+      <c r="L46">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B47" s="15">
+        <f>D32+D31</f>
+        <v>1518</v>
+      </c>
+      <c r="C47" s="14">
+        <f>B47/10</f>
+        <v>151.80000000000001</v>
+      </c>
+      <c r="D47" s="14">
+        <f t="shared" ref="D47:L47" si="2">C47*(1+$B$44)</f>
+        <v>182.16</v>
+      </c>
+      <c r="E47" s="20">
+        <f t="shared" si="2"/>
+        <v>218.59199999999998</v>
+      </c>
+      <c r="F47" s="14">
+        <f t="shared" si="2"/>
+        <v>262.31039999999996</v>
+      </c>
+      <c r="G47" s="14">
+        <f t="shared" si="2"/>
+        <v>314.77247999999992</v>
+      </c>
+      <c r="H47" s="14">
+        <f t="shared" si="2"/>
+        <v>377.72697599999987</v>
+      </c>
+      <c r="I47" s="14">
+        <f t="shared" si="2"/>
+        <v>453.27237119999984</v>
+      </c>
+      <c r="J47" s="14">
+        <f t="shared" si="2"/>
+        <v>543.92684543999974</v>
+      </c>
+      <c r="K47" s="14">
+        <f t="shared" si="2"/>
+        <v>652.71221452799966</v>
+      </c>
+      <c r="L47" s="14">
+        <f t="shared" si="2"/>
+        <v>783.25465743359962</v>
+      </c>
+      <c r="M47" s="14"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="15">
+        <f>D30+D29</f>
+        <v>530</v>
+      </c>
+      <c r="C48" s="14">
+        <f>B48/10</f>
+        <v>53</v>
+      </c>
+      <c r="D48" s="14">
+        <f t="shared" ref="D48:L48" si="3">C48*(1+$B$44)</f>
+        <v>63.599999999999994</v>
+      </c>
+      <c r="E48" s="20">
+        <f t="shared" si="3"/>
+        <v>76.319999999999993</v>
+      </c>
+      <c r="F48" s="14">
+        <f t="shared" si="3"/>
+        <v>91.583999999999989</v>
+      </c>
+      <c r="G48" s="14">
+        <f t="shared" si="3"/>
+        <v>109.90079999999999</v>
+      </c>
+      <c r="H48" s="14">
+        <f t="shared" si="3"/>
+        <v>131.88095999999999</v>
+      </c>
+      <c r="I48" s="14">
+        <f t="shared" si="3"/>
+        <v>158.25715199999999</v>
+      </c>
+      <c r="J48" s="14">
+        <f t="shared" si="3"/>
+        <v>189.90858239999997</v>
+      </c>
+      <c r="K48" s="14">
+        <f t="shared" si="3"/>
+        <v>227.89029887999996</v>
+      </c>
+      <c r="L48" s="14">
+        <f t="shared" si="3"/>
+        <v>273.46835865599996</v>
+      </c>
+      <c r="M48" s="14"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="15">
         <f>D28+D27</f>
-        <v>1518</v>
-      </c>
-      <c r="C43" s="14">
-        <f>B43/10</f>
-        <v>151.80000000000001</v>
-      </c>
-      <c r="D43" s="14">
-        <f t="shared" ref="D43:L43" si="2">C43*(1+$B$40)</f>
-        <v>197.34000000000003</v>
-      </c>
-      <c r="E43" s="20">
-        <f t="shared" si="2"/>
-        <v>256.54200000000003</v>
-      </c>
-      <c r="F43" s="14">
-        <f t="shared" si="2"/>
-        <v>333.50460000000004</v>
-      </c>
-      <c r="G43" s="14">
-        <f t="shared" si="2"/>
-        <v>433.55598000000009</v>
-      </c>
-      <c r="H43" s="14">
-        <f t="shared" si="2"/>
-        <v>563.62277400000016</v>
-      </c>
-      <c r="I43" s="14">
-        <f t="shared" si="2"/>
-        <v>732.70960620000028</v>
-      </c>
-      <c r="J43" s="14">
-        <f t="shared" si="2"/>
-        <v>952.52248806000034</v>
-      </c>
-      <c r="K43" s="14">
-        <f t="shared" si="2"/>
-        <v>1238.2792344780005</v>
-      </c>
-      <c r="L43" s="14">
-        <f t="shared" si="2"/>
-        <v>1609.7630048214007</v>
-      </c>
-      <c r="M43" s="14"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="15">
-        <f>D26+D25</f>
-        <v>530</v>
-      </c>
-      <c r="C44" s="14">
-        <f>B44/10</f>
-        <v>53</v>
-      </c>
-      <c r="D44" s="14">
-        <f t="shared" ref="D44:L44" si="3">C44*(1+$B$40)</f>
-        <v>68.900000000000006</v>
-      </c>
-      <c r="E44" s="20">
-        <f t="shared" si="3"/>
-        <v>89.570000000000007</v>
-      </c>
-      <c r="F44" s="14">
-        <f t="shared" si="3"/>
-        <v>116.44100000000002</v>
-      </c>
-      <c r="G44" s="14">
-        <f t="shared" si="3"/>
-        <v>151.37330000000003</v>
-      </c>
-      <c r="H44" s="14">
-        <f t="shared" si="3"/>
-        <v>196.78529000000003</v>
-      </c>
-      <c r="I44" s="14">
-        <f t="shared" si="3"/>
-        <v>255.82087700000005</v>
-      </c>
-      <c r="J44" s="14">
-        <f t="shared" si="3"/>
-        <v>332.56714010000007</v>
-      </c>
-      <c r="K44" s="14">
-        <f t="shared" si="3"/>
-        <v>432.33728213000012</v>
-      </c>
-      <c r="L44" s="14">
-        <f t="shared" si="3"/>
-        <v>562.03846676900014</v>
-      </c>
-      <c r="M44" s="14"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="15">
-        <f>D24+D23</f>
         <v>16539</v>
       </c>
-      <c r="C45" s="14">
-        <f>B45/10</f>
+      <c r="C49" s="14">
+        <f>B49/10</f>
         <v>1653.9</v>
       </c>
-      <c r="D45" s="14">
-        <f>C45*(1+$B$40)</f>
-        <v>2150.0700000000002</v>
-      </c>
-      <c r="E45" s="20">
-        <f t="shared" ref="E45:L45" si="4">D45*(1+$B$40)</f>
-        <v>2795.0910000000003</v>
-      </c>
-      <c r="F45" s="14">
+      <c r="D49" s="14">
+        <f>C49*(1+$B$44)</f>
+        <v>1984.68</v>
+      </c>
+      <c r="E49" s="20">
+        <f t="shared" ref="E49:L49" si="4">D49*(1+$B$44)</f>
+        <v>2381.616</v>
+      </c>
+      <c r="F49" s="14">
         <f t="shared" si="4"/>
-        <v>3633.6183000000005</v>
-      </c>
-      <c r="G45" s="14">
+        <v>2857.9391999999998</v>
+      </c>
+      <c r="G49" s="14">
         <f t="shared" si="4"/>
-        <v>4723.7037900000005</v>
-      </c>
-      <c r="H45" s="14">
+        <v>3429.5270399999995</v>
+      </c>
+      <c r="H49" s="14">
         <f t="shared" si="4"/>
-        <v>6140.8149270000013</v>
-      </c>
-      <c r="I45" s="14">
+        <v>4115.4324479999996</v>
+      </c>
+      <c r="I49" s="14">
         <f t="shared" si="4"/>
-        <v>7983.0594051000016</v>
-      </c>
-      <c r="J45" s="14">
+        <v>4938.5189375999989</v>
+      </c>
+      <c r="J49" s="14">
         <f t="shared" si="4"/>
-        <v>10377.977226630002</v>
-      </c>
-      <c r="K45" s="14">
+        <v>5926.2227251199984</v>
+      </c>
+      <c r="K49" s="14">
         <f t="shared" si="4"/>
-        <v>13491.370394619003</v>
-      </c>
-      <c r="L45" s="14">
+        <v>7111.4672701439977</v>
+      </c>
+      <c r="L49" s="14">
         <f t="shared" si="4"/>
-        <v>17538.781513004706</v>
-      </c>
-      <c r="M45" s="14"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+        <v>8533.7607241727965</v>
+      </c>
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="15">
-        <f>D29</f>
+      <c r="B50" s="15">
+        <f>D33</f>
         <v>121121</v>
       </c>
-      <c r="C46" s="14">
-        <f>B46/5</f>
+      <c r="C50" s="14">
+        <f>B50/5</f>
         <v>24224.2</v>
       </c>
-      <c r="D46" s="14">
-        <f t="shared" ref="D46:L46" si="5">C46*(1+$B$40)</f>
-        <v>31491.460000000003</v>
-      </c>
-      <c r="E46" s="20">
+      <c r="D50" s="14">
+        <f t="shared" ref="D50:L50" si="5">C50*(1+$B$44)</f>
+        <v>29069.040000000001</v>
+      </c>
+      <c r="E50" s="20">
         <f t="shared" si="5"/>
-        <v>40938.898000000008</v>
-      </c>
-      <c r="F46" s="14">
+        <v>34882.847999999998</v>
+      </c>
+      <c r="F50" s="14">
         <f t="shared" si="5"/>
-        <v>53220.567400000014</v>
-      </c>
-      <c r="G46" s="14">
+        <v>41859.417599999993</v>
+      </c>
+      <c r="G50" s="14">
         <f t="shared" si="5"/>
-        <v>69186.737620000014</v>
-      </c>
-      <c r="H46" s="14">
+        <v>50231.301119999989</v>
+      </c>
+      <c r="H50" s="14">
         <f t="shared" si="5"/>
-        <v>89942.758906000017</v>
-      </c>
-      <c r="I46" s="14">
+        <v>60277.561343999987</v>
+      </c>
+      <c r="I50" s="14">
         <f t="shared" si="5"/>
-        <v>116925.58657780003</v>
-      </c>
-      <c r="J46" s="14">
+        <v>72333.073612799984</v>
+      </c>
+      <c r="J50" s="14">
         <f t="shared" si="5"/>
-        <v>152003.26255114004</v>
-      </c>
-      <c r="K46" s="14">
+        <v>86799.688335359984</v>
+      </c>
+      <c r="K50" s="14">
         <f t="shared" si="5"/>
-        <v>197604.24131648205</v>
-      </c>
-      <c r="L46" s="14">
+        <v>104159.62600243198</v>
+      </c>
+      <c r="L50" s="14">
         <f t="shared" si="5"/>
-        <v>256885.51371142667</v>
-      </c>
-      <c r="M46" s="14"/>
+        <v>124991.55120291837</v>
+      </c>
+      <c r="M50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A27:A32"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3376,6 +3538,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -3586,22 +3763,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3618,21 +3797,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modify UC definition for HGT
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A4E627-0154-4378-94C9-296A6B03B3E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756DCA82-C6DE-4689-A6DA-5A826708479C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -513,15 +513,9 @@
     <t>HGT-Maximum growth rate of NG-ICEs</t>
   </si>
   <si>
-    <t>T-HGT-ICE-NG*</t>
-  </si>
-  <si>
     <t>UC-HGT_MaxGrowthLNGICE</t>
   </si>
   <si>
-    <t>T-HGT-ICE-LNG*</t>
-  </si>
-  <si>
     <t>HGT-Maximum growth rate of LNG-ICEs</t>
   </si>
   <si>
@@ -532,6 +526,12 @@
   </si>
   <si>
     <t>MGT-Maximum growth rate of LNG-ICEs</t>
+  </si>
+  <si>
+    <t>T-HGT-ICE_NG*</t>
+  </si>
+  <si>
+    <t>T-HGT-ICE_LNG*</t>
   </si>
 </sst>
 </file>
@@ -2345,7 +2345,7 @@
   <dimension ref="A2:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>13</v>
@@ -2776,7 +2776,7 @@
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H14" s="18">
         <v>2018</v>
@@ -2798,7 +2798,7 @@
         <v>5</v>
       </c>
       <c r="N14" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
@@ -2928,7 +2928,7 @@
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="18" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="H18" s="18">
         <v>2018</v>
@@ -2955,7 +2955,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>13</v>
@@ -2966,7 +2966,7 @@
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="18" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H19" s="18">
         <v>2018</v>
@@ -2988,7 +2988,7 @@
         <v>5</v>
       </c>
       <c r="N19" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -3538,18 +3538,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3764,18 +3764,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
TRA: apply a 20% growth constraint to CNG cars and LGT vehicles
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Max_Growth.xlsx
+++ b/SuppXLS/Scen_TRA_Max_Growth.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756DCA82-C6DE-4689-A6DA-5A826708479C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0B31CB-00E7-446D-AFB2-B1C12547325C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="154">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -533,15 +533,33 @@
   <si>
     <t>T-HGT-ICE_LNG*</t>
   </si>
+  <si>
+    <t>UC-CAR_MaxGrowthNGICE</t>
+  </si>
+  <si>
+    <t>T-CAR-ICE_NG*</t>
+  </si>
+  <si>
+    <t>Cars-Maximum growth rate of NG-ICEs</t>
+  </si>
+  <si>
+    <t>UC-LGT_MaxGrowthNGICE</t>
+  </si>
+  <si>
+    <t>T-LGT-ICE_NG*</t>
+  </si>
+  <si>
+    <t>LGT-Maximum growth rate of NG-ICEs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -724,224 +742,224 @@
   </borders>
   <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -950,8 +968,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -959,14 +977,14 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -981,6 +999,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="217">
     <cellStyle name="20% - Accent5 2" xfId="10" xr:uid="{72E8C261-0B7B-4154-8B6F-C9901D88251B}"/>
@@ -1584,39 +1604,39 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="3.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5546875" customWidth="1"/>
-    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C3" s="23" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -1730,12 +1750,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -1850,7 +1870,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -1967,7 +1987,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -2084,7 +2104,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>81</v>
       </c>
@@ -2092,7 +2112,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>83</v>
       </c>
@@ -2100,7 +2120,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>85</v>
       </c>
@@ -2108,7 +2128,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>87</v>
       </c>
@@ -2116,7 +2136,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>89</v>
       </c>
@@ -2124,7 +2144,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>91</v>
       </c>
@@ -2132,7 +2152,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>93</v>
       </c>
@@ -2140,7 +2160,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>95</v>
       </c>
@@ -2148,7 +2168,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>97</v>
       </c>
@@ -2156,7 +2176,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>99</v>
       </c>
@@ -2164,7 +2184,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>101</v>
       </c>
@@ -2172,7 +2192,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>103</v>
       </c>
@@ -2180,7 +2200,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>105</v>
       </c>
@@ -2188,7 +2208,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>107</v>
       </c>
@@ -2196,7 +2216,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>109</v>
       </c>
@@ -2204,7 +2224,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>111</v>
       </c>
@@ -2212,7 +2232,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>113</v>
       </c>
@@ -2220,7 +2240,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>115</v>
       </c>
@@ -2228,7 +2248,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>117</v>
       </c>
@@ -2236,7 +2256,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
         <v>119</v>
       </c>
@@ -2244,7 +2264,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
         <v>121</v>
       </c>
@@ -2252,7 +2272,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>123</v>
       </c>
@@ -2260,7 +2280,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
         <v>125</v>
       </c>
@@ -2268,7 +2288,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>127</v>
       </c>
@@ -2276,7 +2296,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
         <v>129</v>
       </c>
@@ -2284,7 +2304,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>131</v>
       </c>
@@ -2292,7 +2312,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
         <v>133</v>
       </c>
@@ -2300,7 +2320,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>135</v>
       </c>
@@ -2342,28 +2362,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
-  <dimension ref="A2:O50"/>
+  <dimension ref="A2:O52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" customWidth="1"/>
     <col min="14" max="14" width="34" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:AD3)</f>
         <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
@@ -2382,7 +2402,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2400,7 +2420,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2418,7 +2438,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -2459,7 +2479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>57</v>
       </c>
@@ -2480,14 +2500,15 @@
       <c r="I6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="30">
+        <f t="shared" ref="J6:J23" si="0">1+$B$46</f>
         <v>1.2</v>
       </c>
       <c r="K6" s="18">
         <v>1</v>
       </c>
       <c r="L6" s="19">
-        <f>-C50/1000</f>
+        <f>-C52/1000</f>
         <v>-24.2242</v>
       </c>
       <c r="M6" s="18">
@@ -2497,7 +2518,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>58</v>
       </c>
@@ -2518,14 +2539,15 @@
       <c r="I7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="30">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="K7" s="18">
         <v>1</v>
       </c>
       <c r="L7" s="19">
-        <f>-C50/1000</f>
+        <f>-C52/1000</f>
         <v>-24.2242</v>
       </c>
       <c r="M7" s="18">
@@ -2535,85 +2557,87 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="21" t="s">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="18">
+        <v>2018</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="30">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="K8" s="18">
+        <v>1</v>
+      </c>
+      <c r="L8" s="19">
+        <f>-C52/1000</f>
+        <v>-24.2242</v>
+      </c>
+      <c r="M8" s="18">
+        <v>5</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21" t="s">
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H9" s="21">
         <v>2018</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J9" s="31">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K9" s="21">
         <v>1</v>
       </c>
-      <c r="L8" s="22">
-        <f>-C50/1000</f>
+      <c r="L9" s="22">
+        <f>-C52/1000</f>
         <v>-24.2242</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M9" s="21">
         <v>5</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N9" s="21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="18" t="s">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="18">
-        <v>2018</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="18">
-        <v>1.2</v>
-      </c>
-      <c r="K9" s="18">
-        <v>1</v>
-      </c>
-      <c r="L9" s="19">
-        <f>-C49/1000</f>
-        <v>-1.6539000000000001</v>
-      </c>
-      <c r="M9" s="18">
-        <v>5</v>
-      </c>
-      <c r="N9" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
-        <v>74</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>13</v>
@@ -2624,7 +2648,7 @@
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="18" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="H10" s="18">
         <v>2018</v>
@@ -2632,64 +2656,66 @@
       <c r="I10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="30">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="K10" s="18">
         <v>1</v>
       </c>
       <c r="L10" s="19">
-        <f>-C49/1000</f>
+        <f>-C51/1000</f>
         <v>-1.6539000000000001</v>
       </c>
       <c r="M10" s="18">
         <v>5</v>
       </c>
       <c r="N10" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="18">
+        <v>2018</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="30">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="K11" s="18">
+        <v>1</v>
+      </c>
+      <c r="L11" s="19">
+        <f>-C51/1000</f>
+        <v>-1.6539000000000001</v>
+      </c>
+      <c r="M11" s="18">
+        <v>5</v>
+      </c>
+      <c r="N11" s="18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11" s="21">
-        <v>2018</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="21">
-        <v>1.2</v>
-      </c>
-      <c r="K11" s="21">
-        <v>1</v>
-      </c>
-      <c r="L11" s="22">
-        <f>-C49/1000</f>
-        <v>-1.6539000000000001</v>
-      </c>
-      <c r="M11" s="21">
-        <v>5</v>
-      </c>
-      <c r="N11" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>51</v>
+        <v>151</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>13</v>
@@ -2700,7 +2726,7 @@
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="H12" s="18">
         <v>2018</v>
@@ -2708,64 +2734,66 @@
       <c r="I12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="30">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="K12" s="18">
         <v>1</v>
       </c>
       <c r="L12" s="19">
-        <f>-C48/1000</f>
-        <v>-5.2999999999999999E-2</v>
+        <f>-C51/1000</f>
+        <v>-1.6539000000000001</v>
       </c>
       <c r="M12" s="18">
         <v>5</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="H13" s="18">
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="21">
         <v>2018</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="I13" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="31">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="21">
         <v>1</v>
       </c>
-      <c r="L13" s="19">
-        <f>-C48/1000</f>
-        <v>-5.2999999999999999E-2</v>
-      </c>
-      <c r="M13" s="18">
+      <c r="L13" s="22">
+        <f>-C51/1000</f>
+        <v>-1.6539000000000001</v>
+      </c>
+      <c r="M13" s="21">
         <v>5</v>
       </c>
-      <c r="N13" s="18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="N13" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>143</v>
+        <v>51</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>13</v>
@@ -2776,7 +2804,7 @@
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18" t="s">
-        <v>144</v>
+        <v>40</v>
       </c>
       <c r="H14" s="18">
         <v>2018</v>
@@ -2784,26 +2812,27 @@
       <c r="I14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="30">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="K14" s="18">
         <v>1</v>
       </c>
       <c r="L14" s="19">
-        <f>-C48/1000</f>
+        <f>-C50/1000</f>
         <v>-5.2999999999999999E-2</v>
       </c>
       <c r="M14" s="18">
         <v>5</v>
       </c>
       <c r="N14" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>13</v>
@@ -2814,7 +2843,7 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="H15" s="18">
         <v>2018</v>
@@ -2822,64 +2851,66 @@
       <c r="I15" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="30">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="K15" s="18">
         <v>1</v>
       </c>
       <c r="L15" s="19">
-        <f>-C48/1000</f>
+        <f>-C50/1000</f>
         <v>-5.2999999999999999E-2</v>
       </c>
       <c r="M15" s="18">
         <v>5</v>
       </c>
       <c r="N15" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="21">
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="H16" s="18">
         <v>2018</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="30">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="K16" s="21">
+      <c r="K16" s="18">
         <v>1</v>
       </c>
-      <c r="L16" s="22">
-        <f>-C48/1000</f>
+      <c r="L16" s="19">
+        <f>-C50/1000</f>
         <v>-5.2999999999999999E-2</v>
       </c>
-      <c r="M16" s="21">
+      <c r="M16" s="18">
         <v>5</v>
       </c>
-      <c r="N16" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N16" s="18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>13</v>
@@ -2890,7 +2921,7 @@
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="H17" s="18">
         <v>2018</v>
@@ -2898,64 +2929,66 @@
       <c r="I17" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="30">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="K17" s="18">
         <v>1</v>
       </c>
       <c r="L17" s="19">
-        <f>-C47/1000</f>
-        <v>-0.15180000000000002</v>
+        <f>-C50/1000</f>
+        <v>-5.2999999999999999E-2</v>
       </c>
       <c r="M17" s="18">
         <v>5</v>
       </c>
       <c r="N17" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="C18" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="H18" s="18">
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="21">
         <v>2018</v>
       </c>
-      <c r="I18" s="18" t="s">
+      <c r="I18" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="31">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="21">
         <v>1</v>
       </c>
-      <c r="L18" s="19">
-        <f>-C47/1000</f>
-        <v>-0.15180000000000002</v>
-      </c>
-      <c r="M18" s="18">
+      <c r="L18" s="22">
+        <f>-C50/1000</f>
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="M18" s="21">
         <v>5</v>
       </c>
-      <c r="N18" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N18" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
-        <v>141</v>
+        <v>47</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>13</v>
@@ -2966,7 +2999,7 @@
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="18" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="H19" s="18">
         <v>2018</v>
@@ -2974,26 +3007,27 @@
       <c r="I19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="30">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="K19" s="18">
         <v>1</v>
       </c>
       <c r="L19" s="19">
-        <f>-C47/1000</f>
+        <f>-C49/1000</f>
         <v>-0.15180000000000002</v>
       </c>
       <c r="M19" s="18">
         <v>5</v>
       </c>
       <c r="N19" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
-        <v>48</v>
+        <v>136</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>13</v>
@@ -3004,7 +3038,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="H20" s="18">
         <v>2018</v>
@@ -3012,524 +3046,604 @@
       <c r="I20" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="30">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="K20" s="18">
         <v>1</v>
       </c>
       <c r="L20" s="19">
-        <f>-C47/1000</f>
+        <f>-C49/1000</f>
         <v>-0.15180000000000002</v>
       </c>
       <c r="M20" s="18">
         <v>5</v>
       </c>
       <c r="N20" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="H21" s="18">
+        <v>2018</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="30">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="K21" s="18">
+        <v>1</v>
+      </c>
+      <c r="L21" s="19">
+        <f>-C49/1000</f>
+        <v>-0.15180000000000002</v>
+      </c>
+      <c r="M21" s="18">
+        <v>5</v>
+      </c>
+      <c r="N21" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="18">
+        <v>2018</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="30">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="K22" s="18">
+        <v>1</v>
+      </c>
+      <c r="L22" s="19">
+        <f>-C49/1000</f>
+        <v>-0.15180000000000002</v>
+      </c>
+      <c r="M22" s="18">
+        <v>5</v>
+      </c>
+      <c r="N22" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B21" s="21" t="s">
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C23" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D23" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21" t="s">
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H23" s="21">
         <v>2018</v>
       </c>
-      <c r="I21" s="21" t="s">
+      <c r="I23" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J23" s="31">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="K21" s="21">
+      <c r="K23" s="21">
         <v>1</v>
       </c>
-      <c r="L21" s="22">
-        <f>-C47/1000</f>
+      <c r="L23" s="22">
+        <f>-C49/1000</f>
         <v>-0.15180000000000002</v>
       </c>
-      <c r="M21" s="21">
+      <c r="M23" s="21">
         <v>5</v>
       </c>
-      <c r="N21" s="21" t="s">
+      <c r="N23" s="21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="10" t="s">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="29" t="s">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C29" s="8">
         <v>228046</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D29" s="8">
         <v>9959</v>
       </c>
-      <c r="E27" s="11">
-        <f t="shared" ref="E27:E32" si="0">D27/C27</f>
+      <c r="E29" s="11">
+        <f t="shared" ref="E29:E34" si="1">D29/C29</f>
         <v>4.3671013742841359E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="29"/>
-      <c r="B28" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="8">
-        <v>100649</v>
-      </c>
-      <c r="D28" s="8">
-        <v>6580</v>
-      </c>
-      <c r="E28" s="11">
-        <f t="shared" si="0"/>
-        <v>6.5375711631511485E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="29"/>
-      <c r="B29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="8">
-        <v>4546</v>
-      </c>
-      <c r="D29" s="8">
-        <v>201</v>
-      </c>
-      <c r="E29" s="11">
-        <f t="shared" si="0"/>
-        <v>4.4214694236691596E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
       <c r="B30" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C30" s="8">
-        <v>6661</v>
+        <v>100649</v>
       </c>
       <c r="D30" s="8">
-        <v>329</v>
+        <v>6580</v>
       </c>
       <c r="E30" s="11">
-        <f t="shared" si="0"/>
-        <v>4.9391983185707852E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>6.5375711631511485E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
       <c r="B31" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C31" s="8">
-        <v>8424</v>
+        <v>4546</v>
       </c>
       <c r="D31" s="8">
-        <v>485</v>
+        <v>201</v>
       </c>
       <c r="E31" s="11">
-        <f t="shared" si="0"/>
-        <v>5.7573599240265907E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>4.4214694236691596E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="29"/>
       <c r="B32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="8">
+        <v>6661</v>
+      </c>
+      <c r="D32" s="8">
+        <v>329</v>
+      </c>
+      <c r="E32" s="11">
+        <f t="shared" si="1"/>
+        <v>4.9391983185707852E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="B33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="8">
+        <v>8424</v>
+      </c>
+      <c r="D33" s="8">
+        <v>485</v>
+      </c>
+      <c r="E33" s="11">
+        <f t="shared" si="1"/>
+        <v>5.7573599240265907E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="29"/>
+      <c r="B34" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C34" s="8">
         <v>14373</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D34" s="8">
         <v>1033</v>
       </c>
-      <c r="E32" s="11">
-        <f t="shared" si="0"/>
+      <c r="E34" s="11">
+        <f t="shared" si="1"/>
         <v>7.187086899046824E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B33" s="3" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C35" s="8">
         <v>2168099</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D35" s="8">
         <v>121121</v>
       </c>
-      <c r="E33" s="11">
-        <f>D33/C33</f>
+      <c r="E35" s="11">
+        <f>D35/C35</f>
         <v>5.5865068892149296E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B34" s="3" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C36" s="8">
         <v>41471</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D36" s="8">
         <v>2566</v>
       </c>
-      <c r="E34" s="11">
-        <f t="shared" ref="E34:E36" si="1">D34/C34</f>
+      <c r="E36" s="11">
+        <f t="shared" ref="E36:E38" si="2">D36/C36</f>
         <v>6.1874562947601935E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B35" s="3" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C37" s="8">
         <v>21457</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D37" s="8">
         <v>1224</v>
       </c>
-      <c r="E35" s="11">
-        <f t="shared" si="1"/>
+      <c r="E37" s="11">
+        <f t="shared" si="2"/>
         <v>5.7044321200540614E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C38" s="9">
         <v>11206</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D38" s="9">
         <v>551</v>
       </c>
-      <c r="E36" s="12">
-        <f t="shared" si="1"/>
+      <c r="E38" s="12">
+        <f t="shared" si="2"/>
         <v>4.9170087453150095E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B44" s="13">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="13">
         <v>0.2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C45">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C47">
         <v>2018</v>
       </c>
-      <c r="D45">
+      <c r="D47">
         <v>2019</v>
       </c>
-      <c r="E45">
+      <c r="E47">
         <v>2020</v>
       </c>
-      <c r="F45">
+      <c r="F47">
         <v>2021</v>
       </c>
-      <c r="G45">
+      <c r="G47">
         <v>2022</v>
       </c>
-      <c r="H45">
+      <c r="H47">
         <v>2023</v>
       </c>
-      <c r="I45">
+      <c r="I47">
         <v>2024</v>
       </c>
-      <c r="J45">
+      <c r="J47">
         <v>2025</v>
       </c>
-      <c r="K45">
+      <c r="K47">
         <v>2026</v>
       </c>
-      <c r="L45">
+      <c r="L47">
         <v>2027</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>34</v>
       </c>
-      <c r="C46">
+      <c r="C48">
         <v>1</v>
       </c>
-      <c r="D46">
+      <c r="D48">
         <v>2</v>
       </c>
-      <c r="E46">
+      <c r="E48">
         <v>3</v>
       </c>
-      <c r="F46">
+      <c r="F48">
         <v>4</v>
       </c>
-      <c r="G46">
+      <c r="G48">
         <v>5</v>
       </c>
-      <c r="H46">
+      <c r="H48">
         <v>6</v>
       </c>
-      <c r="I46">
+      <c r="I48">
         <v>7</v>
       </c>
-      <c r="J46" s="14">
+      <c r="J48" s="14">
         <v>8</v>
       </c>
-      <c r="K46">
+      <c r="K48">
         <v>9</v>
       </c>
-      <c r="L46">
+      <c r="L48">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="15">
-        <f>D32+D31</f>
+      <c r="B49" s="15">
+        <f>D34+D33</f>
         <v>1518</v>
-      </c>
-      <c r="C47" s="14">
-        <f>B47/10</f>
-        <v>151.80000000000001</v>
-      </c>
-      <c r="D47" s="14">
-        <f t="shared" ref="D47:L47" si="2">C47*(1+$B$44)</f>
-        <v>182.16</v>
-      </c>
-      <c r="E47" s="20">
-        <f t="shared" si="2"/>
-        <v>218.59199999999998</v>
-      </c>
-      <c r="F47" s="14">
-        <f t="shared" si="2"/>
-        <v>262.31039999999996</v>
-      </c>
-      <c r="G47" s="14">
-        <f t="shared" si="2"/>
-        <v>314.77247999999992</v>
-      </c>
-      <c r="H47" s="14">
-        <f t="shared" si="2"/>
-        <v>377.72697599999987</v>
-      </c>
-      <c r="I47" s="14">
-        <f t="shared" si="2"/>
-        <v>453.27237119999984</v>
-      </c>
-      <c r="J47" s="14">
-        <f t="shared" si="2"/>
-        <v>543.92684543999974</v>
-      </c>
-      <c r="K47" s="14">
-        <f t="shared" si="2"/>
-        <v>652.71221452799966</v>
-      </c>
-      <c r="L47" s="14">
-        <f t="shared" si="2"/>
-        <v>783.25465743359962</v>
-      </c>
-      <c r="M47" s="14"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>36</v>
-      </c>
-      <c r="B48" s="15">
-        <f>D30+D29</f>
-        <v>530</v>
-      </c>
-      <c r="C48" s="14">
-        <f>B48/10</f>
-        <v>53</v>
-      </c>
-      <c r="D48" s="14">
-        <f t="shared" ref="D48:L48" si="3">C48*(1+$B$44)</f>
-        <v>63.599999999999994</v>
-      </c>
-      <c r="E48" s="20">
-        <f t="shared" si="3"/>
-        <v>76.319999999999993</v>
-      </c>
-      <c r="F48" s="14">
-        <f t="shared" si="3"/>
-        <v>91.583999999999989</v>
-      </c>
-      <c r="G48" s="14">
-        <f t="shared" si="3"/>
-        <v>109.90079999999999</v>
-      </c>
-      <c r="H48" s="14">
-        <f t="shared" si="3"/>
-        <v>131.88095999999999</v>
-      </c>
-      <c r="I48" s="14">
-        <f t="shared" si="3"/>
-        <v>158.25715199999999</v>
-      </c>
-      <c r="J48" s="14">
-        <f t="shared" si="3"/>
-        <v>189.90858239999997</v>
-      </c>
-      <c r="K48" s="14">
-        <f t="shared" si="3"/>
-        <v>227.89029887999996</v>
-      </c>
-      <c r="L48" s="14">
-        <f t="shared" si="3"/>
-        <v>273.46835865599996</v>
-      </c>
-      <c r="M48" s="14"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>37</v>
-      </c>
-      <c r="B49" s="15">
-        <f>D28+D27</f>
-        <v>16539</v>
       </c>
       <c r="C49" s="14">
         <f>B49/10</f>
+        <v>151.80000000000001</v>
+      </c>
+      <c r="D49" s="14">
+        <f t="shared" ref="D49:L49" si="3">C49*(1+$B$46)</f>
+        <v>182.16</v>
+      </c>
+      <c r="E49" s="20">
+        <f t="shared" si="3"/>
+        <v>218.59199999999998</v>
+      </c>
+      <c r="F49" s="14">
+        <f t="shared" si="3"/>
+        <v>262.31039999999996</v>
+      </c>
+      <c r="G49" s="14">
+        <f t="shared" si="3"/>
+        <v>314.77247999999992</v>
+      </c>
+      <c r="H49" s="14">
+        <f t="shared" si="3"/>
+        <v>377.72697599999987</v>
+      </c>
+      <c r="I49" s="14">
+        <f t="shared" si="3"/>
+        <v>453.27237119999984</v>
+      </c>
+      <c r="J49" s="14">
+        <f t="shared" si="3"/>
+        <v>543.92684543999974</v>
+      </c>
+      <c r="K49" s="14">
+        <f t="shared" si="3"/>
+        <v>652.71221452799966</v>
+      </c>
+      <c r="L49" s="14">
+        <f t="shared" si="3"/>
+        <v>783.25465743359962</v>
+      </c>
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="15">
+        <f>D32+D31</f>
+        <v>530</v>
+      </c>
+      <c r="C50" s="14">
+        <f>B50/10</f>
+        <v>53</v>
+      </c>
+      <c r="D50" s="14">
+        <f t="shared" ref="D50:L50" si="4">C50*(1+$B$46)</f>
+        <v>63.599999999999994</v>
+      </c>
+      <c r="E50" s="20">
+        <f t="shared" si="4"/>
+        <v>76.319999999999993</v>
+      </c>
+      <c r="F50" s="14">
+        <f t="shared" si="4"/>
+        <v>91.583999999999989</v>
+      </c>
+      <c r="G50" s="14">
+        <f t="shared" si="4"/>
+        <v>109.90079999999999</v>
+      </c>
+      <c r="H50" s="14">
+        <f t="shared" si="4"/>
+        <v>131.88095999999999</v>
+      </c>
+      <c r="I50" s="14">
+        <f t="shared" si="4"/>
+        <v>158.25715199999999</v>
+      </c>
+      <c r="J50" s="14">
+        <f t="shared" si="4"/>
+        <v>189.90858239999997</v>
+      </c>
+      <c r="K50" s="14">
+        <f t="shared" si="4"/>
+        <v>227.89029887999996</v>
+      </c>
+      <c r="L50" s="14">
+        <f t="shared" si="4"/>
+        <v>273.46835865599996</v>
+      </c>
+      <c r="M50" s="14"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B51" s="15">
+        <f>D30+D29</f>
+        <v>16539</v>
+      </c>
+      <c r="C51" s="14">
+        <f>B51/10</f>
         <v>1653.9</v>
       </c>
-      <c r="D49" s="14">
-        <f>C49*(1+$B$44)</f>
+      <c r="D51" s="14">
+        <f>C51*(1+$B$46)</f>
         <v>1984.68</v>
       </c>
-      <c r="E49" s="20">
-        <f t="shared" ref="E49:L49" si="4">D49*(1+$B$44)</f>
+      <c r="E51" s="20">
+        <f t="shared" ref="E51:L51" si="5">D51*(1+$B$46)</f>
         <v>2381.616</v>
       </c>
-      <c r="F49" s="14">
-        <f t="shared" si="4"/>
+      <c r="F51" s="14">
+        <f t="shared" si="5"/>
         <v>2857.9391999999998</v>
       </c>
-      <c r="G49" s="14">
-        <f t="shared" si="4"/>
+      <c r="G51" s="14">
+        <f t="shared" si="5"/>
         <v>3429.5270399999995</v>
       </c>
-      <c r="H49" s="14">
-        <f t="shared" si="4"/>
+      <c r="H51" s="14">
+        <f t="shared" si="5"/>
         <v>4115.4324479999996</v>
       </c>
-      <c r="I49" s="14">
-        <f t="shared" si="4"/>
+      <c r="I51" s="14">
+        <f t="shared" si="5"/>
         <v>4938.5189375999989</v>
       </c>
-      <c r="J49" s="14">
-        <f t="shared" si="4"/>
+      <c r="J51" s="14">
+        <f t="shared" si="5"/>
         <v>5926.2227251199984</v>
       </c>
-      <c r="K49" s="14">
-        <f t="shared" si="4"/>
+      <c r="K51" s="14">
+        <f t="shared" si="5"/>
         <v>7111.4672701439977</v>
       </c>
-      <c r="L49" s="14">
-        <f t="shared" si="4"/>
+      <c r="L51" s="14">
+        <f t="shared" si="5"/>
         <v>8533.7607241727965</v>
       </c>
-      <c r="M49" s="14"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="M51" s="14"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="15">
-        <f>D33</f>
+      <c r="B52" s="15">
+        <f>D35</f>
         <v>121121</v>
       </c>
-      <c r="C50" s="14">
-        <f>B50/5</f>
+      <c r="C52" s="14">
+        <f>B52/5</f>
         <v>24224.2</v>
       </c>
-      <c r="D50" s="14">
-        <f t="shared" ref="D50:L50" si="5">C50*(1+$B$44)</f>
+      <c r="D52" s="14">
+        <f t="shared" ref="D52:L52" si="6">C52*(1+$B$46)</f>
         <v>29069.040000000001</v>
       </c>
-      <c r="E50" s="20">
-        <f t="shared" si="5"/>
+      <c r="E52" s="20">
+        <f t="shared" si="6"/>
         <v>34882.847999999998</v>
       </c>
-      <c r="F50" s="14">
-        <f t="shared" si="5"/>
+      <c r="F52" s="14">
+        <f t="shared" si="6"/>
         <v>41859.417599999993</v>
       </c>
-      <c r="G50" s="14">
-        <f t="shared" si="5"/>
+      <c r="G52" s="14">
+        <f t="shared" si="6"/>
         <v>50231.301119999989</v>
       </c>
-      <c r="H50" s="14">
-        <f t="shared" si="5"/>
+      <c r="H52" s="14">
+        <f t="shared" si="6"/>
         <v>60277.561343999987</v>
       </c>
-      <c r="I50" s="14">
-        <f t="shared" si="5"/>
+      <c r="I52" s="14">
+        <f t="shared" si="6"/>
         <v>72333.073612799984</v>
       </c>
-      <c r="J50" s="14">
-        <f t="shared" si="5"/>
+      <c r="J52" s="14">
+        <f t="shared" si="6"/>
         <v>86799.688335359984</v>
       </c>
-      <c r="K50" s="14">
-        <f t="shared" si="5"/>
+      <c r="K52" s="14">
+        <f t="shared" si="6"/>
         <v>104159.62600243198</v>
       </c>
-      <c r="L50" s="14">
-        <f t="shared" si="5"/>
+      <c r="L52" s="14">
+        <f t="shared" si="6"/>
         <v>124991.55120291837</v>
       </c>
-      <c r="M50" s="14"/>
+      <c r="M52" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>